<commit_message>
Hid worksheets other than 'patterns'
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -9,8 +9,8 @@
   </bookViews>
   <sheets>
     <sheet name="patterns" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="patterns_dev" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="literal" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="patterns_dev" sheetId="2" state="hidden" r:id="rId3"/>
+    <sheet name="literal" sheetId="3" state="hidden" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -663,35 +663,7 @@
     <t xml:space="preserve">$1‌$2</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFC9211E"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(&lt;text&gt;\s+&lt;(strong|em)&gt;(?!\u200C))([^&lt;]+)(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFC9211E"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(?&lt;!\u200C)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFC9211E"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;/\2&gt;\s+&lt;/text&gt;)</t>
-    </r>
+    <t xml:space="preserve">(&lt;text&gt;\s+&lt;(strong|em)&gt;(?!\u200C))([^&lt;]+)((?&lt;!\u200C)&lt;/\2&gt;\s+&lt;/text&gt;)</t>
   </si>
   <si>
     <t xml:space="preserve">$1‌$3‌$4</t>
@@ -1377,7 +1349,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1465,12 +1437,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFC9211E"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1532,7 +1498,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1597,11 +1563,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1610,10 +1576,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1645,7 +1607,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1731,7 +1693,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5462,7 +5424,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="65" s="20" customFormat="true" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" s="14" customFormat="true" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="19" t="s">
         <v>131</v>
       </c>
@@ -5473,1021 +5435,8 @@
       <c r="D65" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="L65" s="14"/>
-      <c r="M65" s="14"/>
-      <c r="N65" s="14"/>
-      <c r="O65" s="14"/>
-      <c r="P65" s="14"/>
-      <c r="Q65" s="14"/>
-      <c r="R65" s="14"/>
-      <c r="S65" s="14"/>
-      <c r="T65" s="14"/>
-      <c r="U65" s="14"/>
-      <c r="V65" s="14"/>
-      <c r="W65" s="14"/>
-      <c r="X65" s="14"/>
-      <c r="Y65" s="14"/>
-      <c r="Z65" s="14"/>
-      <c r="AA65" s="14"/>
-      <c r="AB65" s="14"/>
-      <c r="AC65" s="14"/>
-      <c r="AD65" s="14"/>
-      <c r="AE65" s="14"/>
-      <c r="AF65" s="14"/>
-      <c r="AG65" s="14"/>
-      <c r="AH65" s="14"/>
-      <c r="AI65" s="14"/>
-      <c r="AJ65" s="14"/>
-      <c r="AK65" s="14"/>
-      <c r="AL65" s="14"/>
-      <c r="AM65" s="14"/>
-      <c r="AN65" s="14"/>
-      <c r="AO65" s="14"/>
-      <c r="AP65" s="14"/>
-      <c r="AQ65" s="14"/>
-      <c r="AR65" s="14"/>
-      <c r="AS65" s="14"/>
-      <c r="AT65" s="14"/>
-      <c r="AU65" s="14"/>
-      <c r="AV65" s="14"/>
-      <c r="AW65" s="14"/>
-      <c r="AX65" s="14"/>
-      <c r="AY65" s="14"/>
-      <c r="AZ65" s="14"/>
-      <c r="BA65" s="14"/>
-      <c r="BB65" s="14"/>
-      <c r="BC65" s="14"/>
-      <c r="BD65" s="14"/>
-      <c r="BE65" s="14"/>
-      <c r="BF65" s="14"/>
-      <c r="BG65" s="14"/>
-      <c r="BH65" s="14"/>
-      <c r="BI65" s="14"/>
-      <c r="BJ65" s="14"/>
-      <c r="BK65" s="14"/>
-      <c r="BL65" s="14"/>
-      <c r="BM65" s="14"/>
-      <c r="BN65" s="14"/>
-      <c r="BO65" s="14"/>
-      <c r="BP65" s="14"/>
-      <c r="BQ65" s="14"/>
-      <c r="BR65" s="14"/>
-      <c r="BS65" s="14"/>
-      <c r="BT65" s="14"/>
-      <c r="BU65" s="14"/>
-      <c r="BV65" s="14"/>
-      <c r="BW65" s="14"/>
-      <c r="BX65" s="14"/>
-      <c r="BY65" s="14"/>
-      <c r="BZ65" s="14"/>
-      <c r="CA65" s="14"/>
-      <c r="CB65" s="14"/>
-      <c r="CC65" s="14"/>
-      <c r="CD65" s="14"/>
-      <c r="CE65" s="14"/>
-      <c r="CF65" s="14"/>
-      <c r="CG65" s="14"/>
-      <c r="CH65" s="14"/>
-      <c r="CI65" s="14"/>
-      <c r="CJ65" s="14"/>
-      <c r="CK65" s="14"/>
-      <c r="CL65" s="14"/>
-      <c r="CM65" s="14"/>
-      <c r="CN65" s="14"/>
-      <c r="CO65" s="14"/>
-      <c r="CP65" s="14"/>
-      <c r="CQ65" s="14"/>
-      <c r="CR65" s="14"/>
-      <c r="CS65" s="14"/>
-      <c r="CT65" s="14"/>
-      <c r="CU65" s="14"/>
-      <c r="CV65" s="14"/>
-      <c r="CW65" s="14"/>
-      <c r="CX65" s="14"/>
-      <c r="CY65" s="14"/>
-      <c r="CZ65" s="14"/>
-      <c r="DA65" s="14"/>
-      <c r="DB65" s="14"/>
-      <c r="DC65" s="14"/>
-      <c r="DD65" s="14"/>
-      <c r="DE65" s="14"/>
-      <c r="DF65" s="14"/>
-      <c r="DG65" s="14"/>
-      <c r="DH65" s="14"/>
-      <c r="DI65" s="14"/>
-      <c r="DJ65" s="14"/>
-      <c r="DK65" s="14"/>
-      <c r="DL65" s="14"/>
-      <c r="DM65" s="14"/>
-      <c r="DN65" s="14"/>
-      <c r="DO65" s="14"/>
-      <c r="DP65" s="14"/>
-      <c r="DQ65" s="14"/>
-      <c r="DR65" s="14"/>
-      <c r="DS65" s="14"/>
-      <c r="DT65" s="14"/>
-      <c r="DU65" s="14"/>
-      <c r="DV65" s="14"/>
-      <c r="DW65" s="14"/>
-      <c r="DX65" s="14"/>
-      <c r="DY65" s="14"/>
-      <c r="DZ65" s="14"/>
-      <c r="EA65" s="14"/>
-      <c r="EB65" s="14"/>
-      <c r="EC65" s="14"/>
-      <c r="ED65" s="14"/>
-      <c r="EE65" s="14"/>
-      <c r="EF65" s="14"/>
-      <c r="EG65" s="14"/>
-      <c r="EH65" s="14"/>
-      <c r="EI65" s="14"/>
-      <c r="EJ65" s="14"/>
-      <c r="EK65" s="14"/>
-      <c r="EL65" s="14"/>
-      <c r="EM65" s="14"/>
-      <c r="EN65" s="14"/>
-      <c r="EO65" s="14"/>
-      <c r="EP65" s="14"/>
-      <c r="EQ65" s="14"/>
-      <c r="ER65" s="14"/>
-      <c r="ES65" s="14"/>
-      <c r="ET65" s="14"/>
-      <c r="EU65" s="14"/>
-      <c r="EV65" s="14"/>
-      <c r="EW65" s="14"/>
-      <c r="EX65" s="14"/>
-      <c r="EY65" s="14"/>
-      <c r="EZ65" s="14"/>
-      <c r="FA65" s="14"/>
-      <c r="FB65" s="14"/>
-      <c r="FC65" s="14"/>
-      <c r="FD65" s="14"/>
-      <c r="FE65" s="14"/>
-      <c r="FF65" s="14"/>
-      <c r="FG65" s="14"/>
-      <c r="FH65" s="14"/>
-      <c r="FI65" s="14"/>
-      <c r="FJ65" s="14"/>
-      <c r="FK65" s="14"/>
-      <c r="FL65" s="14"/>
-      <c r="FM65" s="14"/>
-      <c r="FN65" s="14"/>
-      <c r="FO65" s="14"/>
-      <c r="FP65" s="14"/>
-      <c r="FQ65" s="14"/>
-      <c r="FR65" s="14"/>
-      <c r="FS65" s="14"/>
-      <c r="FT65" s="14"/>
-      <c r="FU65" s="14"/>
-      <c r="FV65" s="14"/>
-      <c r="FW65" s="14"/>
-      <c r="FX65" s="14"/>
-      <c r="FY65" s="14"/>
-      <c r="FZ65" s="14"/>
-      <c r="GA65" s="14"/>
-      <c r="GB65" s="14"/>
-      <c r="GC65" s="14"/>
-      <c r="GD65" s="14"/>
-      <c r="GE65" s="14"/>
-      <c r="GF65" s="14"/>
-      <c r="GG65" s="14"/>
-      <c r="GH65" s="14"/>
-      <c r="GI65" s="14"/>
-      <c r="GJ65" s="14"/>
-      <c r="GK65" s="14"/>
-      <c r="GL65" s="14"/>
-      <c r="GM65" s="14"/>
-      <c r="GN65" s="14"/>
-      <c r="GO65" s="14"/>
-      <c r="GP65" s="14"/>
-      <c r="GQ65" s="14"/>
-      <c r="GR65" s="14"/>
-      <c r="GS65" s="14"/>
-      <c r="GT65" s="14"/>
-      <c r="GU65" s="14"/>
-      <c r="GV65" s="14"/>
-      <c r="GW65" s="14"/>
-      <c r="GX65" s="14"/>
-      <c r="GY65" s="14"/>
-      <c r="GZ65" s="14"/>
-      <c r="HA65" s="14"/>
-      <c r="HB65" s="14"/>
-      <c r="HC65" s="14"/>
-      <c r="HD65" s="14"/>
-      <c r="HE65" s="14"/>
-      <c r="HF65" s="14"/>
-      <c r="HG65" s="14"/>
-      <c r="HH65" s="14"/>
-      <c r="HI65" s="14"/>
-      <c r="HJ65" s="14"/>
-      <c r="HK65" s="14"/>
-      <c r="HL65" s="14"/>
-      <c r="HM65" s="14"/>
-      <c r="HN65" s="14"/>
-      <c r="HO65" s="14"/>
-      <c r="HP65" s="14"/>
-      <c r="HQ65" s="14"/>
-      <c r="HR65" s="14"/>
-      <c r="HS65" s="14"/>
-      <c r="HT65" s="14"/>
-      <c r="HU65" s="14"/>
-      <c r="HV65" s="14"/>
-      <c r="HW65" s="14"/>
-      <c r="HX65" s="14"/>
-      <c r="HY65" s="14"/>
-      <c r="HZ65" s="14"/>
-      <c r="IA65" s="14"/>
-      <c r="IB65" s="14"/>
-      <c r="IC65" s="14"/>
-      <c r="ID65" s="14"/>
-      <c r="IE65" s="14"/>
-      <c r="IF65" s="14"/>
-      <c r="IG65" s="14"/>
-      <c r="IH65" s="14"/>
-      <c r="II65" s="14"/>
-      <c r="IJ65" s="14"/>
-      <c r="IK65" s="14"/>
-      <c r="IL65" s="14"/>
-      <c r="IM65" s="14"/>
-      <c r="IN65" s="14"/>
-      <c r="IO65" s="14"/>
-      <c r="IP65" s="14"/>
-      <c r="IQ65" s="14"/>
-      <c r="IR65" s="14"/>
-      <c r="IS65" s="14"/>
-      <c r="IT65" s="14"/>
-      <c r="IU65" s="14"/>
-      <c r="IV65" s="14"/>
-      <c r="IW65" s="14"/>
-      <c r="IX65" s="14"/>
-      <c r="IY65" s="14"/>
-      <c r="IZ65" s="14"/>
-      <c r="JA65" s="14"/>
-      <c r="JB65" s="14"/>
-      <c r="JC65" s="14"/>
-      <c r="JD65" s="14"/>
-      <c r="JE65" s="14"/>
-      <c r="JF65" s="14"/>
-      <c r="JG65" s="14"/>
-      <c r="JH65" s="14"/>
-      <c r="JI65" s="14"/>
-      <c r="JJ65" s="14"/>
-      <c r="JK65" s="14"/>
-      <c r="JL65" s="14"/>
-      <c r="JM65" s="14"/>
-      <c r="JN65" s="14"/>
-      <c r="JO65" s="14"/>
-      <c r="JP65" s="14"/>
-      <c r="JQ65" s="14"/>
-      <c r="JR65" s="14"/>
-      <c r="JS65" s="14"/>
-      <c r="JT65" s="14"/>
-      <c r="JU65" s="14"/>
-      <c r="JV65" s="14"/>
-      <c r="JW65" s="14"/>
-      <c r="JX65" s="14"/>
-      <c r="JY65" s="14"/>
-      <c r="JZ65" s="14"/>
-      <c r="KA65" s="14"/>
-      <c r="KB65" s="14"/>
-      <c r="KC65" s="14"/>
-      <c r="KD65" s="14"/>
-      <c r="KE65" s="14"/>
-      <c r="KF65" s="14"/>
-      <c r="KG65" s="14"/>
-      <c r="KH65" s="14"/>
-      <c r="KI65" s="14"/>
-      <c r="KJ65" s="14"/>
-      <c r="KK65" s="14"/>
-      <c r="KL65" s="14"/>
-      <c r="KM65" s="14"/>
-      <c r="KN65" s="14"/>
-      <c r="KO65" s="14"/>
-      <c r="KP65" s="14"/>
-      <c r="KQ65" s="14"/>
-      <c r="KR65" s="14"/>
-      <c r="KS65" s="14"/>
-      <c r="KT65" s="14"/>
-      <c r="KU65" s="14"/>
-      <c r="KV65" s="14"/>
-      <c r="KW65" s="14"/>
-      <c r="KX65" s="14"/>
-      <c r="KY65" s="14"/>
-      <c r="KZ65" s="14"/>
-      <c r="LA65" s="14"/>
-      <c r="LB65" s="14"/>
-      <c r="LC65" s="14"/>
-      <c r="LD65" s="14"/>
-      <c r="LE65" s="14"/>
-      <c r="LF65" s="14"/>
-      <c r="LG65" s="14"/>
-      <c r="LH65" s="14"/>
-      <c r="LI65" s="14"/>
-      <c r="LJ65" s="14"/>
-      <c r="LK65" s="14"/>
-      <c r="LL65" s="14"/>
-      <c r="LM65" s="14"/>
-      <c r="LN65" s="14"/>
-      <c r="LO65" s="14"/>
-      <c r="LP65" s="14"/>
-      <c r="LQ65" s="14"/>
-      <c r="LR65" s="14"/>
-      <c r="LS65" s="14"/>
-      <c r="LT65" s="14"/>
-      <c r="LU65" s="14"/>
-      <c r="LV65" s="14"/>
-      <c r="LW65" s="14"/>
-      <c r="LX65" s="14"/>
-      <c r="LY65" s="14"/>
-      <c r="LZ65" s="14"/>
-      <c r="MA65" s="14"/>
-      <c r="MB65" s="14"/>
-      <c r="MC65" s="14"/>
-      <c r="MD65" s="14"/>
-      <c r="ME65" s="14"/>
-      <c r="MF65" s="14"/>
-      <c r="MG65" s="14"/>
-      <c r="MH65" s="14"/>
-      <c r="MI65" s="14"/>
-      <c r="MJ65" s="14"/>
-      <c r="MK65" s="14"/>
-      <c r="ML65" s="14"/>
-      <c r="MM65" s="14"/>
-      <c r="MN65" s="14"/>
-      <c r="MO65" s="14"/>
-      <c r="MP65" s="14"/>
-      <c r="MQ65" s="14"/>
-      <c r="MR65" s="14"/>
-      <c r="MS65" s="14"/>
-      <c r="MT65" s="14"/>
-      <c r="MU65" s="14"/>
-      <c r="MV65" s="14"/>
-      <c r="MW65" s="14"/>
-      <c r="MX65" s="14"/>
-      <c r="MY65" s="14"/>
-      <c r="MZ65" s="14"/>
-      <c r="NA65" s="14"/>
-      <c r="NB65" s="14"/>
-      <c r="NC65" s="14"/>
-      <c r="ND65" s="14"/>
-      <c r="NE65" s="14"/>
-      <c r="NF65" s="14"/>
-      <c r="NG65" s="14"/>
-      <c r="NH65" s="14"/>
-      <c r="NI65" s="14"/>
-      <c r="NJ65" s="14"/>
-      <c r="NK65" s="14"/>
-      <c r="NL65" s="14"/>
-      <c r="NM65" s="14"/>
-      <c r="NN65" s="14"/>
-      <c r="NO65" s="14"/>
-      <c r="NP65" s="14"/>
-      <c r="NQ65" s="14"/>
-      <c r="NR65" s="14"/>
-      <c r="NS65" s="14"/>
-      <c r="NT65" s="14"/>
-      <c r="NU65" s="14"/>
-      <c r="NV65" s="14"/>
-      <c r="NW65" s="14"/>
-      <c r="NX65" s="14"/>
-      <c r="NY65" s="14"/>
-      <c r="NZ65" s="14"/>
-      <c r="OA65" s="14"/>
-      <c r="OB65" s="14"/>
-      <c r="OC65" s="14"/>
-      <c r="OD65" s="14"/>
-      <c r="OE65" s="14"/>
-      <c r="OF65" s="14"/>
-      <c r="OG65" s="14"/>
-      <c r="OH65" s="14"/>
-      <c r="OI65" s="14"/>
-      <c r="OJ65" s="14"/>
-      <c r="OK65" s="14"/>
-      <c r="OL65" s="14"/>
-      <c r="OM65" s="14"/>
-      <c r="ON65" s="14"/>
-      <c r="OO65" s="14"/>
-      <c r="OP65" s="14"/>
-      <c r="OQ65" s="14"/>
-      <c r="OR65" s="14"/>
-      <c r="OS65" s="14"/>
-      <c r="OT65" s="14"/>
-      <c r="OU65" s="14"/>
-      <c r="OV65" s="14"/>
-      <c r="OW65" s="14"/>
-      <c r="OX65" s="14"/>
-      <c r="OY65" s="14"/>
-      <c r="OZ65" s="14"/>
-      <c r="PA65" s="14"/>
-      <c r="PB65" s="14"/>
-      <c r="PC65" s="14"/>
-      <c r="PD65" s="14"/>
-      <c r="PE65" s="14"/>
-      <c r="PF65" s="14"/>
-      <c r="PG65" s="14"/>
-      <c r="PH65" s="14"/>
-      <c r="PI65" s="14"/>
-      <c r="PJ65" s="14"/>
-      <c r="PK65" s="14"/>
-      <c r="PL65" s="14"/>
-      <c r="PM65" s="14"/>
-      <c r="PN65" s="14"/>
-      <c r="PO65" s="14"/>
-      <c r="PP65" s="14"/>
-      <c r="PQ65" s="14"/>
-      <c r="PR65" s="14"/>
-      <c r="PS65" s="14"/>
-      <c r="PT65" s="14"/>
-      <c r="PU65" s="14"/>
-      <c r="PV65" s="14"/>
-      <c r="PW65" s="14"/>
-      <c r="PX65" s="14"/>
-      <c r="PY65" s="14"/>
-      <c r="PZ65" s="14"/>
-      <c r="QA65" s="14"/>
-      <c r="QB65" s="14"/>
-      <c r="QC65" s="14"/>
-      <c r="QD65" s="14"/>
-      <c r="QE65" s="14"/>
-      <c r="QF65" s="14"/>
-      <c r="QG65" s="14"/>
-      <c r="QH65" s="14"/>
-      <c r="QI65" s="14"/>
-      <c r="QJ65" s="14"/>
-      <c r="QK65" s="14"/>
-      <c r="QL65" s="14"/>
-      <c r="QM65" s="14"/>
-      <c r="QN65" s="14"/>
-      <c r="QO65" s="14"/>
-      <c r="QP65" s="14"/>
-      <c r="QQ65" s="14"/>
-      <c r="QR65" s="14"/>
-      <c r="QS65" s="14"/>
-      <c r="QT65" s="14"/>
-      <c r="QU65" s="14"/>
-      <c r="QV65" s="14"/>
-      <c r="QW65" s="14"/>
-      <c r="QX65" s="14"/>
-      <c r="QY65" s="14"/>
-      <c r="QZ65" s="14"/>
-      <c r="RA65" s="14"/>
-      <c r="RB65" s="14"/>
-      <c r="RC65" s="14"/>
-      <c r="RD65" s="14"/>
-      <c r="RE65" s="14"/>
-      <c r="RF65" s="14"/>
-      <c r="RG65" s="14"/>
-      <c r="RH65" s="14"/>
-      <c r="RI65" s="14"/>
-      <c r="RJ65" s="14"/>
-      <c r="RK65" s="14"/>
-      <c r="RL65" s="14"/>
-      <c r="RM65" s="14"/>
-      <c r="RN65" s="14"/>
-      <c r="RO65" s="14"/>
-      <c r="RP65" s="14"/>
-      <c r="RQ65" s="14"/>
-      <c r="RR65" s="14"/>
-      <c r="RS65" s="14"/>
-      <c r="RT65" s="14"/>
-      <c r="RU65" s="14"/>
-      <c r="RV65" s="14"/>
-      <c r="RW65" s="14"/>
-      <c r="RX65" s="14"/>
-      <c r="RY65" s="14"/>
-      <c r="RZ65" s="14"/>
-      <c r="SA65" s="14"/>
-      <c r="SB65" s="14"/>
-      <c r="SC65" s="14"/>
-      <c r="SD65" s="14"/>
-      <c r="SE65" s="14"/>
-      <c r="SF65" s="14"/>
-      <c r="SG65" s="14"/>
-      <c r="SH65" s="14"/>
-      <c r="SI65" s="14"/>
-      <c r="SJ65" s="14"/>
-      <c r="SK65" s="14"/>
-      <c r="SL65" s="14"/>
-      <c r="SM65" s="14"/>
-      <c r="SN65" s="14"/>
-      <c r="SO65" s="14"/>
-      <c r="SP65" s="14"/>
-      <c r="SQ65" s="14"/>
-      <c r="SR65" s="14"/>
-      <c r="SS65" s="14"/>
-      <c r="ST65" s="14"/>
-      <c r="SU65" s="14"/>
-      <c r="SV65" s="14"/>
-      <c r="SW65" s="14"/>
-      <c r="SX65" s="14"/>
-      <c r="SY65" s="14"/>
-      <c r="SZ65" s="14"/>
-      <c r="TA65" s="14"/>
-      <c r="TB65" s="14"/>
-      <c r="TC65" s="14"/>
-      <c r="TD65" s="14"/>
-      <c r="TE65" s="14"/>
-      <c r="TF65" s="14"/>
-      <c r="TG65" s="14"/>
-      <c r="TH65" s="14"/>
-      <c r="TI65" s="14"/>
-      <c r="TJ65" s="14"/>
-      <c r="TK65" s="14"/>
-      <c r="TL65" s="14"/>
-      <c r="TM65" s="14"/>
-      <c r="TN65" s="14"/>
-      <c r="TO65" s="14"/>
-      <c r="TP65" s="14"/>
-      <c r="TQ65" s="14"/>
-      <c r="TR65" s="14"/>
-      <c r="TS65" s="14"/>
-      <c r="TT65" s="14"/>
-      <c r="TU65" s="14"/>
-      <c r="TV65" s="14"/>
-      <c r="TW65" s="14"/>
-      <c r="TX65" s="14"/>
-      <c r="TY65" s="14"/>
-      <c r="TZ65" s="14"/>
-      <c r="UA65" s="14"/>
-      <c r="UB65" s="14"/>
-      <c r="UC65" s="14"/>
-      <c r="UD65" s="14"/>
-      <c r="UE65" s="14"/>
-      <c r="UF65" s="14"/>
-      <c r="UG65" s="14"/>
-      <c r="UH65" s="14"/>
-      <c r="UI65" s="14"/>
-      <c r="UJ65" s="14"/>
-      <c r="UK65" s="14"/>
-      <c r="UL65" s="14"/>
-      <c r="UM65" s="14"/>
-      <c r="UN65" s="14"/>
-      <c r="UO65" s="14"/>
-      <c r="UP65" s="14"/>
-      <c r="UQ65" s="14"/>
-      <c r="UR65" s="14"/>
-      <c r="US65" s="14"/>
-      <c r="UT65" s="14"/>
-      <c r="UU65" s="14"/>
-      <c r="UV65" s="14"/>
-      <c r="UW65" s="14"/>
-      <c r="UX65" s="14"/>
-      <c r="UY65" s="14"/>
-      <c r="UZ65" s="14"/>
-      <c r="VA65" s="14"/>
-      <c r="VB65" s="14"/>
-      <c r="VC65" s="14"/>
-      <c r="VD65" s="14"/>
-      <c r="VE65" s="14"/>
-      <c r="VF65" s="14"/>
-      <c r="VG65" s="14"/>
-      <c r="VH65" s="14"/>
-      <c r="VI65" s="14"/>
-      <c r="VJ65" s="14"/>
-      <c r="VK65" s="14"/>
-      <c r="VL65" s="14"/>
-      <c r="VM65" s="14"/>
-      <c r="VN65" s="14"/>
-      <c r="VO65" s="14"/>
-      <c r="VP65" s="14"/>
-      <c r="VQ65" s="14"/>
-      <c r="VR65" s="14"/>
-      <c r="VS65" s="14"/>
-      <c r="VT65" s="14"/>
-      <c r="VU65" s="14"/>
-      <c r="VV65" s="14"/>
-      <c r="VW65" s="14"/>
-      <c r="VX65" s="14"/>
-      <c r="VY65" s="14"/>
-      <c r="VZ65" s="14"/>
-      <c r="WA65" s="14"/>
-      <c r="WB65" s="14"/>
-      <c r="WC65" s="14"/>
-      <c r="WD65" s="14"/>
-      <c r="WE65" s="14"/>
-      <c r="WF65" s="14"/>
-      <c r="WG65" s="14"/>
-      <c r="WH65" s="14"/>
-      <c r="WI65" s="14"/>
-      <c r="WJ65" s="14"/>
-      <c r="WK65" s="14"/>
-      <c r="WL65" s="14"/>
-      <c r="WM65" s="14"/>
-      <c r="WN65" s="14"/>
-      <c r="WO65" s="14"/>
-      <c r="WP65" s="14"/>
-      <c r="WQ65" s="14"/>
-      <c r="WR65" s="14"/>
-      <c r="WS65" s="14"/>
-      <c r="WT65" s="14"/>
-      <c r="WU65" s="14"/>
-      <c r="WV65" s="14"/>
-      <c r="WW65" s="14"/>
-      <c r="WX65" s="14"/>
-      <c r="WY65" s="14"/>
-      <c r="WZ65" s="14"/>
-      <c r="XA65" s="14"/>
-      <c r="XB65" s="14"/>
-      <c r="XC65" s="14"/>
-      <c r="XD65" s="14"/>
-      <c r="XE65" s="14"/>
-      <c r="XF65" s="14"/>
-      <c r="XG65" s="14"/>
-      <c r="XH65" s="14"/>
-      <c r="XI65" s="14"/>
-      <c r="XJ65" s="14"/>
-      <c r="XK65" s="14"/>
-      <c r="XL65" s="14"/>
-      <c r="XM65" s="14"/>
-      <c r="XN65" s="14"/>
-      <c r="XO65" s="14"/>
-      <c r="XP65" s="14"/>
-      <c r="XQ65" s="14"/>
-      <c r="XR65" s="14"/>
-      <c r="XS65" s="14"/>
-      <c r="XT65" s="14"/>
-      <c r="XU65" s="14"/>
-      <c r="XV65" s="14"/>
-      <c r="XW65" s="14"/>
-      <c r="XX65" s="14"/>
-      <c r="XY65" s="14"/>
-      <c r="XZ65" s="14"/>
-      <c r="YA65" s="14"/>
-      <c r="YB65" s="14"/>
-      <c r="YC65" s="14"/>
-      <c r="YD65" s="14"/>
-      <c r="YE65" s="14"/>
-      <c r="YF65" s="14"/>
-      <c r="YG65" s="14"/>
-      <c r="YH65" s="14"/>
-      <c r="YI65" s="14"/>
-      <c r="YJ65" s="14"/>
-      <c r="YK65" s="14"/>
-      <c r="YL65" s="14"/>
-      <c r="YM65" s="14"/>
-      <c r="YN65" s="14"/>
-      <c r="YO65" s="14"/>
-      <c r="YP65" s="14"/>
-      <c r="YQ65" s="14"/>
-      <c r="YR65" s="14"/>
-      <c r="YS65" s="14"/>
-      <c r="YT65" s="14"/>
-      <c r="YU65" s="14"/>
-      <c r="YV65" s="14"/>
-      <c r="YW65" s="14"/>
-      <c r="YX65" s="14"/>
-      <c r="YY65" s="14"/>
-      <c r="YZ65" s="14"/>
-      <c r="ZA65" s="14"/>
-      <c r="ZB65" s="14"/>
-      <c r="ZC65" s="14"/>
-      <c r="ZD65" s="14"/>
-      <c r="ZE65" s="14"/>
-      <c r="ZF65" s="14"/>
-      <c r="ZG65" s="14"/>
-      <c r="ZH65" s="14"/>
-      <c r="ZI65" s="14"/>
-      <c r="ZJ65" s="14"/>
-      <c r="ZK65" s="14"/>
-      <c r="ZL65" s="14"/>
-      <c r="ZM65" s="14"/>
-      <c r="ZN65" s="14"/>
-      <c r="ZO65" s="14"/>
-      <c r="ZP65" s="14"/>
-      <c r="ZQ65" s="14"/>
-      <c r="ZR65" s="14"/>
-      <c r="ZS65" s="14"/>
-      <c r="ZT65" s="14"/>
-      <c r="ZU65" s="14"/>
-      <c r="ZV65" s="14"/>
-      <c r="ZW65" s="14"/>
-      <c r="ZX65" s="14"/>
-      <c r="ZY65" s="14"/>
-      <c r="ZZ65" s="14"/>
-      <c r="AAA65" s="14"/>
-      <c r="AAB65" s="14"/>
-      <c r="AAC65" s="14"/>
-      <c r="AAD65" s="14"/>
-      <c r="AAE65" s="14"/>
-      <c r="AAF65" s="14"/>
-      <c r="AAG65" s="14"/>
-      <c r="AAH65" s="14"/>
-      <c r="AAI65" s="14"/>
-      <c r="AAJ65" s="14"/>
-      <c r="AAK65" s="14"/>
-      <c r="AAL65" s="14"/>
-      <c r="AAM65" s="14"/>
-      <c r="AAN65" s="14"/>
-      <c r="AAO65" s="14"/>
-      <c r="AAP65" s="14"/>
-      <c r="AAQ65" s="14"/>
-      <c r="AAR65" s="14"/>
-      <c r="AAS65" s="14"/>
-      <c r="AAT65" s="14"/>
-      <c r="AAU65" s="14"/>
-      <c r="AAV65" s="14"/>
-      <c r="AAW65" s="14"/>
-      <c r="AAX65" s="14"/>
-      <c r="AAY65" s="14"/>
-      <c r="AAZ65" s="14"/>
-      <c r="ABA65" s="14"/>
-      <c r="ABB65" s="14"/>
-      <c r="ABC65" s="14"/>
-      <c r="ABD65" s="14"/>
-      <c r="ABE65" s="14"/>
-      <c r="ABF65" s="14"/>
-      <c r="ABG65" s="14"/>
-      <c r="ABH65" s="14"/>
-      <c r="ABI65" s="14"/>
-      <c r="ABJ65" s="14"/>
-      <c r="ABK65" s="14"/>
-      <c r="ABL65" s="14"/>
-      <c r="ABM65" s="14"/>
-      <c r="ABN65" s="14"/>
-      <c r="ABO65" s="14"/>
-      <c r="ABP65" s="14"/>
-      <c r="ABQ65" s="14"/>
-      <c r="ABR65" s="14"/>
-      <c r="ABS65" s="14"/>
-      <c r="ABT65" s="14"/>
-      <c r="ABU65" s="14"/>
-      <c r="ABV65" s="14"/>
-      <c r="ABW65" s="14"/>
-      <c r="ABX65" s="14"/>
-      <c r="ABY65" s="14"/>
-      <c r="ABZ65" s="14"/>
-      <c r="ACA65" s="14"/>
-      <c r="ACB65" s="14"/>
-      <c r="ACC65" s="14"/>
-      <c r="ACD65" s="14"/>
-      <c r="ACE65" s="14"/>
-      <c r="ACF65" s="14"/>
-      <c r="ACG65" s="14"/>
-      <c r="ACH65" s="14"/>
-      <c r="ACI65" s="14"/>
-      <c r="ACJ65" s="14"/>
-      <c r="ACK65" s="14"/>
-      <c r="ACL65" s="14"/>
-      <c r="ACM65" s="14"/>
-      <c r="ACN65" s="14"/>
-      <c r="ACO65" s="14"/>
-      <c r="ACP65" s="14"/>
-      <c r="ACQ65" s="14"/>
-      <c r="ACR65" s="14"/>
-      <c r="ACS65" s="14"/>
-      <c r="ACT65" s="14"/>
-      <c r="ACU65" s="14"/>
-      <c r="ACV65" s="14"/>
-      <c r="ACW65" s="14"/>
-      <c r="ACX65" s="14"/>
-      <c r="ACY65" s="14"/>
-      <c r="ACZ65" s="14"/>
-      <c r="ADA65" s="14"/>
-      <c r="ADB65" s="14"/>
-      <c r="ADC65" s="14"/>
-      <c r="ADD65" s="14"/>
-      <c r="ADE65" s="14"/>
-      <c r="ADF65" s="14"/>
-      <c r="ADG65" s="14"/>
-      <c r="ADH65" s="14"/>
-      <c r="ADI65" s="14"/>
-      <c r="ADJ65" s="14"/>
-      <c r="ADK65" s="14"/>
-      <c r="ADL65" s="14"/>
-      <c r="ADM65" s="14"/>
-      <c r="ADN65" s="14"/>
-      <c r="ADO65" s="14"/>
-      <c r="ADP65" s="14"/>
-      <c r="ADQ65" s="14"/>
-      <c r="ADR65" s="14"/>
-      <c r="ADS65" s="14"/>
-      <c r="ADT65" s="14"/>
-      <c r="ADU65" s="14"/>
-      <c r="ADV65" s="14"/>
-      <c r="ADW65" s="14"/>
-      <c r="ADX65" s="14"/>
-      <c r="ADY65" s="14"/>
-      <c r="ADZ65" s="14"/>
-      <c r="AEA65" s="14"/>
-      <c r="AEB65" s="14"/>
-      <c r="AEC65" s="14"/>
-      <c r="AED65" s="14"/>
-      <c r="AEE65" s="14"/>
-      <c r="AEF65" s="14"/>
-      <c r="AEG65" s="14"/>
-      <c r="AEH65" s="14"/>
-      <c r="AEI65" s="14"/>
-      <c r="AEJ65" s="14"/>
-      <c r="AEK65" s="14"/>
-      <c r="AEL65" s="14"/>
-      <c r="AEM65" s="14"/>
-      <c r="AEN65" s="14"/>
-      <c r="AEO65" s="14"/>
-      <c r="AEP65" s="14"/>
-      <c r="AEQ65" s="14"/>
-      <c r="AER65" s="14"/>
-      <c r="AES65" s="14"/>
-      <c r="AET65" s="14"/>
-      <c r="AEU65" s="14"/>
-      <c r="AEV65" s="14"/>
-      <c r="AEW65" s="14"/>
-      <c r="AEX65" s="14"/>
-      <c r="AEY65" s="14"/>
-      <c r="AEZ65" s="14"/>
-      <c r="AFA65" s="14"/>
-      <c r="AFB65" s="14"/>
-      <c r="AFC65" s="14"/>
-      <c r="AFD65" s="14"/>
-      <c r="AFE65" s="14"/>
-      <c r="AFF65" s="14"/>
-      <c r="AFG65" s="14"/>
-      <c r="AFH65" s="14"/>
-      <c r="AFI65" s="14"/>
-      <c r="AFJ65" s="14"/>
-      <c r="AFK65" s="14"/>
-      <c r="AFL65" s="14"/>
-      <c r="AFM65" s="14"/>
-      <c r="AFN65" s="14"/>
-      <c r="AFO65" s="14"/>
-      <c r="AFP65" s="14"/>
-      <c r="AFQ65" s="14"/>
-      <c r="AFR65" s="14"/>
-      <c r="AFS65" s="14"/>
-      <c r="AFT65" s="14"/>
-      <c r="AFU65" s="14"/>
-      <c r="AFV65" s="14"/>
-      <c r="AFW65" s="14"/>
-      <c r="AFX65" s="14"/>
-      <c r="AFY65" s="14"/>
-      <c r="AFZ65" s="14"/>
-      <c r="AGA65" s="14"/>
-      <c r="AGB65" s="14"/>
-      <c r="AGC65" s="14"/>
-      <c r="AGD65" s="14"/>
-      <c r="AGE65" s="14"/>
-      <c r="AGF65" s="14"/>
-      <c r="AGG65" s="14"/>
-      <c r="AGH65" s="14"/>
-      <c r="AGI65" s="14"/>
-      <c r="AGJ65" s="14"/>
-      <c r="AGK65" s="14"/>
-      <c r="AGL65" s="14"/>
-      <c r="AGM65" s="14"/>
-      <c r="AGN65" s="14"/>
-      <c r="AGO65" s="14"/>
-      <c r="AGP65" s="14"/>
-      <c r="AGQ65" s="14"/>
-      <c r="AGR65" s="14"/>
-      <c r="AGS65" s="14"/>
-      <c r="AGT65" s="14"/>
-      <c r="AGU65" s="14"/>
-      <c r="AGV65" s="14"/>
-      <c r="AGW65" s="14"/>
-      <c r="AGX65" s="14"/>
-      <c r="AGY65" s="14"/>
-      <c r="AGZ65" s="14"/>
-      <c r="AHA65" s="14"/>
-      <c r="AHB65" s="14"/>
-      <c r="AHC65" s="14"/>
-      <c r="AHD65" s="14"/>
-      <c r="AHE65" s="14"/>
-      <c r="AHF65" s="14"/>
-      <c r="AHG65" s="14"/>
-      <c r="AHH65" s="14"/>
-      <c r="AHI65" s="14"/>
-      <c r="AHJ65" s="14"/>
-      <c r="AHK65" s="14"/>
-      <c r="AHL65" s="14"/>
-      <c r="AHM65" s="14"/>
-      <c r="AHN65" s="14"/>
-      <c r="AHO65" s="14"/>
-      <c r="AHP65" s="14"/>
-      <c r="AHQ65" s="14"/>
-      <c r="AHR65" s="14"/>
-      <c r="AHS65" s="14"/>
-      <c r="AHT65" s="14"/>
-      <c r="AHU65" s="14"/>
-      <c r="AHV65" s="14"/>
-      <c r="AHW65" s="14"/>
-      <c r="AHX65" s="14"/>
-      <c r="AHY65" s="14"/>
-      <c r="AHZ65" s="14"/>
-      <c r="AIA65" s="14"/>
-      <c r="AIB65" s="14"/>
-      <c r="AIC65" s="14"/>
-      <c r="AID65" s="14"/>
-      <c r="AIE65" s="14"/>
-      <c r="AIF65" s="14"/>
-      <c r="AIG65" s="14"/>
-      <c r="AIH65" s="14"/>
-      <c r="AII65" s="14"/>
-      <c r="AIJ65" s="14"/>
-      <c r="AIK65" s="14"/>
-      <c r="AIL65" s="14"/>
-      <c r="AIM65" s="14"/>
-      <c r="AIN65" s="14"/>
-      <c r="AIO65" s="14"/>
-      <c r="AIP65" s="14"/>
-      <c r="AIQ65" s="14"/>
-      <c r="AIR65" s="14"/>
-      <c r="AIS65" s="14"/>
-      <c r="AIT65" s="14"/>
-      <c r="AIU65" s="14"/>
-      <c r="AIV65" s="14"/>
-      <c r="AIW65" s="14"/>
-      <c r="AIX65" s="14"/>
-      <c r="AIY65" s="14"/>
-      <c r="AIZ65" s="14"/>
-      <c r="AJA65" s="14"/>
-      <c r="AJB65" s="14"/>
-      <c r="AJC65" s="14"/>
-      <c r="AJD65" s="14"/>
-      <c r="AJE65" s="14"/>
-      <c r="AJF65" s="14"/>
-      <c r="AJG65" s="14"/>
-      <c r="AJH65" s="14"/>
-      <c r="AJI65" s="14"/>
-      <c r="AJJ65" s="14"/>
-      <c r="AJK65" s="14"/>
-      <c r="AJL65" s="14"/>
-      <c r="AJM65" s="14"/>
-      <c r="AJN65" s="14"/>
-      <c r="AJO65" s="14"/>
-      <c r="AJP65" s="14"/>
-      <c r="AJQ65" s="14"/>
-      <c r="AJR65" s="14"/>
-      <c r="AJS65" s="14"/>
-      <c r="AJT65" s="14"/>
-      <c r="AJU65" s="14"/>
-      <c r="AJV65" s="14"/>
-      <c r="AJW65" s="14"/>
-      <c r="AJX65" s="14"/>
-      <c r="AJY65" s="14"/>
-      <c r="AJZ65" s="14"/>
-      <c r="AKA65" s="14"/>
-      <c r="AKB65" s="14"/>
-      <c r="AKC65" s="14"/>
-      <c r="AKD65" s="14"/>
-      <c r="AKE65" s="14"/>
-      <c r="AKF65" s="14"/>
-      <c r="AKG65" s="14"/>
-      <c r="AKH65" s="14"/>
-      <c r="AKI65" s="14"/>
-      <c r="AKJ65" s="14"/>
-      <c r="AKK65" s="14"/>
-      <c r="AKL65" s="14"/>
-      <c r="AKM65" s="14"/>
-      <c r="AKN65" s="14"/>
-      <c r="AKO65" s="14"/>
-      <c r="AKP65" s="14"/>
-      <c r="AKQ65" s="14"/>
-      <c r="AKR65" s="14"/>
-      <c r="AKS65" s="14"/>
-      <c r="AKT65" s="14"/>
-      <c r="AKU65" s="14"/>
-      <c r="AKV65" s="14"/>
-      <c r="AKW65" s="14"/>
-      <c r="AKX65" s="14"/>
-      <c r="AKY65" s="14"/>
-      <c r="AKZ65" s="14"/>
-      <c r="ALA65" s="14"/>
-      <c r="ALB65" s="14"/>
-      <c r="ALC65" s="14"/>
-      <c r="ALD65" s="14"/>
-      <c r="ALE65" s="14"/>
-      <c r="ALF65" s="14"/>
-      <c r="ALG65" s="14"/>
-      <c r="ALH65" s="14"/>
-      <c r="ALI65" s="14"/>
-      <c r="ALJ65" s="14"/>
-      <c r="ALK65" s="14"/>
-      <c r="ALL65" s="14"/>
-      <c r="ALM65" s="14"/>
-      <c r="ALN65" s="14"/>
-      <c r="ALO65" s="14"/>
-      <c r="ALP65" s="14"/>
-      <c r="ALQ65" s="14"/>
-      <c r="ALR65" s="14"/>
-      <c r="ALS65" s="14"/>
-      <c r="ALT65" s="14"/>
-      <c r="ALU65" s="14"/>
-      <c r="ALV65" s="14"/>
-      <c r="ALW65" s="14"/>
-      <c r="ALX65" s="14"/>
-      <c r="ALY65" s="14"/>
-      <c r="ALZ65" s="14"/>
-      <c r="AMA65" s="14"/>
-      <c r="AMB65" s="14"/>
-      <c r="AMC65" s="14"/>
-      <c r="AMD65" s="14"/>
-      <c r="AME65" s="14"/>
-      <c r="AMF65" s="14"/>
-      <c r="AMG65" s="14"/>
-      <c r="AMH65" s="14"/>
-      <c r="AMI65" s="14"/>
-      <c r="AMJ65" s="14"/>
-    </row>
-    <row r="66" s="20" customFormat="true" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="66" s="14" customFormat="true" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="14" t="s">
         <v>133</v>
       </c>
@@ -6498,1021 +5447,8 @@
       <c r="D66" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="L66" s="14"/>
-      <c r="M66" s="14"/>
-      <c r="N66" s="14"/>
-      <c r="O66" s="14"/>
-      <c r="P66" s="14"/>
-      <c r="Q66" s="14"/>
-      <c r="R66" s="14"/>
-      <c r="S66" s="14"/>
-      <c r="T66" s="14"/>
-      <c r="U66" s="14"/>
-      <c r="V66" s="14"/>
-      <c r="W66" s="14"/>
-      <c r="X66" s="14"/>
-      <c r="Y66" s="14"/>
-      <c r="Z66" s="14"/>
-      <c r="AA66" s="14"/>
-      <c r="AB66" s="14"/>
-      <c r="AC66" s="14"/>
-      <c r="AD66" s="14"/>
-      <c r="AE66" s="14"/>
-      <c r="AF66" s="14"/>
-      <c r="AG66" s="14"/>
-      <c r="AH66" s="14"/>
-      <c r="AI66" s="14"/>
-      <c r="AJ66" s="14"/>
-      <c r="AK66" s="14"/>
-      <c r="AL66" s="14"/>
-      <c r="AM66" s="14"/>
-      <c r="AN66" s="14"/>
-      <c r="AO66" s="14"/>
-      <c r="AP66" s="14"/>
-      <c r="AQ66" s="14"/>
-      <c r="AR66" s="14"/>
-      <c r="AS66" s="14"/>
-      <c r="AT66" s="14"/>
-      <c r="AU66" s="14"/>
-      <c r="AV66" s="14"/>
-      <c r="AW66" s="14"/>
-      <c r="AX66" s="14"/>
-      <c r="AY66" s="14"/>
-      <c r="AZ66" s="14"/>
-      <c r="BA66" s="14"/>
-      <c r="BB66" s="14"/>
-      <c r="BC66" s="14"/>
-      <c r="BD66" s="14"/>
-      <c r="BE66" s="14"/>
-      <c r="BF66" s="14"/>
-      <c r="BG66" s="14"/>
-      <c r="BH66" s="14"/>
-      <c r="BI66" s="14"/>
-      <c r="BJ66" s="14"/>
-      <c r="BK66" s="14"/>
-      <c r="BL66" s="14"/>
-      <c r="BM66" s="14"/>
-      <c r="BN66" s="14"/>
-      <c r="BO66" s="14"/>
-      <c r="BP66" s="14"/>
-      <c r="BQ66" s="14"/>
-      <c r="BR66" s="14"/>
-      <c r="BS66" s="14"/>
-      <c r="BT66" s="14"/>
-      <c r="BU66" s="14"/>
-      <c r="BV66" s="14"/>
-      <c r="BW66" s="14"/>
-      <c r="BX66" s="14"/>
-      <c r="BY66" s="14"/>
-      <c r="BZ66" s="14"/>
-      <c r="CA66" s="14"/>
-      <c r="CB66" s="14"/>
-      <c r="CC66" s="14"/>
-      <c r="CD66" s="14"/>
-      <c r="CE66" s="14"/>
-      <c r="CF66" s="14"/>
-      <c r="CG66" s="14"/>
-      <c r="CH66" s="14"/>
-      <c r="CI66" s="14"/>
-      <c r="CJ66" s="14"/>
-      <c r="CK66" s="14"/>
-      <c r="CL66" s="14"/>
-      <c r="CM66" s="14"/>
-      <c r="CN66" s="14"/>
-      <c r="CO66" s="14"/>
-      <c r="CP66" s="14"/>
-      <c r="CQ66" s="14"/>
-      <c r="CR66" s="14"/>
-      <c r="CS66" s="14"/>
-      <c r="CT66" s="14"/>
-      <c r="CU66" s="14"/>
-      <c r="CV66" s="14"/>
-      <c r="CW66" s="14"/>
-      <c r="CX66" s="14"/>
-      <c r="CY66" s="14"/>
-      <c r="CZ66" s="14"/>
-      <c r="DA66" s="14"/>
-      <c r="DB66" s="14"/>
-      <c r="DC66" s="14"/>
-      <c r="DD66" s="14"/>
-      <c r="DE66" s="14"/>
-      <c r="DF66" s="14"/>
-      <c r="DG66" s="14"/>
-      <c r="DH66" s="14"/>
-      <c r="DI66" s="14"/>
-      <c r="DJ66" s="14"/>
-      <c r="DK66" s="14"/>
-      <c r="DL66" s="14"/>
-      <c r="DM66" s="14"/>
-      <c r="DN66" s="14"/>
-      <c r="DO66" s="14"/>
-      <c r="DP66" s="14"/>
-      <c r="DQ66" s="14"/>
-      <c r="DR66" s="14"/>
-      <c r="DS66" s="14"/>
-      <c r="DT66" s="14"/>
-      <c r="DU66" s="14"/>
-      <c r="DV66" s="14"/>
-      <c r="DW66" s="14"/>
-      <c r="DX66" s="14"/>
-      <c r="DY66" s="14"/>
-      <c r="DZ66" s="14"/>
-      <c r="EA66" s="14"/>
-      <c r="EB66" s="14"/>
-      <c r="EC66" s="14"/>
-      <c r="ED66" s="14"/>
-      <c r="EE66" s="14"/>
-      <c r="EF66" s="14"/>
-      <c r="EG66" s="14"/>
-      <c r="EH66" s="14"/>
-      <c r="EI66" s="14"/>
-      <c r="EJ66" s="14"/>
-      <c r="EK66" s="14"/>
-      <c r="EL66" s="14"/>
-      <c r="EM66" s="14"/>
-      <c r="EN66" s="14"/>
-      <c r="EO66" s="14"/>
-      <c r="EP66" s="14"/>
-      <c r="EQ66" s="14"/>
-      <c r="ER66" s="14"/>
-      <c r="ES66" s="14"/>
-      <c r="ET66" s="14"/>
-      <c r="EU66" s="14"/>
-      <c r="EV66" s="14"/>
-      <c r="EW66" s="14"/>
-      <c r="EX66" s="14"/>
-      <c r="EY66" s="14"/>
-      <c r="EZ66" s="14"/>
-      <c r="FA66" s="14"/>
-      <c r="FB66" s="14"/>
-      <c r="FC66" s="14"/>
-      <c r="FD66" s="14"/>
-      <c r="FE66" s="14"/>
-      <c r="FF66" s="14"/>
-      <c r="FG66" s="14"/>
-      <c r="FH66" s="14"/>
-      <c r="FI66" s="14"/>
-      <c r="FJ66" s="14"/>
-      <c r="FK66" s="14"/>
-      <c r="FL66" s="14"/>
-      <c r="FM66" s="14"/>
-      <c r="FN66" s="14"/>
-      <c r="FO66" s="14"/>
-      <c r="FP66" s="14"/>
-      <c r="FQ66" s="14"/>
-      <c r="FR66" s="14"/>
-      <c r="FS66" s="14"/>
-      <c r="FT66" s="14"/>
-      <c r="FU66" s="14"/>
-      <c r="FV66" s="14"/>
-      <c r="FW66" s="14"/>
-      <c r="FX66" s="14"/>
-      <c r="FY66" s="14"/>
-      <c r="FZ66" s="14"/>
-      <c r="GA66" s="14"/>
-      <c r="GB66" s="14"/>
-      <c r="GC66" s="14"/>
-      <c r="GD66" s="14"/>
-      <c r="GE66" s="14"/>
-      <c r="GF66" s="14"/>
-      <c r="GG66" s="14"/>
-      <c r="GH66" s="14"/>
-      <c r="GI66" s="14"/>
-      <c r="GJ66" s="14"/>
-      <c r="GK66" s="14"/>
-      <c r="GL66" s="14"/>
-      <c r="GM66" s="14"/>
-      <c r="GN66" s="14"/>
-      <c r="GO66" s="14"/>
-      <c r="GP66" s="14"/>
-      <c r="GQ66" s="14"/>
-      <c r="GR66" s="14"/>
-      <c r="GS66" s="14"/>
-      <c r="GT66" s="14"/>
-      <c r="GU66" s="14"/>
-      <c r="GV66" s="14"/>
-      <c r="GW66" s="14"/>
-      <c r="GX66" s="14"/>
-      <c r="GY66" s="14"/>
-      <c r="GZ66" s="14"/>
-      <c r="HA66" s="14"/>
-      <c r="HB66" s="14"/>
-      <c r="HC66" s="14"/>
-      <c r="HD66" s="14"/>
-      <c r="HE66" s="14"/>
-      <c r="HF66" s="14"/>
-      <c r="HG66" s="14"/>
-      <c r="HH66" s="14"/>
-      <c r="HI66" s="14"/>
-      <c r="HJ66" s="14"/>
-      <c r="HK66" s="14"/>
-      <c r="HL66" s="14"/>
-      <c r="HM66" s="14"/>
-      <c r="HN66" s="14"/>
-      <c r="HO66" s="14"/>
-      <c r="HP66" s="14"/>
-      <c r="HQ66" s="14"/>
-      <c r="HR66" s="14"/>
-      <c r="HS66" s="14"/>
-      <c r="HT66" s="14"/>
-      <c r="HU66" s="14"/>
-      <c r="HV66" s="14"/>
-      <c r="HW66" s="14"/>
-      <c r="HX66" s="14"/>
-      <c r="HY66" s="14"/>
-      <c r="HZ66" s="14"/>
-      <c r="IA66" s="14"/>
-      <c r="IB66" s="14"/>
-      <c r="IC66" s="14"/>
-      <c r="ID66" s="14"/>
-      <c r="IE66" s="14"/>
-      <c r="IF66" s="14"/>
-      <c r="IG66" s="14"/>
-      <c r="IH66" s="14"/>
-      <c r="II66" s="14"/>
-      <c r="IJ66" s="14"/>
-      <c r="IK66" s="14"/>
-      <c r="IL66" s="14"/>
-      <c r="IM66" s="14"/>
-      <c r="IN66" s="14"/>
-      <c r="IO66" s="14"/>
-      <c r="IP66" s="14"/>
-      <c r="IQ66" s="14"/>
-      <c r="IR66" s="14"/>
-      <c r="IS66" s="14"/>
-      <c r="IT66" s="14"/>
-      <c r="IU66" s="14"/>
-      <c r="IV66" s="14"/>
-      <c r="IW66" s="14"/>
-      <c r="IX66" s="14"/>
-      <c r="IY66" s="14"/>
-      <c r="IZ66" s="14"/>
-      <c r="JA66" s="14"/>
-      <c r="JB66" s="14"/>
-      <c r="JC66" s="14"/>
-      <c r="JD66" s="14"/>
-      <c r="JE66" s="14"/>
-      <c r="JF66" s="14"/>
-      <c r="JG66" s="14"/>
-      <c r="JH66" s="14"/>
-      <c r="JI66" s="14"/>
-      <c r="JJ66" s="14"/>
-      <c r="JK66" s="14"/>
-      <c r="JL66" s="14"/>
-      <c r="JM66" s="14"/>
-      <c r="JN66" s="14"/>
-      <c r="JO66" s="14"/>
-      <c r="JP66" s="14"/>
-      <c r="JQ66" s="14"/>
-      <c r="JR66" s="14"/>
-      <c r="JS66" s="14"/>
-      <c r="JT66" s="14"/>
-      <c r="JU66" s="14"/>
-      <c r="JV66" s="14"/>
-      <c r="JW66" s="14"/>
-      <c r="JX66" s="14"/>
-      <c r="JY66" s="14"/>
-      <c r="JZ66" s="14"/>
-      <c r="KA66" s="14"/>
-      <c r="KB66" s="14"/>
-      <c r="KC66" s="14"/>
-      <c r="KD66" s="14"/>
-      <c r="KE66" s="14"/>
-      <c r="KF66" s="14"/>
-      <c r="KG66" s="14"/>
-      <c r="KH66" s="14"/>
-      <c r="KI66" s="14"/>
-      <c r="KJ66" s="14"/>
-      <c r="KK66" s="14"/>
-      <c r="KL66" s="14"/>
-      <c r="KM66" s="14"/>
-      <c r="KN66" s="14"/>
-      <c r="KO66" s="14"/>
-      <c r="KP66" s="14"/>
-      <c r="KQ66" s="14"/>
-      <c r="KR66" s="14"/>
-      <c r="KS66" s="14"/>
-      <c r="KT66" s="14"/>
-      <c r="KU66" s="14"/>
-      <c r="KV66" s="14"/>
-      <c r="KW66" s="14"/>
-      <c r="KX66" s="14"/>
-      <c r="KY66" s="14"/>
-      <c r="KZ66" s="14"/>
-      <c r="LA66" s="14"/>
-      <c r="LB66" s="14"/>
-      <c r="LC66" s="14"/>
-      <c r="LD66" s="14"/>
-      <c r="LE66" s="14"/>
-      <c r="LF66" s="14"/>
-      <c r="LG66" s="14"/>
-      <c r="LH66" s="14"/>
-      <c r="LI66" s="14"/>
-      <c r="LJ66" s="14"/>
-      <c r="LK66" s="14"/>
-      <c r="LL66" s="14"/>
-      <c r="LM66" s="14"/>
-      <c r="LN66" s="14"/>
-      <c r="LO66" s="14"/>
-      <c r="LP66" s="14"/>
-      <c r="LQ66" s="14"/>
-      <c r="LR66" s="14"/>
-      <c r="LS66" s="14"/>
-      <c r="LT66" s="14"/>
-      <c r="LU66" s="14"/>
-      <c r="LV66" s="14"/>
-      <c r="LW66" s="14"/>
-      <c r="LX66" s="14"/>
-      <c r="LY66" s="14"/>
-      <c r="LZ66" s="14"/>
-      <c r="MA66" s="14"/>
-      <c r="MB66" s="14"/>
-      <c r="MC66" s="14"/>
-      <c r="MD66" s="14"/>
-      <c r="ME66" s="14"/>
-      <c r="MF66" s="14"/>
-      <c r="MG66" s="14"/>
-      <c r="MH66" s="14"/>
-      <c r="MI66" s="14"/>
-      <c r="MJ66" s="14"/>
-      <c r="MK66" s="14"/>
-      <c r="ML66" s="14"/>
-      <c r="MM66" s="14"/>
-      <c r="MN66" s="14"/>
-      <c r="MO66" s="14"/>
-      <c r="MP66" s="14"/>
-      <c r="MQ66" s="14"/>
-      <c r="MR66" s="14"/>
-      <c r="MS66" s="14"/>
-      <c r="MT66" s="14"/>
-      <c r="MU66" s="14"/>
-      <c r="MV66" s="14"/>
-      <c r="MW66" s="14"/>
-      <c r="MX66" s="14"/>
-      <c r="MY66" s="14"/>
-      <c r="MZ66" s="14"/>
-      <c r="NA66" s="14"/>
-      <c r="NB66" s="14"/>
-      <c r="NC66" s="14"/>
-      <c r="ND66" s="14"/>
-      <c r="NE66" s="14"/>
-      <c r="NF66" s="14"/>
-      <c r="NG66" s="14"/>
-      <c r="NH66" s="14"/>
-      <c r="NI66" s="14"/>
-      <c r="NJ66" s="14"/>
-      <c r="NK66" s="14"/>
-      <c r="NL66" s="14"/>
-      <c r="NM66" s="14"/>
-      <c r="NN66" s="14"/>
-      <c r="NO66" s="14"/>
-      <c r="NP66" s="14"/>
-      <c r="NQ66" s="14"/>
-      <c r="NR66" s="14"/>
-      <c r="NS66" s="14"/>
-      <c r="NT66" s="14"/>
-      <c r="NU66" s="14"/>
-      <c r="NV66" s="14"/>
-      <c r="NW66" s="14"/>
-      <c r="NX66" s="14"/>
-      <c r="NY66" s="14"/>
-      <c r="NZ66" s="14"/>
-      <c r="OA66" s="14"/>
-      <c r="OB66" s="14"/>
-      <c r="OC66" s="14"/>
-      <c r="OD66" s="14"/>
-      <c r="OE66" s="14"/>
-      <c r="OF66" s="14"/>
-      <c r="OG66" s="14"/>
-      <c r="OH66" s="14"/>
-      <c r="OI66" s="14"/>
-      <c r="OJ66" s="14"/>
-      <c r="OK66" s="14"/>
-      <c r="OL66" s="14"/>
-      <c r="OM66" s="14"/>
-      <c r="ON66" s="14"/>
-      <c r="OO66" s="14"/>
-      <c r="OP66" s="14"/>
-      <c r="OQ66" s="14"/>
-      <c r="OR66" s="14"/>
-      <c r="OS66" s="14"/>
-      <c r="OT66" s="14"/>
-      <c r="OU66" s="14"/>
-      <c r="OV66" s="14"/>
-      <c r="OW66" s="14"/>
-      <c r="OX66" s="14"/>
-      <c r="OY66" s="14"/>
-      <c r="OZ66" s="14"/>
-      <c r="PA66" s="14"/>
-      <c r="PB66" s="14"/>
-      <c r="PC66" s="14"/>
-      <c r="PD66" s="14"/>
-      <c r="PE66" s="14"/>
-      <c r="PF66" s="14"/>
-      <c r="PG66" s="14"/>
-      <c r="PH66" s="14"/>
-      <c r="PI66" s="14"/>
-      <c r="PJ66" s="14"/>
-      <c r="PK66" s="14"/>
-      <c r="PL66" s="14"/>
-      <c r="PM66" s="14"/>
-      <c r="PN66" s="14"/>
-      <c r="PO66" s="14"/>
-      <c r="PP66" s="14"/>
-      <c r="PQ66" s="14"/>
-      <c r="PR66" s="14"/>
-      <c r="PS66" s="14"/>
-      <c r="PT66" s="14"/>
-      <c r="PU66" s="14"/>
-      <c r="PV66" s="14"/>
-      <c r="PW66" s="14"/>
-      <c r="PX66" s="14"/>
-      <c r="PY66" s="14"/>
-      <c r="PZ66" s="14"/>
-      <c r="QA66" s="14"/>
-      <c r="QB66" s="14"/>
-      <c r="QC66" s="14"/>
-      <c r="QD66" s="14"/>
-      <c r="QE66" s="14"/>
-      <c r="QF66" s="14"/>
-      <c r="QG66" s="14"/>
-      <c r="QH66" s="14"/>
-      <c r="QI66" s="14"/>
-      <c r="QJ66" s="14"/>
-      <c r="QK66" s="14"/>
-      <c r="QL66" s="14"/>
-      <c r="QM66" s="14"/>
-      <c r="QN66" s="14"/>
-      <c r="QO66" s="14"/>
-      <c r="QP66" s="14"/>
-      <c r="QQ66" s="14"/>
-      <c r="QR66" s="14"/>
-      <c r="QS66" s="14"/>
-      <c r="QT66" s="14"/>
-      <c r="QU66" s="14"/>
-      <c r="QV66" s="14"/>
-      <c r="QW66" s="14"/>
-      <c r="QX66" s="14"/>
-      <c r="QY66" s="14"/>
-      <c r="QZ66" s="14"/>
-      <c r="RA66" s="14"/>
-      <c r="RB66" s="14"/>
-      <c r="RC66" s="14"/>
-      <c r="RD66" s="14"/>
-      <c r="RE66" s="14"/>
-      <c r="RF66" s="14"/>
-      <c r="RG66" s="14"/>
-      <c r="RH66" s="14"/>
-      <c r="RI66" s="14"/>
-      <c r="RJ66" s="14"/>
-      <c r="RK66" s="14"/>
-      <c r="RL66" s="14"/>
-      <c r="RM66" s="14"/>
-      <c r="RN66" s="14"/>
-      <c r="RO66" s="14"/>
-      <c r="RP66" s="14"/>
-      <c r="RQ66" s="14"/>
-      <c r="RR66" s="14"/>
-      <c r="RS66" s="14"/>
-      <c r="RT66" s="14"/>
-      <c r="RU66" s="14"/>
-      <c r="RV66" s="14"/>
-      <c r="RW66" s="14"/>
-      <c r="RX66" s="14"/>
-      <c r="RY66" s="14"/>
-      <c r="RZ66" s="14"/>
-      <c r="SA66" s="14"/>
-      <c r="SB66" s="14"/>
-      <c r="SC66" s="14"/>
-      <c r="SD66" s="14"/>
-      <c r="SE66" s="14"/>
-      <c r="SF66" s="14"/>
-      <c r="SG66" s="14"/>
-      <c r="SH66" s="14"/>
-      <c r="SI66" s="14"/>
-      <c r="SJ66" s="14"/>
-      <c r="SK66" s="14"/>
-      <c r="SL66" s="14"/>
-      <c r="SM66" s="14"/>
-      <c r="SN66" s="14"/>
-      <c r="SO66" s="14"/>
-      <c r="SP66" s="14"/>
-      <c r="SQ66" s="14"/>
-      <c r="SR66" s="14"/>
-      <c r="SS66" s="14"/>
-      <c r="ST66" s="14"/>
-      <c r="SU66" s="14"/>
-      <c r="SV66" s="14"/>
-      <c r="SW66" s="14"/>
-      <c r="SX66" s="14"/>
-      <c r="SY66" s="14"/>
-      <c r="SZ66" s="14"/>
-      <c r="TA66" s="14"/>
-      <c r="TB66" s="14"/>
-      <c r="TC66" s="14"/>
-      <c r="TD66" s="14"/>
-      <c r="TE66" s="14"/>
-      <c r="TF66" s="14"/>
-      <c r="TG66" s="14"/>
-      <c r="TH66" s="14"/>
-      <c r="TI66" s="14"/>
-      <c r="TJ66" s="14"/>
-      <c r="TK66" s="14"/>
-      <c r="TL66" s="14"/>
-      <c r="TM66" s="14"/>
-      <c r="TN66" s="14"/>
-      <c r="TO66" s="14"/>
-      <c r="TP66" s="14"/>
-      <c r="TQ66" s="14"/>
-      <c r="TR66" s="14"/>
-      <c r="TS66" s="14"/>
-      <c r="TT66" s="14"/>
-      <c r="TU66" s="14"/>
-      <c r="TV66" s="14"/>
-      <c r="TW66" s="14"/>
-      <c r="TX66" s="14"/>
-      <c r="TY66" s="14"/>
-      <c r="TZ66" s="14"/>
-      <c r="UA66" s="14"/>
-      <c r="UB66" s="14"/>
-      <c r="UC66" s="14"/>
-      <c r="UD66" s="14"/>
-      <c r="UE66" s="14"/>
-      <c r="UF66" s="14"/>
-      <c r="UG66" s="14"/>
-      <c r="UH66" s="14"/>
-      <c r="UI66" s="14"/>
-      <c r="UJ66" s="14"/>
-      <c r="UK66" s="14"/>
-      <c r="UL66" s="14"/>
-      <c r="UM66" s="14"/>
-      <c r="UN66" s="14"/>
-      <c r="UO66" s="14"/>
-      <c r="UP66" s="14"/>
-      <c r="UQ66" s="14"/>
-      <c r="UR66" s="14"/>
-      <c r="US66" s="14"/>
-      <c r="UT66" s="14"/>
-      <c r="UU66" s="14"/>
-      <c r="UV66" s="14"/>
-      <c r="UW66" s="14"/>
-      <c r="UX66" s="14"/>
-      <c r="UY66" s="14"/>
-      <c r="UZ66" s="14"/>
-      <c r="VA66" s="14"/>
-      <c r="VB66" s="14"/>
-      <c r="VC66" s="14"/>
-      <c r="VD66" s="14"/>
-      <c r="VE66" s="14"/>
-      <c r="VF66" s="14"/>
-      <c r="VG66" s="14"/>
-      <c r="VH66" s="14"/>
-      <c r="VI66" s="14"/>
-      <c r="VJ66" s="14"/>
-      <c r="VK66" s="14"/>
-      <c r="VL66" s="14"/>
-      <c r="VM66" s="14"/>
-      <c r="VN66" s="14"/>
-      <c r="VO66" s="14"/>
-      <c r="VP66" s="14"/>
-      <c r="VQ66" s="14"/>
-      <c r="VR66" s="14"/>
-      <c r="VS66" s="14"/>
-      <c r="VT66" s="14"/>
-      <c r="VU66" s="14"/>
-      <c r="VV66" s="14"/>
-      <c r="VW66" s="14"/>
-      <c r="VX66" s="14"/>
-      <c r="VY66" s="14"/>
-      <c r="VZ66" s="14"/>
-      <c r="WA66" s="14"/>
-      <c r="WB66" s="14"/>
-      <c r="WC66" s="14"/>
-      <c r="WD66" s="14"/>
-      <c r="WE66" s="14"/>
-      <c r="WF66" s="14"/>
-      <c r="WG66" s="14"/>
-      <c r="WH66" s="14"/>
-      <c r="WI66" s="14"/>
-      <c r="WJ66" s="14"/>
-      <c r="WK66" s="14"/>
-      <c r="WL66" s="14"/>
-      <c r="WM66" s="14"/>
-      <c r="WN66" s="14"/>
-      <c r="WO66" s="14"/>
-      <c r="WP66" s="14"/>
-      <c r="WQ66" s="14"/>
-      <c r="WR66" s="14"/>
-      <c r="WS66" s="14"/>
-      <c r="WT66" s="14"/>
-      <c r="WU66" s="14"/>
-      <c r="WV66" s="14"/>
-      <c r="WW66" s="14"/>
-      <c r="WX66" s="14"/>
-      <c r="WY66" s="14"/>
-      <c r="WZ66" s="14"/>
-      <c r="XA66" s="14"/>
-      <c r="XB66" s="14"/>
-      <c r="XC66" s="14"/>
-      <c r="XD66" s="14"/>
-      <c r="XE66" s="14"/>
-      <c r="XF66" s="14"/>
-      <c r="XG66" s="14"/>
-      <c r="XH66" s="14"/>
-      <c r="XI66" s="14"/>
-      <c r="XJ66" s="14"/>
-      <c r="XK66" s="14"/>
-      <c r="XL66" s="14"/>
-      <c r="XM66" s="14"/>
-      <c r="XN66" s="14"/>
-      <c r="XO66" s="14"/>
-      <c r="XP66" s="14"/>
-      <c r="XQ66" s="14"/>
-      <c r="XR66" s="14"/>
-      <c r="XS66" s="14"/>
-      <c r="XT66" s="14"/>
-      <c r="XU66" s="14"/>
-      <c r="XV66" s="14"/>
-      <c r="XW66" s="14"/>
-      <c r="XX66" s="14"/>
-      <c r="XY66" s="14"/>
-      <c r="XZ66" s="14"/>
-      <c r="YA66" s="14"/>
-      <c r="YB66" s="14"/>
-      <c r="YC66" s="14"/>
-      <c r="YD66" s="14"/>
-      <c r="YE66" s="14"/>
-      <c r="YF66" s="14"/>
-      <c r="YG66" s="14"/>
-      <c r="YH66" s="14"/>
-      <c r="YI66" s="14"/>
-      <c r="YJ66" s="14"/>
-      <c r="YK66" s="14"/>
-      <c r="YL66" s="14"/>
-      <c r="YM66" s="14"/>
-      <c r="YN66" s="14"/>
-      <c r="YO66" s="14"/>
-      <c r="YP66" s="14"/>
-      <c r="YQ66" s="14"/>
-      <c r="YR66" s="14"/>
-      <c r="YS66" s="14"/>
-      <c r="YT66" s="14"/>
-      <c r="YU66" s="14"/>
-      <c r="YV66" s="14"/>
-      <c r="YW66" s="14"/>
-      <c r="YX66" s="14"/>
-      <c r="YY66" s="14"/>
-      <c r="YZ66" s="14"/>
-      <c r="ZA66" s="14"/>
-      <c r="ZB66" s="14"/>
-      <c r="ZC66" s="14"/>
-      <c r="ZD66" s="14"/>
-      <c r="ZE66" s="14"/>
-      <c r="ZF66" s="14"/>
-      <c r="ZG66" s="14"/>
-      <c r="ZH66" s="14"/>
-      <c r="ZI66" s="14"/>
-      <c r="ZJ66" s="14"/>
-      <c r="ZK66" s="14"/>
-      <c r="ZL66" s="14"/>
-      <c r="ZM66" s="14"/>
-      <c r="ZN66" s="14"/>
-      <c r="ZO66" s="14"/>
-      <c r="ZP66" s="14"/>
-      <c r="ZQ66" s="14"/>
-      <c r="ZR66" s="14"/>
-      <c r="ZS66" s="14"/>
-      <c r="ZT66" s="14"/>
-      <c r="ZU66" s="14"/>
-      <c r="ZV66" s="14"/>
-      <c r="ZW66" s="14"/>
-      <c r="ZX66" s="14"/>
-      <c r="ZY66" s="14"/>
-      <c r="ZZ66" s="14"/>
-      <c r="AAA66" s="14"/>
-      <c r="AAB66" s="14"/>
-      <c r="AAC66" s="14"/>
-      <c r="AAD66" s="14"/>
-      <c r="AAE66" s="14"/>
-      <c r="AAF66" s="14"/>
-      <c r="AAG66" s="14"/>
-      <c r="AAH66" s="14"/>
-      <c r="AAI66" s="14"/>
-      <c r="AAJ66" s="14"/>
-      <c r="AAK66" s="14"/>
-      <c r="AAL66" s="14"/>
-      <c r="AAM66" s="14"/>
-      <c r="AAN66" s="14"/>
-      <c r="AAO66" s="14"/>
-      <c r="AAP66" s="14"/>
-      <c r="AAQ66" s="14"/>
-      <c r="AAR66" s="14"/>
-      <c r="AAS66" s="14"/>
-      <c r="AAT66" s="14"/>
-      <c r="AAU66" s="14"/>
-      <c r="AAV66" s="14"/>
-      <c r="AAW66" s="14"/>
-      <c r="AAX66" s="14"/>
-      <c r="AAY66" s="14"/>
-      <c r="AAZ66" s="14"/>
-      <c r="ABA66" s="14"/>
-      <c r="ABB66" s="14"/>
-      <c r="ABC66" s="14"/>
-      <c r="ABD66" s="14"/>
-      <c r="ABE66" s="14"/>
-      <c r="ABF66" s="14"/>
-      <c r="ABG66" s="14"/>
-      <c r="ABH66" s="14"/>
-      <c r="ABI66" s="14"/>
-      <c r="ABJ66" s="14"/>
-      <c r="ABK66" s="14"/>
-      <c r="ABL66" s="14"/>
-      <c r="ABM66" s="14"/>
-      <c r="ABN66" s="14"/>
-      <c r="ABO66" s="14"/>
-      <c r="ABP66" s="14"/>
-      <c r="ABQ66" s="14"/>
-      <c r="ABR66" s="14"/>
-      <c r="ABS66" s="14"/>
-      <c r="ABT66" s="14"/>
-      <c r="ABU66" s="14"/>
-      <c r="ABV66" s="14"/>
-      <c r="ABW66" s="14"/>
-      <c r="ABX66" s="14"/>
-      <c r="ABY66" s="14"/>
-      <c r="ABZ66" s="14"/>
-      <c r="ACA66" s="14"/>
-      <c r="ACB66" s="14"/>
-      <c r="ACC66" s="14"/>
-      <c r="ACD66" s="14"/>
-      <c r="ACE66" s="14"/>
-      <c r="ACF66" s="14"/>
-      <c r="ACG66" s="14"/>
-      <c r="ACH66" s="14"/>
-      <c r="ACI66" s="14"/>
-      <c r="ACJ66" s="14"/>
-      <c r="ACK66" s="14"/>
-      <c r="ACL66" s="14"/>
-      <c r="ACM66" s="14"/>
-      <c r="ACN66" s="14"/>
-      <c r="ACO66" s="14"/>
-      <c r="ACP66" s="14"/>
-      <c r="ACQ66" s="14"/>
-      <c r="ACR66" s="14"/>
-      <c r="ACS66" s="14"/>
-      <c r="ACT66" s="14"/>
-      <c r="ACU66" s="14"/>
-      <c r="ACV66" s="14"/>
-      <c r="ACW66" s="14"/>
-      <c r="ACX66" s="14"/>
-      <c r="ACY66" s="14"/>
-      <c r="ACZ66" s="14"/>
-      <c r="ADA66" s="14"/>
-      <c r="ADB66" s="14"/>
-      <c r="ADC66" s="14"/>
-      <c r="ADD66" s="14"/>
-      <c r="ADE66" s="14"/>
-      <c r="ADF66" s="14"/>
-      <c r="ADG66" s="14"/>
-      <c r="ADH66" s="14"/>
-      <c r="ADI66" s="14"/>
-      <c r="ADJ66" s="14"/>
-      <c r="ADK66" s="14"/>
-      <c r="ADL66" s="14"/>
-      <c r="ADM66" s="14"/>
-      <c r="ADN66" s="14"/>
-      <c r="ADO66" s="14"/>
-      <c r="ADP66" s="14"/>
-      <c r="ADQ66" s="14"/>
-      <c r="ADR66" s="14"/>
-      <c r="ADS66" s="14"/>
-      <c r="ADT66" s="14"/>
-      <c r="ADU66" s="14"/>
-      <c r="ADV66" s="14"/>
-      <c r="ADW66" s="14"/>
-      <c r="ADX66" s="14"/>
-      <c r="ADY66" s="14"/>
-      <c r="ADZ66" s="14"/>
-      <c r="AEA66" s="14"/>
-      <c r="AEB66" s="14"/>
-      <c r="AEC66" s="14"/>
-      <c r="AED66" s="14"/>
-      <c r="AEE66" s="14"/>
-      <c r="AEF66" s="14"/>
-      <c r="AEG66" s="14"/>
-      <c r="AEH66" s="14"/>
-      <c r="AEI66" s="14"/>
-      <c r="AEJ66" s="14"/>
-      <c r="AEK66" s="14"/>
-      <c r="AEL66" s="14"/>
-      <c r="AEM66" s="14"/>
-      <c r="AEN66" s="14"/>
-      <c r="AEO66" s="14"/>
-      <c r="AEP66" s="14"/>
-      <c r="AEQ66" s="14"/>
-      <c r="AER66" s="14"/>
-      <c r="AES66" s="14"/>
-      <c r="AET66" s="14"/>
-      <c r="AEU66" s="14"/>
-      <c r="AEV66" s="14"/>
-      <c r="AEW66" s="14"/>
-      <c r="AEX66" s="14"/>
-      <c r="AEY66" s="14"/>
-      <c r="AEZ66" s="14"/>
-      <c r="AFA66" s="14"/>
-      <c r="AFB66" s="14"/>
-      <c r="AFC66" s="14"/>
-      <c r="AFD66" s="14"/>
-      <c r="AFE66" s="14"/>
-      <c r="AFF66" s="14"/>
-      <c r="AFG66" s="14"/>
-      <c r="AFH66" s="14"/>
-      <c r="AFI66" s="14"/>
-      <c r="AFJ66" s="14"/>
-      <c r="AFK66" s="14"/>
-      <c r="AFL66" s="14"/>
-      <c r="AFM66" s="14"/>
-      <c r="AFN66" s="14"/>
-      <c r="AFO66" s="14"/>
-      <c r="AFP66" s="14"/>
-      <c r="AFQ66" s="14"/>
-      <c r="AFR66" s="14"/>
-      <c r="AFS66" s="14"/>
-      <c r="AFT66" s="14"/>
-      <c r="AFU66" s="14"/>
-      <c r="AFV66" s="14"/>
-      <c r="AFW66" s="14"/>
-      <c r="AFX66" s="14"/>
-      <c r="AFY66" s="14"/>
-      <c r="AFZ66" s="14"/>
-      <c r="AGA66" s="14"/>
-      <c r="AGB66" s="14"/>
-      <c r="AGC66" s="14"/>
-      <c r="AGD66" s="14"/>
-      <c r="AGE66" s="14"/>
-      <c r="AGF66" s="14"/>
-      <c r="AGG66" s="14"/>
-      <c r="AGH66" s="14"/>
-      <c r="AGI66" s="14"/>
-      <c r="AGJ66" s="14"/>
-      <c r="AGK66" s="14"/>
-      <c r="AGL66" s="14"/>
-      <c r="AGM66" s="14"/>
-      <c r="AGN66" s="14"/>
-      <c r="AGO66" s="14"/>
-      <c r="AGP66" s="14"/>
-      <c r="AGQ66" s="14"/>
-      <c r="AGR66" s="14"/>
-      <c r="AGS66" s="14"/>
-      <c r="AGT66" s="14"/>
-      <c r="AGU66" s="14"/>
-      <c r="AGV66" s="14"/>
-      <c r="AGW66" s="14"/>
-      <c r="AGX66" s="14"/>
-      <c r="AGY66" s="14"/>
-      <c r="AGZ66" s="14"/>
-      <c r="AHA66" s="14"/>
-      <c r="AHB66" s="14"/>
-      <c r="AHC66" s="14"/>
-      <c r="AHD66" s="14"/>
-      <c r="AHE66" s="14"/>
-      <c r="AHF66" s="14"/>
-      <c r="AHG66" s="14"/>
-      <c r="AHH66" s="14"/>
-      <c r="AHI66" s="14"/>
-      <c r="AHJ66" s="14"/>
-      <c r="AHK66" s="14"/>
-      <c r="AHL66" s="14"/>
-      <c r="AHM66" s="14"/>
-      <c r="AHN66" s="14"/>
-      <c r="AHO66" s="14"/>
-      <c r="AHP66" s="14"/>
-      <c r="AHQ66" s="14"/>
-      <c r="AHR66" s="14"/>
-      <c r="AHS66" s="14"/>
-      <c r="AHT66" s="14"/>
-      <c r="AHU66" s="14"/>
-      <c r="AHV66" s="14"/>
-      <c r="AHW66" s="14"/>
-      <c r="AHX66" s="14"/>
-      <c r="AHY66" s="14"/>
-      <c r="AHZ66" s="14"/>
-      <c r="AIA66" s="14"/>
-      <c r="AIB66" s="14"/>
-      <c r="AIC66" s="14"/>
-      <c r="AID66" s="14"/>
-      <c r="AIE66" s="14"/>
-      <c r="AIF66" s="14"/>
-      <c r="AIG66" s="14"/>
-      <c r="AIH66" s="14"/>
-      <c r="AII66" s="14"/>
-      <c r="AIJ66" s="14"/>
-      <c r="AIK66" s="14"/>
-      <c r="AIL66" s="14"/>
-      <c r="AIM66" s="14"/>
-      <c r="AIN66" s="14"/>
-      <c r="AIO66" s="14"/>
-      <c r="AIP66" s="14"/>
-      <c r="AIQ66" s="14"/>
-      <c r="AIR66" s="14"/>
-      <c r="AIS66" s="14"/>
-      <c r="AIT66" s="14"/>
-      <c r="AIU66" s="14"/>
-      <c r="AIV66" s="14"/>
-      <c r="AIW66" s="14"/>
-      <c r="AIX66" s="14"/>
-      <c r="AIY66" s="14"/>
-      <c r="AIZ66" s="14"/>
-      <c r="AJA66" s="14"/>
-      <c r="AJB66" s="14"/>
-      <c r="AJC66" s="14"/>
-      <c r="AJD66" s="14"/>
-      <c r="AJE66" s="14"/>
-      <c r="AJF66" s="14"/>
-      <c r="AJG66" s="14"/>
-      <c r="AJH66" s="14"/>
-      <c r="AJI66" s="14"/>
-      <c r="AJJ66" s="14"/>
-      <c r="AJK66" s="14"/>
-      <c r="AJL66" s="14"/>
-      <c r="AJM66" s="14"/>
-      <c r="AJN66" s="14"/>
-      <c r="AJO66" s="14"/>
-      <c r="AJP66" s="14"/>
-      <c r="AJQ66" s="14"/>
-      <c r="AJR66" s="14"/>
-      <c r="AJS66" s="14"/>
-      <c r="AJT66" s="14"/>
-      <c r="AJU66" s="14"/>
-      <c r="AJV66" s="14"/>
-      <c r="AJW66" s="14"/>
-      <c r="AJX66" s="14"/>
-      <c r="AJY66" s="14"/>
-      <c r="AJZ66" s="14"/>
-      <c r="AKA66" s="14"/>
-      <c r="AKB66" s="14"/>
-      <c r="AKC66" s="14"/>
-      <c r="AKD66" s="14"/>
-      <c r="AKE66" s="14"/>
-      <c r="AKF66" s="14"/>
-      <c r="AKG66" s="14"/>
-      <c r="AKH66" s="14"/>
-      <c r="AKI66" s="14"/>
-      <c r="AKJ66" s="14"/>
-      <c r="AKK66" s="14"/>
-      <c r="AKL66" s="14"/>
-      <c r="AKM66" s="14"/>
-      <c r="AKN66" s="14"/>
-      <c r="AKO66" s="14"/>
-      <c r="AKP66" s="14"/>
-      <c r="AKQ66" s="14"/>
-      <c r="AKR66" s="14"/>
-      <c r="AKS66" s="14"/>
-      <c r="AKT66" s="14"/>
-      <c r="AKU66" s="14"/>
-      <c r="AKV66" s="14"/>
-      <c r="AKW66" s="14"/>
-      <c r="AKX66" s="14"/>
-      <c r="AKY66" s="14"/>
-      <c r="AKZ66" s="14"/>
-      <c r="ALA66" s="14"/>
-      <c r="ALB66" s="14"/>
-      <c r="ALC66" s="14"/>
-      <c r="ALD66" s="14"/>
-      <c r="ALE66" s="14"/>
-      <c r="ALF66" s="14"/>
-      <c r="ALG66" s="14"/>
-      <c r="ALH66" s="14"/>
-      <c r="ALI66" s="14"/>
-      <c r="ALJ66" s="14"/>
-      <c r="ALK66" s="14"/>
-      <c r="ALL66" s="14"/>
-      <c r="ALM66" s="14"/>
-      <c r="ALN66" s="14"/>
-      <c r="ALO66" s="14"/>
-      <c r="ALP66" s="14"/>
-      <c r="ALQ66" s="14"/>
-      <c r="ALR66" s="14"/>
-      <c r="ALS66" s="14"/>
-      <c r="ALT66" s="14"/>
-      <c r="ALU66" s="14"/>
-      <c r="ALV66" s="14"/>
-      <c r="ALW66" s="14"/>
-      <c r="ALX66" s="14"/>
-      <c r="ALY66" s="14"/>
-      <c r="ALZ66" s="14"/>
-      <c r="AMA66" s="14"/>
-      <c r="AMB66" s="14"/>
-      <c r="AMC66" s="14"/>
-      <c r="AMD66" s="14"/>
-      <c r="AME66" s="14"/>
-      <c r="AMF66" s="14"/>
-      <c r="AMG66" s="14"/>
-      <c r="AMH66" s="14"/>
-      <c r="AMI66" s="14"/>
-      <c r="AMJ66" s="14"/>
-    </row>
-    <row r="67" s="20" customFormat="true" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="67" s="14" customFormat="true" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="14" t="s">
         <v>134</v>
       </c>
@@ -7523,1019 +5459,6 @@
       <c r="D67" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="L67" s="14"/>
-      <c r="M67" s="14"/>
-      <c r="N67" s="14"/>
-      <c r="O67" s="14"/>
-      <c r="P67" s="14"/>
-      <c r="Q67" s="14"/>
-      <c r="R67" s="14"/>
-      <c r="S67" s="14"/>
-      <c r="T67" s="14"/>
-      <c r="U67" s="14"/>
-      <c r="V67" s="14"/>
-      <c r="W67" s="14"/>
-      <c r="X67" s="14"/>
-      <c r="Y67" s="14"/>
-      <c r="Z67" s="14"/>
-      <c r="AA67" s="14"/>
-      <c r="AB67" s="14"/>
-      <c r="AC67" s="14"/>
-      <c r="AD67" s="14"/>
-      <c r="AE67" s="14"/>
-      <c r="AF67" s="14"/>
-      <c r="AG67" s="14"/>
-      <c r="AH67" s="14"/>
-      <c r="AI67" s="14"/>
-      <c r="AJ67" s="14"/>
-      <c r="AK67" s="14"/>
-      <c r="AL67" s="14"/>
-      <c r="AM67" s="14"/>
-      <c r="AN67" s="14"/>
-      <c r="AO67" s="14"/>
-      <c r="AP67" s="14"/>
-      <c r="AQ67" s="14"/>
-      <c r="AR67" s="14"/>
-      <c r="AS67" s="14"/>
-      <c r="AT67" s="14"/>
-      <c r="AU67" s="14"/>
-      <c r="AV67" s="14"/>
-      <c r="AW67" s="14"/>
-      <c r="AX67" s="14"/>
-      <c r="AY67" s="14"/>
-      <c r="AZ67" s="14"/>
-      <c r="BA67" s="14"/>
-      <c r="BB67" s="14"/>
-      <c r="BC67" s="14"/>
-      <c r="BD67" s="14"/>
-      <c r="BE67" s="14"/>
-      <c r="BF67" s="14"/>
-      <c r="BG67" s="14"/>
-      <c r="BH67" s="14"/>
-      <c r="BI67" s="14"/>
-      <c r="BJ67" s="14"/>
-      <c r="BK67" s="14"/>
-      <c r="BL67" s="14"/>
-      <c r="BM67" s="14"/>
-      <c r="BN67" s="14"/>
-      <c r="BO67" s="14"/>
-      <c r="BP67" s="14"/>
-      <c r="BQ67" s="14"/>
-      <c r="BR67" s="14"/>
-      <c r="BS67" s="14"/>
-      <c r="BT67" s="14"/>
-      <c r="BU67" s="14"/>
-      <c r="BV67" s="14"/>
-      <c r="BW67" s="14"/>
-      <c r="BX67" s="14"/>
-      <c r="BY67" s="14"/>
-      <c r="BZ67" s="14"/>
-      <c r="CA67" s="14"/>
-      <c r="CB67" s="14"/>
-      <c r="CC67" s="14"/>
-      <c r="CD67" s="14"/>
-      <c r="CE67" s="14"/>
-      <c r="CF67" s="14"/>
-      <c r="CG67" s="14"/>
-      <c r="CH67" s="14"/>
-      <c r="CI67" s="14"/>
-      <c r="CJ67" s="14"/>
-      <c r="CK67" s="14"/>
-      <c r="CL67" s="14"/>
-      <c r="CM67" s="14"/>
-      <c r="CN67" s="14"/>
-      <c r="CO67" s="14"/>
-      <c r="CP67" s="14"/>
-      <c r="CQ67" s="14"/>
-      <c r="CR67" s="14"/>
-      <c r="CS67" s="14"/>
-      <c r="CT67" s="14"/>
-      <c r="CU67" s="14"/>
-      <c r="CV67" s="14"/>
-      <c r="CW67" s="14"/>
-      <c r="CX67" s="14"/>
-      <c r="CY67" s="14"/>
-      <c r="CZ67" s="14"/>
-      <c r="DA67" s="14"/>
-      <c r="DB67" s="14"/>
-      <c r="DC67" s="14"/>
-      <c r="DD67" s="14"/>
-      <c r="DE67" s="14"/>
-      <c r="DF67" s="14"/>
-      <c r="DG67" s="14"/>
-      <c r="DH67" s="14"/>
-      <c r="DI67" s="14"/>
-      <c r="DJ67" s="14"/>
-      <c r="DK67" s="14"/>
-      <c r="DL67" s="14"/>
-      <c r="DM67" s="14"/>
-      <c r="DN67" s="14"/>
-      <c r="DO67" s="14"/>
-      <c r="DP67" s="14"/>
-      <c r="DQ67" s="14"/>
-      <c r="DR67" s="14"/>
-      <c r="DS67" s="14"/>
-      <c r="DT67" s="14"/>
-      <c r="DU67" s="14"/>
-      <c r="DV67" s="14"/>
-      <c r="DW67" s="14"/>
-      <c r="DX67" s="14"/>
-      <c r="DY67" s="14"/>
-      <c r="DZ67" s="14"/>
-      <c r="EA67" s="14"/>
-      <c r="EB67" s="14"/>
-      <c r="EC67" s="14"/>
-      <c r="ED67" s="14"/>
-      <c r="EE67" s="14"/>
-      <c r="EF67" s="14"/>
-      <c r="EG67" s="14"/>
-      <c r="EH67" s="14"/>
-      <c r="EI67" s="14"/>
-      <c r="EJ67" s="14"/>
-      <c r="EK67" s="14"/>
-      <c r="EL67" s="14"/>
-      <c r="EM67" s="14"/>
-      <c r="EN67" s="14"/>
-      <c r="EO67" s="14"/>
-      <c r="EP67" s="14"/>
-      <c r="EQ67" s="14"/>
-      <c r="ER67" s="14"/>
-      <c r="ES67" s="14"/>
-      <c r="ET67" s="14"/>
-      <c r="EU67" s="14"/>
-      <c r="EV67" s="14"/>
-      <c r="EW67" s="14"/>
-      <c r="EX67" s="14"/>
-      <c r="EY67" s="14"/>
-      <c r="EZ67" s="14"/>
-      <c r="FA67" s="14"/>
-      <c r="FB67" s="14"/>
-      <c r="FC67" s="14"/>
-      <c r="FD67" s="14"/>
-      <c r="FE67" s="14"/>
-      <c r="FF67" s="14"/>
-      <c r="FG67" s="14"/>
-      <c r="FH67" s="14"/>
-      <c r="FI67" s="14"/>
-      <c r="FJ67" s="14"/>
-      <c r="FK67" s="14"/>
-      <c r="FL67" s="14"/>
-      <c r="FM67" s="14"/>
-      <c r="FN67" s="14"/>
-      <c r="FO67" s="14"/>
-      <c r="FP67" s="14"/>
-      <c r="FQ67" s="14"/>
-      <c r="FR67" s="14"/>
-      <c r="FS67" s="14"/>
-      <c r="FT67" s="14"/>
-      <c r="FU67" s="14"/>
-      <c r="FV67" s="14"/>
-      <c r="FW67" s="14"/>
-      <c r="FX67" s="14"/>
-      <c r="FY67" s="14"/>
-      <c r="FZ67" s="14"/>
-      <c r="GA67" s="14"/>
-      <c r="GB67" s="14"/>
-      <c r="GC67" s="14"/>
-      <c r="GD67" s="14"/>
-      <c r="GE67" s="14"/>
-      <c r="GF67" s="14"/>
-      <c r="GG67" s="14"/>
-      <c r="GH67" s="14"/>
-      <c r="GI67" s="14"/>
-      <c r="GJ67" s="14"/>
-      <c r="GK67" s="14"/>
-      <c r="GL67" s="14"/>
-      <c r="GM67" s="14"/>
-      <c r="GN67" s="14"/>
-      <c r="GO67" s="14"/>
-      <c r="GP67" s="14"/>
-      <c r="GQ67" s="14"/>
-      <c r="GR67" s="14"/>
-      <c r="GS67" s="14"/>
-      <c r="GT67" s="14"/>
-      <c r="GU67" s="14"/>
-      <c r="GV67" s="14"/>
-      <c r="GW67" s="14"/>
-      <c r="GX67" s="14"/>
-      <c r="GY67" s="14"/>
-      <c r="GZ67" s="14"/>
-      <c r="HA67" s="14"/>
-      <c r="HB67" s="14"/>
-      <c r="HC67" s="14"/>
-      <c r="HD67" s="14"/>
-      <c r="HE67" s="14"/>
-      <c r="HF67" s="14"/>
-      <c r="HG67" s="14"/>
-      <c r="HH67" s="14"/>
-      <c r="HI67" s="14"/>
-      <c r="HJ67" s="14"/>
-      <c r="HK67" s="14"/>
-      <c r="HL67" s="14"/>
-      <c r="HM67" s="14"/>
-      <c r="HN67" s="14"/>
-      <c r="HO67" s="14"/>
-      <c r="HP67" s="14"/>
-      <c r="HQ67" s="14"/>
-      <c r="HR67" s="14"/>
-      <c r="HS67" s="14"/>
-      <c r="HT67" s="14"/>
-      <c r="HU67" s="14"/>
-      <c r="HV67" s="14"/>
-      <c r="HW67" s="14"/>
-      <c r="HX67" s="14"/>
-      <c r="HY67" s="14"/>
-      <c r="HZ67" s="14"/>
-      <c r="IA67" s="14"/>
-      <c r="IB67" s="14"/>
-      <c r="IC67" s="14"/>
-      <c r="ID67" s="14"/>
-      <c r="IE67" s="14"/>
-      <c r="IF67" s="14"/>
-      <c r="IG67" s="14"/>
-      <c r="IH67" s="14"/>
-      <c r="II67" s="14"/>
-      <c r="IJ67" s="14"/>
-      <c r="IK67" s="14"/>
-      <c r="IL67" s="14"/>
-      <c r="IM67" s="14"/>
-      <c r="IN67" s="14"/>
-      <c r="IO67" s="14"/>
-      <c r="IP67" s="14"/>
-      <c r="IQ67" s="14"/>
-      <c r="IR67" s="14"/>
-      <c r="IS67" s="14"/>
-      <c r="IT67" s="14"/>
-      <c r="IU67" s="14"/>
-      <c r="IV67" s="14"/>
-      <c r="IW67" s="14"/>
-      <c r="IX67" s="14"/>
-      <c r="IY67" s="14"/>
-      <c r="IZ67" s="14"/>
-      <c r="JA67" s="14"/>
-      <c r="JB67" s="14"/>
-      <c r="JC67" s="14"/>
-      <c r="JD67" s="14"/>
-      <c r="JE67" s="14"/>
-      <c r="JF67" s="14"/>
-      <c r="JG67" s="14"/>
-      <c r="JH67" s="14"/>
-      <c r="JI67" s="14"/>
-      <c r="JJ67" s="14"/>
-      <c r="JK67" s="14"/>
-      <c r="JL67" s="14"/>
-      <c r="JM67" s="14"/>
-      <c r="JN67" s="14"/>
-      <c r="JO67" s="14"/>
-      <c r="JP67" s="14"/>
-      <c r="JQ67" s="14"/>
-      <c r="JR67" s="14"/>
-      <c r="JS67" s="14"/>
-      <c r="JT67" s="14"/>
-      <c r="JU67" s="14"/>
-      <c r="JV67" s="14"/>
-      <c r="JW67" s="14"/>
-      <c r="JX67" s="14"/>
-      <c r="JY67" s="14"/>
-      <c r="JZ67" s="14"/>
-      <c r="KA67" s="14"/>
-      <c r="KB67" s="14"/>
-      <c r="KC67" s="14"/>
-      <c r="KD67" s="14"/>
-      <c r="KE67" s="14"/>
-      <c r="KF67" s="14"/>
-      <c r="KG67" s="14"/>
-      <c r="KH67" s="14"/>
-      <c r="KI67" s="14"/>
-      <c r="KJ67" s="14"/>
-      <c r="KK67" s="14"/>
-      <c r="KL67" s="14"/>
-      <c r="KM67" s="14"/>
-      <c r="KN67" s="14"/>
-      <c r="KO67" s="14"/>
-      <c r="KP67" s="14"/>
-      <c r="KQ67" s="14"/>
-      <c r="KR67" s="14"/>
-      <c r="KS67" s="14"/>
-      <c r="KT67" s="14"/>
-      <c r="KU67" s="14"/>
-      <c r="KV67" s="14"/>
-      <c r="KW67" s="14"/>
-      <c r="KX67" s="14"/>
-      <c r="KY67" s="14"/>
-      <c r="KZ67" s="14"/>
-      <c r="LA67" s="14"/>
-      <c r="LB67" s="14"/>
-      <c r="LC67" s="14"/>
-      <c r="LD67" s="14"/>
-      <c r="LE67" s="14"/>
-      <c r="LF67" s="14"/>
-      <c r="LG67" s="14"/>
-      <c r="LH67" s="14"/>
-      <c r="LI67" s="14"/>
-      <c r="LJ67" s="14"/>
-      <c r="LK67" s="14"/>
-      <c r="LL67" s="14"/>
-      <c r="LM67" s="14"/>
-      <c r="LN67" s="14"/>
-      <c r="LO67" s="14"/>
-      <c r="LP67" s="14"/>
-      <c r="LQ67" s="14"/>
-      <c r="LR67" s="14"/>
-      <c r="LS67" s="14"/>
-      <c r="LT67" s="14"/>
-      <c r="LU67" s="14"/>
-      <c r="LV67" s="14"/>
-      <c r="LW67" s="14"/>
-      <c r="LX67" s="14"/>
-      <c r="LY67" s="14"/>
-      <c r="LZ67" s="14"/>
-      <c r="MA67" s="14"/>
-      <c r="MB67" s="14"/>
-      <c r="MC67" s="14"/>
-      <c r="MD67" s="14"/>
-      <c r="ME67" s="14"/>
-      <c r="MF67" s="14"/>
-      <c r="MG67" s="14"/>
-      <c r="MH67" s="14"/>
-      <c r="MI67" s="14"/>
-      <c r="MJ67" s="14"/>
-      <c r="MK67" s="14"/>
-      <c r="ML67" s="14"/>
-      <c r="MM67" s="14"/>
-      <c r="MN67" s="14"/>
-      <c r="MO67" s="14"/>
-      <c r="MP67" s="14"/>
-      <c r="MQ67" s="14"/>
-      <c r="MR67" s="14"/>
-      <c r="MS67" s="14"/>
-      <c r="MT67" s="14"/>
-      <c r="MU67" s="14"/>
-      <c r="MV67" s="14"/>
-      <c r="MW67" s="14"/>
-      <c r="MX67" s="14"/>
-      <c r="MY67" s="14"/>
-      <c r="MZ67" s="14"/>
-      <c r="NA67" s="14"/>
-      <c r="NB67" s="14"/>
-      <c r="NC67" s="14"/>
-      <c r="ND67" s="14"/>
-      <c r="NE67" s="14"/>
-      <c r="NF67" s="14"/>
-      <c r="NG67" s="14"/>
-      <c r="NH67" s="14"/>
-      <c r="NI67" s="14"/>
-      <c r="NJ67" s="14"/>
-      <c r="NK67" s="14"/>
-      <c r="NL67" s="14"/>
-      <c r="NM67" s="14"/>
-      <c r="NN67" s="14"/>
-      <c r="NO67" s="14"/>
-      <c r="NP67" s="14"/>
-      <c r="NQ67" s="14"/>
-      <c r="NR67" s="14"/>
-      <c r="NS67" s="14"/>
-      <c r="NT67" s="14"/>
-      <c r="NU67" s="14"/>
-      <c r="NV67" s="14"/>
-      <c r="NW67" s="14"/>
-      <c r="NX67" s="14"/>
-      <c r="NY67" s="14"/>
-      <c r="NZ67" s="14"/>
-      <c r="OA67" s="14"/>
-      <c r="OB67" s="14"/>
-      <c r="OC67" s="14"/>
-      <c r="OD67" s="14"/>
-      <c r="OE67" s="14"/>
-      <c r="OF67" s="14"/>
-      <c r="OG67" s="14"/>
-      <c r="OH67" s="14"/>
-      <c r="OI67" s="14"/>
-      <c r="OJ67" s="14"/>
-      <c r="OK67" s="14"/>
-      <c r="OL67" s="14"/>
-      <c r="OM67" s="14"/>
-      <c r="ON67" s="14"/>
-      <c r="OO67" s="14"/>
-      <c r="OP67" s="14"/>
-      <c r="OQ67" s="14"/>
-      <c r="OR67" s="14"/>
-      <c r="OS67" s="14"/>
-      <c r="OT67" s="14"/>
-      <c r="OU67" s="14"/>
-      <c r="OV67" s="14"/>
-      <c r="OW67" s="14"/>
-      <c r="OX67" s="14"/>
-      <c r="OY67" s="14"/>
-      <c r="OZ67" s="14"/>
-      <c r="PA67" s="14"/>
-      <c r="PB67" s="14"/>
-      <c r="PC67" s="14"/>
-      <c r="PD67" s="14"/>
-      <c r="PE67" s="14"/>
-      <c r="PF67" s="14"/>
-      <c r="PG67" s="14"/>
-      <c r="PH67" s="14"/>
-      <c r="PI67" s="14"/>
-      <c r="PJ67" s="14"/>
-      <c r="PK67" s="14"/>
-      <c r="PL67" s="14"/>
-      <c r="PM67" s="14"/>
-      <c r="PN67" s="14"/>
-      <c r="PO67" s="14"/>
-      <c r="PP67" s="14"/>
-      <c r="PQ67" s="14"/>
-      <c r="PR67" s="14"/>
-      <c r="PS67" s="14"/>
-      <c r="PT67" s="14"/>
-      <c r="PU67" s="14"/>
-      <c r="PV67" s="14"/>
-      <c r="PW67" s="14"/>
-      <c r="PX67" s="14"/>
-      <c r="PY67" s="14"/>
-      <c r="PZ67" s="14"/>
-      <c r="QA67" s="14"/>
-      <c r="QB67" s="14"/>
-      <c r="QC67" s="14"/>
-      <c r="QD67" s="14"/>
-      <c r="QE67" s="14"/>
-      <c r="QF67" s="14"/>
-      <c r="QG67" s="14"/>
-      <c r="QH67" s="14"/>
-      <c r="QI67" s="14"/>
-      <c r="QJ67" s="14"/>
-      <c r="QK67" s="14"/>
-      <c r="QL67" s="14"/>
-      <c r="QM67" s="14"/>
-      <c r="QN67" s="14"/>
-      <c r="QO67" s="14"/>
-      <c r="QP67" s="14"/>
-      <c r="QQ67" s="14"/>
-      <c r="QR67" s="14"/>
-      <c r="QS67" s="14"/>
-      <c r="QT67" s="14"/>
-      <c r="QU67" s="14"/>
-      <c r="QV67" s="14"/>
-      <c r="QW67" s="14"/>
-      <c r="QX67" s="14"/>
-      <c r="QY67" s="14"/>
-      <c r="QZ67" s="14"/>
-      <c r="RA67" s="14"/>
-      <c r="RB67" s="14"/>
-      <c r="RC67" s="14"/>
-      <c r="RD67" s="14"/>
-      <c r="RE67" s="14"/>
-      <c r="RF67" s="14"/>
-      <c r="RG67" s="14"/>
-      <c r="RH67" s="14"/>
-      <c r="RI67" s="14"/>
-      <c r="RJ67" s="14"/>
-      <c r="RK67" s="14"/>
-      <c r="RL67" s="14"/>
-      <c r="RM67" s="14"/>
-      <c r="RN67" s="14"/>
-      <c r="RO67" s="14"/>
-      <c r="RP67" s="14"/>
-      <c r="RQ67" s="14"/>
-      <c r="RR67" s="14"/>
-      <c r="RS67" s="14"/>
-      <c r="RT67" s="14"/>
-      <c r="RU67" s="14"/>
-      <c r="RV67" s="14"/>
-      <c r="RW67" s="14"/>
-      <c r="RX67" s="14"/>
-      <c r="RY67" s="14"/>
-      <c r="RZ67" s="14"/>
-      <c r="SA67" s="14"/>
-      <c r="SB67" s="14"/>
-      <c r="SC67" s="14"/>
-      <c r="SD67" s="14"/>
-      <c r="SE67" s="14"/>
-      <c r="SF67" s="14"/>
-      <c r="SG67" s="14"/>
-      <c r="SH67" s="14"/>
-      <c r="SI67" s="14"/>
-      <c r="SJ67" s="14"/>
-      <c r="SK67" s="14"/>
-      <c r="SL67" s="14"/>
-      <c r="SM67" s="14"/>
-      <c r="SN67" s="14"/>
-      <c r="SO67" s="14"/>
-      <c r="SP67" s="14"/>
-      <c r="SQ67" s="14"/>
-      <c r="SR67" s="14"/>
-      <c r="SS67" s="14"/>
-      <c r="ST67" s="14"/>
-      <c r="SU67" s="14"/>
-      <c r="SV67" s="14"/>
-      <c r="SW67" s="14"/>
-      <c r="SX67" s="14"/>
-      <c r="SY67" s="14"/>
-      <c r="SZ67" s="14"/>
-      <c r="TA67" s="14"/>
-      <c r="TB67" s="14"/>
-      <c r="TC67" s="14"/>
-      <c r="TD67" s="14"/>
-      <c r="TE67" s="14"/>
-      <c r="TF67" s="14"/>
-      <c r="TG67" s="14"/>
-      <c r="TH67" s="14"/>
-      <c r="TI67" s="14"/>
-      <c r="TJ67" s="14"/>
-      <c r="TK67" s="14"/>
-      <c r="TL67" s="14"/>
-      <c r="TM67" s="14"/>
-      <c r="TN67" s="14"/>
-      <c r="TO67" s="14"/>
-      <c r="TP67" s="14"/>
-      <c r="TQ67" s="14"/>
-      <c r="TR67" s="14"/>
-      <c r="TS67" s="14"/>
-      <c r="TT67" s="14"/>
-      <c r="TU67" s="14"/>
-      <c r="TV67" s="14"/>
-      <c r="TW67" s="14"/>
-      <c r="TX67" s="14"/>
-      <c r="TY67" s="14"/>
-      <c r="TZ67" s="14"/>
-      <c r="UA67" s="14"/>
-      <c r="UB67" s="14"/>
-      <c r="UC67" s="14"/>
-      <c r="UD67" s="14"/>
-      <c r="UE67" s="14"/>
-      <c r="UF67" s="14"/>
-      <c r="UG67" s="14"/>
-      <c r="UH67" s="14"/>
-      <c r="UI67" s="14"/>
-      <c r="UJ67" s="14"/>
-      <c r="UK67" s="14"/>
-      <c r="UL67" s="14"/>
-      <c r="UM67" s="14"/>
-      <c r="UN67" s="14"/>
-      <c r="UO67" s="14"/>
-      <c r="UP67" s="14"/>
-      <c r="UQ67" s="14"/>
-      <c r="UR67" s="14"/>
-      <c r="US67" s="14"/>
-      <c r="UT67" s="14"/>
-      <c r="UU67" s="14"/>
-      <c r="UV67" s="14"/>
-      <c r="UW67" s="14"/>
-      <c r="UX67" s="14"/>
-      <c r="UY67" s="14"/>
-      <c r="UZ67" s="14"/>
-      <c r="VA67" s="14"/>
-      <c r="VB67" s="14"/>
-      <c r="VC67" s="14"/>
-      <c r="VD67" s="14"/>
-      <c r="VE67" s="14"/>
-      <c r="VF67" s="14"/>
-      <c r="VG67" s="14"/>
-      <c r="VH67" s="14"/>
-      <c r="VI67" s="14"/>
-      <c r="VJ67" s="14"/>
-      <c r="VK67" s="14"/>
-      <c r="VL67" s="14"/>
-      <c r="VM67" s="14"/>
-      <c r="VN67" s="14"/>
-      <c r="VO67" s="14"/>
-      <c r="VP67" s="14"/>
-      <c r="VQ67" s="14"/>
-      <c r="VR67" s="14"/>
-      <c r="VS67" s="14"/>
-      <c r="VT67" s="14"/>
-      <c r="VU67" s="14"/>
-      <c r="VV67" s="14"/>
-      <c r="VW67" s="14"/>
-      <c r="VX67" s="14"/>
-      <c r="VY67" s="14"/>
-      <c r="VZ67" s="14"/>
-      <c r="WA67" s="14"/>
-      <c r="WB67" s="14"/>
-      <c r="WC67" s="14"/>
-      <c r="WD67" s="14"/>
-      <c r="WE67" s="14"/>
-      <c r="WF67" s="14"/>
-      <c r="WG67" s="14"/>
-      <c r="WH67" s="14"/>
-      <c r="WI67" s="14"/>
-      <c r="WJ67" s="14"/>
-      <c r="WK67" s="14"/>
-      <c r="WL67" s="14"/>
-      <c r="WM67" s="14"/>
-      <c r="WN67" s="14"/>
-      <c r="WO67" s="14"/>
-      <c r="WP67" s="14"/>
-      <c r="WQ67" s="14"/>
-      <c r="WR67" s="14"/>
-      <c r="WS67" s="14"/>
-      <c r="WT67" s="14"/>
-      <c r="WU67" s="14"/>
-      <c r="WV67" s="14"/>
-      <c r="WW67" s="14"/>
-      <c r="WX67" s="14"/>
-      <c r="WY67" s="14"/>
-      <c r="WZ67" s="14"/>
-      <c r="XA67" s="14"/>
-      <c r="XB67" s="14"/>
-      <c r="XC67" s="14"/>
-      <c r="XD67" s="14"/>
-      <c r="XE67" s="14"/>
-      <c r="XF67" s="14"/>
-      <c r="XG67" s="14"/>
-      <c r="XH67" s="14"/>
-      <c r="XI67" s="14"/>
-      <c r="XJ67" s="14"/>
-      <c r="XK67" s="14"/>
-      <c r="XL67" s="14"/>
-      <c r="XM67" s="14"/>
-      <c r="XN67" s="14"/>
-      <c r="XO67" s="14"/>
-      <c r="XP67" s="14"/>
-      <c r="XQ67" s="14"/>
-      <c r="XR67" s="14"/>
-      <c r="XS67" s="14"/>
-      <c r="XT67" s="14"/>
-      <c r="XU67" s="14"/>
-      <c r="XV67" s="14"/>
-      <c r="XW67" s="14"/>
-      <c r="XX67" s="14"/>
-      <c r="XY67" s="14"/>
-      <c r="XZ67" s="14"/>
-      <c r="YA67" s="14"/>
-      <c r="YB67" s="14"/>
-      <c r="YC67" s="14"/>
-      <c r="YD67" s="14"/>
-      <c r="YE67" s="14"/>
-      <c r="YF67" s="14"/>
-      <c r="YG67" s="14"/>
-      <c r="YH67" s="14"/>
-      <c r="YI67" s="14"/>
-      <c r="YJ67" s="14"/>
-      <c r="YK67" s="14"/>
-      <c r="YL67" s="14"/>
-      <c r="YM67" s="14"/>
-      <c r="YN67" s="14"/>
-      <c r="YO67" s="14"/>
-      <c r="YP67" s="14"/>
-      <c r="YQ67" s="14"/>
-      <c r="YR67" s="14"/>
-      <c r="YS67" s="14"/>
-      <c r="YT67" s="14"/>
-      <c r="YU67" s="14"/>
-      <c r="YV67" s="14"/>
-      <c r="YW67" s="14"/>
-      <c r="YX67" s="14"/>
-      <c r="YY67" s="14"/>
-      <c r="YZ67" s="14"/>
-      <c r="ZA67" s="14"/>
-      <c r="ZB67" s="14"/>
-      <c r="ZC67" s="14"/>
-      <c r="ZD67" s="14"/>
-      <c r="ZE67" s="14"/>
-      <c r="ZF67" s="14"/>
-      <c r="ZG67" s="14"/>
-      <c r="ZH67" s="14"/>
-      <c r="ZI67" s="14"/>
-      <c r="ZJ67" s="14"/>
-      <c r="ZK67" s="14"/>
-      <c r="ZL67" s="14"/>
-      <c r="ZM67" s="14"/>
-      <c r="ZN67" s="14"/>
-      <c r="ZO67" s="14"/>
-      <c r="ZP67" s="14"/>
-      <c r="ZQ67" s="14"/>
-      <c r="ZR67" s="14"/>
-      <c r="ZS67" s="14"/>
-      <c r="ZT67" s="14"/>
-      <c r="ZU67" s="14"/>
-      <c r="ZV67" s="14"/>
-      <c r="ZW67" s="14"/>
-      <c r="ZX67" s="14"/>
-      <c r="ZY67" s="14"/>
-      <c r="ZZ67" s="14"/>
-      <c r="AAA67" s="14"/>
-      <c r="AAB67" s="14"/>
-      <c r="AAC67" s="14"/>
-      <c r="AAD67" s="14"/>
-      <c r="AAE67" s="14"/>
-      <c r="AAF67" s="14"/>
-      <c r="AAG67" s="14"/>
-      <c r="AAH67" s="14"/>
-      <c r="AAI67" s="14"/>
-      <c r="AAJ67" s="14"/>
-      <c r="AAK67" s="14"/>
-      <c r="AAL67" s="14"/>
-      <c r="AAM67" s="14"/>
-      <c r="AAN67" s="14"/>
-      <c r="AAO67" s="14"/>
-      <c r="AAP67" s="14"/>
-      <c r="AAQ67" s="14"/>
-      <c r="AAR67" s="14"/>
-      <c r="AAS67" s="14"/>
-      <c r="AAT67" s="14"/>
-      <c r="AAU67" s="14"/>
-      <c r="AAV67" s="14"/>
-      <c r="AAW67" s="14"/>
-      <c r="AAX67" s="14"/>
-      <c r="AAY67" s="14"/>
-      <c r="AAZ67" s="14"/>
-      <c r="ABA67" s="14"/>
-      <c r="ABB67" s="14"/>
-      <c r="ABC67" s="14"/>
-      <c r="ABD67" s="14"/>
-      <c r="ABE67" s="14"/>
-      <c r="ABF67" s="14"/>
-      <c r="ABG67" s="14"/>
-      <c r="ABH67" s="14"/>
-      <c r="ABI67" s="14"/>
-      <c r="ABJ67" s="14"/>
-      <c r="ABK67" s="14"/>
-      <c r="ABL67" s="14"/>
-      <c r="ABM67" s="14"/>
-      <c r="ABN67" s="14"/>
-      <c r="ABO67" s="14"/>
-      <c r="ABP67" s="14"/>
-      <c r="ABQ67" s="14"/>
-      <c r="ABR67" s="14"/>
-      <c r="ABS67" s="14"/>
-      <c r="ABT67" s="14"/>
-      <c r="ABU67" s="14"/>
-      <c r="ABV67" s="14"/>
-      <c r="ABW67" s="14"/>
-      <c r="ABX67" s="14"/>
-      <c r="ABY67" s="14"/>
-      <c r="ABZ67" s="14"/>
-      <c r="ACA67" s="14"/>
-      <c r="ACB67" s="14"/>
-      <c r="ACC67" s="14"/>
-      <c r="ACD67" s="14"/>
-      <c r="ACE67" s="14"/>
-      <c r="ACF67" s="14"/>
-      <c r="ACG67" s="14"/>
-      <c r="ACH67" s="14"/>
-      <c r="ACI67" s="14"/>
-      <c r="ACJ67" s="14"/>
-      <c r="ACK67" s="14"/>
-      <c r="ACL67" s="14"/>
-      <c r="ACM67" s="14"/>
-      <c r="ACN67" s="14"/>
-      <c r="ACO67" s="14"/>
-      <c r="ACP67" s="14"/>
-      <c r="ACQ67" s="14"/>
-      <c r="ACR67" s="14"/>
-      <c r="ACS67" s="14"/>
-      <c r="ACT67" s="14"/>
-      <c r="ACU67" s="14"/>
-      <c r="ACV67" s="14"/>
-      <c r="ACW67" s="14"/>
-      <c r="ACX67" s="14"/>
-      <c r="ACY67" s="14"/>
-      <c r="ACZ67" s="14"/>
-      <c r="ADA67" s="14"/>
-      <c r="ADB67" s="14"/>
-      <c r="ADC67" s="14"/>
-      <c r="ADD67" s="14"/>
-      <c r="ADE67" s="14"/>
-      <c r="ADF67" s="14"/>
-      <c r="ADG67" s="14"/>
-      <c r="ADH67" s="14"/>
-      <c r="ADI67" s="14"/>
-      <c r="ADJ67" s="14"/>
-      <c r="ADK67" s="14"/>
-      <c r="ADL67" s="14"/>
-      <c r="ADM67" s="14"/>
-      <c r="ADN67" s="14"/>
-      <c r="ADO67" s="14"/>
-      <c r="ADP67" s="14"/>
-      <c r="ADQ67" s="14"/>
-      <c r="ADR67" s="14"/>
-      <c r="ADS67" s="14"/>
-      <c r="ADT67" s="14"/>
-      <c r="ADU67" s="14"/>
-      <c r="ADV67" s="14"/>
-      <c r="ADW67" s="14"/>
-      <c r="ADX67" s="14"/>
-      <c r="ADY67" s="14"/>
-      <c r="ADZ67" s="14"/>
-      <c r="AEA67" s="14"/>
-      <c r="AEB67" s="14"/>
-      <c r="AEC67" s="14"/>
-      <c r="AED67" s="14"/>
-      <c r="AEE67" s="14"/>
-      <c r="AEF67" s="14"/>
-      <c r="AEG67" s="14"/>
-      <c r="AEH67" s="14"/>
-      <c r="AEI67" s="14"/>
-      <c r="AEJ67" s="14"/>
-      <c r="AEK67" s="14"/>
-      <c r="AEL67" s="14"/>
-      <c r="AEM67" s="14"/>
-      <c r="AEN67" s="14"/>
-      <c r="AEO67" s="14"/>
-      <c r="AEP67" s="14"/>
-      <c r="AEQ67" s="14"/>
-      <c r="AER67" s="14"/>
-      <c r="AES67" s="14"/>
-      <c r="AET67" s="14"/>
-      <c r="AEU67" s="14"/>
-      <c r="AEV67" s="14"/>
-      <c r="AEW67" s="14"/>
-      <c r="AEX67" s="14"/>
-      <c r="AEY67" s="14"/>
-      <c r="AEZ67" s="14"/>
-      <c r="AFA67" s="14"/>
-      <c r="AFB67" s="14"/>
-      <c r="AFC67" s="14"/>
-      <c r="AFD67" s="14"/>
-      <c r="AFE67" s="14"/>
-      <c r="AFF67" s="14"/>
-      <c r="AFG67" s="14"/>
-      <c r="AFH67" s="14"/>
-      <c r="AFI67" s="14"/>
-      <c r="AFJ67" s="14"/>
-      <c r="AFK67" s="14"/>
-      <c r="AFL67" s="14"/>
-      <c r="AFM67" s="14"/>
-      <c r="AFN67" s="14"/>
-      <c r="AFO67" s="14"/>
-      <c r="AFP67" s="14"/>
-      <c r="AFQ67" s="14"/>
-      <c r="AFR67" s="14"/>
-      <c r="AFS67" s="14"/>
-      <c r="AFT67" s="14"/>
-      <c r="AFU67" s="14"/>
-      <c r="AFV67" s="14"/>
-      <c r="AFW67" s="14"/>
-      <c r="AFX67" s="14"/>
-      <c r="AFY67" s="14"/>
-      <c r="AFZ67" s="14"/>
-      <c r="AGA67" s="14"/>
-      <c r="AGB67" s="14"/>
-      <c r="AGC67" s="14"/>
-      <c r="AGD67" s="14"/>
-      <c r="AGE67" s="14"/>
-      <c r="AGF67" s="14"/>
-      <c r="AGG67" s="14"/>
-      <c r="AGH67" s="14"/>
-      <c r="AGI67" s="14"/>
-      <c r="AGJ67" s="14"/>
-      <c r="AGK67" s="14"/>
-      <c r="AGL67" s="14"/>
-      <c r="AGM67" s="14"/>
-      <c r="AGN67" s="14"/>
-      <c r="AGO67" s="14"/>
-      <c r="AGP67" s="14"/>
-      <c r="AGQ67" s="14"/>
-      <c r="AGR67" s="14"/>
-      <c r="AGS67" s="14"/>
-      <c r="AGT67" s="14"/>
-      <c r="AGU67" s="14"/>
-      <c r="AGV67" s="14"/>
-      <c r="AGW67" s="14"/>
-      <c r="AGX67" s="14"/>
-      <c r="AGY67" s="14"/>
-      <c r="AGZ67" s="14"/>
-      <c r="AHA67" s="14"/>
-      <c r="AHB67" s="14"/>
-      <c r="AHC67" s="14"/>
-      <c r="AHD67" s="14"/>
-      <c r="AHE67" s="14"/>
-      <c r="AHF67" s="14"/>
-      <c r="AHG67" s="14"/>
-      <c r="AHH67" s="14"/>
-      <c r="AHI67" s="14"/>
-      <c r="AHJ67" s="14"/>
-      <c r="AHK67" s="14"/>
-      <c r="AHL67" s="14"/>
-      <c r="AHM67" s="14"/>
-      <c r="AHN67" s="14"/>
-      <c r="AHO67" s="14"/>
-      <c r="AHP67" s="14"/>
-      <c r="AHQ67" s="14"/>
-      <c r="AHR67" s="14"/>
-      <c r="AHS67" s="14"/>
-      <c r="AHT67" s="14"/>
-      <c r="AHU67" s="14"/>
-      <c r="AHV67" s="14"/>
-      <c r="AHW67" s="14"/>
-      <c r="AHX67" s="14"/>
-      <c r="AHY67" s="14"/>
-      <c r="AHZ67" s="14"/>
-      <c r="AIA67" s="14"/>
-      <c r="AIB67" s="14"/>
-      <c r="AIC67" s="14"/>
-      <c r="AID67" s="14"/>
-      <c r="AIE67" s="14"/>
-      <c r="AIF67" s="14"/>
-      <c r="AIG67" s="14"/>
-      <c r="AIH67" s="14"/>
-      <c r="AII67" s="14"/>
-      <c r="AIJ67" s="14"/>
-      <c r="AIK67" s="14"/>
-      <c r="AIL67" s="14"/>
-      <c r="AIM67" s="14"/>
-      <c r="AIN67" s="14"/>
-      <c r="AIO67" s="14"/>
-      <c r="AIP67" s="14"/>
-      <c r="AIQ67" s="14"/>
-      <c r="AIR67" s="14"/>
-      <c r="AIS67" s="14"/>
-      <c r="AIT67" s="14"/>
-      <c r="AIU67" s="14"/>
-      <c r="AIV67" s="14"/>
-      <c r="AIW67" s="14"/>
-      <c r="AIX67" s="14"/>
-      <c r="AIY67" s="14"/>
-      <c r="AIZ67" s="14"/>
-      <c r="AJA67" s="14"/>
-      <c r="AJB67" s="14"/>
-      <c r="AJC67" s="14"/>
-      <c r="AJD67" s="14"/>
-      <c r="AJE67" s="14"/>
-      <c r="AJF67" s="14"/>
-      <c r="AJG67" s="14"/>
-      <c r="AJH67" s="14"/>
-      <c r="AJI67" s="14"/>
-      <c r="AJJ67" s="14"/>
-      <c r="AJK67" s="14"/>
-      <c r="AJL67" s="14"/>
-      <c r="AJM67" s="14"/>
-      <c r="AJN67" s="14"/>
-      <c r="AJO67" s="14"/>
-      <c r="AJP67" s="14"/>
-      <c r="AJQ67" s="14"/>
-      <c r="AJR67" s="14"/>
-      <c r="AJS67" s="14"/>
-      <c r="AJT67" s="14"/>
-      <c r="AJU67" s="14"/>
-      <c r="AJV67" s="14"/>
-      <c r="AJW67" s="14"/>
-      <c r="AJX67" s="14"/>
-      <c r="AJY67" s="14"/>
-      <c r="AJZ67" s="14"/>
-      <c r="AKA67" s="14"/>
-      <c r="AKB67" s="14"/>
-      <c r="AKC67" s="14"/>
-      <c r="AKD67" s="14"/>
-      <c r="AKE67" s="14"/>
-      <c r="AKF67" s="14"/>
-      <c r="AKG67" s="14"/>
-      <c r="AKH67" s="14"/>
-      <c r="AKI67" s="14"/>
-      <c r="AKJ67" s="14"/>
-      <c r="AKK67" s="14"/>
-      <c r="AKL67" s="14"/>
-      <c r="AKM67" s="14"/>
-      <c r="AKN67" s="14"/>
-      <c r="AKO67" s="14"/>
-      <c r="AKP67" s="14"/>
-      <c r="AKQ67" s="14"/>
-      <c r="AKR67" s="14"/>
-      <c r="AKS67" s="14"/>
-      <c r="AKT67" s="14"/>
-      <c r="AKU67" s="14"/>
-      <c r="AKV67" s="14"/>
-      <c r="AKW67" s="14"/>
-      <c r="AKX67" s="14"/>
-      <c r="AKY67" s="14"/>
-      <c r="AKZ67" s="14"/>
-      <c r="ALA67" s="14"/>
-      <c r="ALB67" s="14"/>
-      <c r="ALC67" s="14"/>
-      <c r="ALD67" s="14"/>
-      <c r="ALE67" s="14"/>
-      <c r="ALF67" s="14"/>
-      <c r="ALG67" s="14"/>
-      <c r="ALH67" s="14"/>
-      <c r="ALI67" s="14"/>
-      <c r="ALJ67" s="14"/>
-      <c r="ALK67" s="14"/>
-      <c r="ALL67" s="14"/>
-      <c r="ALM67" s="14"/>
-      <c r="ALN67" s="14"/>
-      <c r="ALO67" s="14"/>
-      <c r="ALP67" s="14"/>
-      <c r="ALQ67" s="14"/>
-      <c r="ALR67" s="14"/>
-      <c r="ALS67" s="14"/>
-      <c r="ALT67" s="14"/>
-      <c r="ALU67" s="14"/>
-      <c r="ALV67" s="14"/>
-      <c r="ALW67" s="14"/>
-      <c r="ALX67" s="14"/>
-      <c r="ALY67" s="14"/>
-      <c r="ALZ67" s="14"/>
-      <c r="AMA67" s="14"/>
-      <c r="AMB67" s="14"/>
-      <c r="AMC67" s="14"/>
-      <c r="AMD67" s="14"/>
-      <c r="AME67" s="14"/>
-      <c r="AMF67" s="14"/>
-      <c r="AMG67" s="14"/>
-      <c r="AMH67" s="14"/>
-      <c r="AMI67" s="14"/>
-      <c r="AMJ67" s="14"/>
     </row>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -8578,110 +5501,110 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="2" width="9.13"/>
   </cols>
   <sheetData>
-    <row r="1" s="23" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
+    <row r="1" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-    </row>
-    <row r="3" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24" t="s">
+    <row r="2" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+    </row>
+    <row r="3" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-    </row>
-    <row r="4" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="24" t="s">
+      <c r="C3" s="24"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+    </row>
+    <row r="4" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-    </row>
-    <row r="5" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="27" t="s">
+      <c r="C4" s="24"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+    </row>
+    <row r="5" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-    </row>
-    <row r="6" s="28" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="27" t="s">
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+    </row>
+    <row r="6" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-    </row>
-    <row r="7" s="28" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27" t="s">
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+    </row>
+    <row r="7" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
@@ -8707,53 +5630,53 @@
         <v>144</v>
       </c>
     </row>
-    <row r="11" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="27" t="s">
+    <row r="11" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-    </row>
-    <row r="12" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="27" t="s">
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+    </row>
+    <row r="12" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-    </row>
-    <row r="13" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="27" t="s">
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+    </row>
+    <row r="13" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
@@ -8790,51 +5713,51 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="27" t="s">
+    <row r="18" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-    </row>
-    <row r="20" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="27" t="s">
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+    </row>
+    <row r="20" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
@@ -8869,23 +5792,23 @@
         <v>162</v>
       </c>
     </row>
-    <row r="24" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="27" t="s">
+    <row r="24" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="25" t="s">
         <v>164</v>
       </c>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
     </row>
     <row r="30" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="12" t="s">

</xml_diff>

<commit_message>
Updated config (replacement ruleset)
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="196">
   <si>
     <t xml:space="preserve">search</t>
   </si>
@@ -1252,6 +1252,24 @@
     <t xml:space="preserve">the water in an estuary is more likely to cause an increase in the number of most aquatic species</t>
   </si>
   <si>
+    <t xml:space="preserve">Oysters need calcium ions and carbonate ions to make their shells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oysters need calcium ions and carbonate ions to make their shells.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Why are costs are reduced if desalination plants are located close to where freshwater is needed\?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Why are costs reduced if desalination plants are located close to where freshwater is needed?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should salt be added to the water that that is sprayed on the ice stupas, as Saha suggested\?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should salt be added to the water that is sprayed on the ice stupas, as Saha suggested?</t>
+  </si>
+  <si>
     <t xml:space="preserve">'fragments'</t>
   </si>
   <si>
@@ -1555,7 +1573,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1634,6 +1652,14 @@
     </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1750,7 +1776,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A79" activeCellId="0" sqref="A79:A80"/>
+      <selection pane="bottomLeft" activeCell="A74" activeCellId="0" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17849,1026 +17875,1026 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+      <c r="A77" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="B77" s="0" t="s">
+      <c r="B77" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="C77" s="0"/>
-      <c r="L77" s="0"/>
-      <c r="M77" s="0"/>
-      <c r="N77" s="0"/>
-      <c r="O77" s="0"/>
-      <c r="P77" s="0"/>
-      <c r="Q77" s="0"/>
-      <c r="R77" s="0"/>
-      <c r="S77" s="0"/>
-      <c r="T77" s="0"/>
-      <c r="U77" s="0"/>
-      <c r="V77" s="0"/>
-      <c r="W77" s="0"/>
-      <c r="X77" s="0"/>
-      <c r="Y77" s="0"/>
-      <c r="Z77" s="0"/>
-      <c r="AA77" s="0"/>
-      <c r="AB77" s="0"/>
-      <c r="AC77" s="0"/>
-      <c r="AD77" s="0"/>
-      <c r="AE77" s="0"/>
-      <c r="AF77" s="0"/>
-      <c r="AG77" s="0"/>
-      <c r="AH77" s="0"/>
-      <c r="AI77" s="0"/>
-      <c r="AJ77" s="0"/>
-      <c r="AK77" s="0"/>
-      <c r="AL77" s="0"/>
-      <c r="AM77" s="0"/>
-      <c r="AN77" s="0"/>
-      <c r="AO77" s="0"/>
-      <c r="AP77" s="0"/>
-      <c r="AQ77" s="0"/>
-      <c r="AR77" s="0"/>
-      <c r="AS77" s="0"/>
-      <c r="AT77" s="0"/>
-      <c r="AU77" s="0"/>
-      <c r="AV77" s="0"/>
-      <c r="AW77" s="0"/>
-      <c r="AX77" s="0"/>
-      <c r="AY77" s="0"/>
-      <c r="AZ77" s="0"/>
-      <c r="BA77" s="0"/>
-      <c r="BB77" s="0"/>
-      <c r="BC77" s="0"/>
-      <c r="BD77" s="0"/>
-      <c r="BE77" s="0"/>
-      <c r="BF77" s="0"/>
-      <c r="BG77" s="0"/>
-      <c r="BH77" s="0"/>
-      <c r="BI77" s="0"/>
-      <c r="BJ77" s="0"/>
-      <c r="BK77" s="0"/>
-      <c r="BL77" s="0"/>
-      <c r="BM77" s="0"/>
-      <c r="BN77" s="0"/>
-      <c r="BO77" s="0"/>
-      <c r="BP77" s="0"/>
-      <c r="BQ77" s="0"/>
-      <c r="BR77" s="0"/>
-      <c r="BS77" s="0"/>
-      <c r="BT77" s="0"/>
-      <c r="BU77" s="0"/>
-      <c r="BV77" s="0"/>
-      <c r="BW77" s="0"/>
-      <c r="BX77" s="0"/>
-      <c r="BY77" s="0"/>
-      <c r="BZ77" s="0"/>
-      <c r="CA77" s="0"/>
-      <c r="CB77" s="0"/>
-      <c r="CC77" s="0"/>
-      <c r="CD77" s="0"/>
-      <c r="CE77" s="0"/>
-      <c r="CF77" s="0"/>
-      <c r="CG77" s="0"/>
-      <c r="CH77" s="0"/>
-      <c r="CI77" s="0"/>
-      <c r="CJ77" s="0"/>
-      <c r="CK77" s="0"/>
-      <c r="CL77" s="0"/>
-      <c r="CM77" s="0"/>
-      <c r="CN77" s="0"/>
-      <c r="CO77" s="0"/>
-      <c r="CP77" s="0"/>
-      <c r="CQ77" s="0"/>
-      <c r="CR77" s="0"/>
-      <c r="CS77" s="0"/>
-      <c r="CT77" s="0"/>
-      <c r="CU77" s="0"/>
-      <c r="CV77" s="0"/>
-      <c r="CW77" s="0"/>
-      <c r="CX77" s="0"/>
-      <c r="CY77" s="0"/>
-      <c r="CZ77" s="0"/>
-      <c r="DA77" s="0"/>
-      <c r="DB77" s="0"/>
-      <c r="DC77" s="0"/>
-      <c r="DD77" s="0"/>
-      <c r="DE77" s="0"/>
-      <c r="DF77" s="0"/>
-      <c r="DG77" s="0"/>
-      <c r="DH77" s="0"/>
-      <c r="DI77" s="0"/>
-      <c r="DJ77" s="0"/>
-      <c r="DK77" s="0"/>
-      <c r="DL77" s="0"/>
-      <c r="DM77" s="0"/>
-      <c r="DN77" s="0"/>
-      <c r="DO77" s="0"/>
-      <c r="DP77" s="0"/>
-      <c r="DQ77" s="0"/>
-      <c r="DR77" s="0"/>
-      <c r="DS77" s="0"/>
-      <c r="DT77" s="0"/>
-      <c r="DU77" s="0"/>
-      <c r="DV77" s="0"/>
-      <c r="DW77" s="0"/>
-      <c r="DX77" s="0"/>
-      <c r="DY77" s="0"/>
-      <c r="DZ77" s="0"/>
-      <c r="EA77" s="0"/>
-      <c r="EB77" s="0"/>
-      <c r="EC77" s="0"/>
-      <c r="ED77" s="0"/>
-      <c r="EE77" s="0"/>
-      <c r="EF77" s="0"/>
-      <c r="EG77" s="0"/>
-      <c r="EH77" s="0"/>
-      <c r="EI77" s="0"/>
-      <c r="EJ77" s="0"/>
-      <c r="EK77" s="0"/>
-      <c r="EL77" s="0"/>
-      <c r="EM77" s="0"/>
-      <c r="EN77" s="0"/>
-      <c r="EO77" s="0"/>
-      <c r="EP77" s="0"/>
-      <c r="EQ77" s="0"/>
-      <c r="ER77" s="0"/>
-      <c r="ES77" s="0"/>
-      <c r="ET77" s="0"/>
-      <c r="EU77" s="0"/>
-      <c r="EV77" s="0"/>
-      <c r="EW77" s="0"/>
-      <c r="EX77" s="0"/>
-      <c r="EY77" s="0"/>
-      <c r="EZ77" s="0"/>
-      <c r="FA77" s="0"/>
-      <c r="FB77" s="0"/>
-      <c r="FC77" s="0"/>
-      <c r="FD77" s="0"/>
-      <c r="FE77" s="0"/>
-      <c r="FF77" s="0"/>
-      <c r="FG77" s="0"/>
-      <c r="FH77" s="0"/>
-      <c r="FI77" s="0"/>
-      <c r="FJ77" s="0"/>
-      <c r="FK77" s="0"/>
-      <c r="FL77" s="0"/>
-      <c r="FM77" s="0"/>
-      <c r="FN77" s="0"/>
-      <c r="FO77" s="0"/>
-      <c r="FP77" s="0"/>
-      <c r="FQ77" s="0"/>
-      <c r="FR77" s="0"/>
-      <c r="FS77" s="0"/>
-      <c r="FT77" s="0"/>
-      <c r="FU77" s="0"/>
-      <c r="FV77" s="0"/>
-      <c r="FW77" s="0"/>
-      <c r="FX77" s="0"/>
-      <c r="FY77" s="0"/>
-      <c r="FZ77" s="0"/>
-      <c r="GA77" s="0"/>
-      <c r="GB77" s="0"/>
-      <c r="GC77" s="0"/>
-      <c r="GD77" s="0"/>
-      <c r="GE77" s="0"/>
-      <c r="GF77" s="0"/>
-      <c r="GG77" s="0"/>
-      <c r="GH77" s="0"/>
-      <c r="GI77" s="0"/>
-      <c r="GJ77" s="0"/>
-      <c r="GK77" s="0"/>
-      <c r="GL77" s="0"/>
-      <c r="GM77" s="0"/>
-      <c r="GN77" s="0"/>
-      <c r="GO77" s="0"/>
-      <c r="GP77" s="0"/>
-      <c r="GQ77" s="0"/>
-      <c r="GR77" s="0"/>
-      <c r="GS77" s="0"/>
-      <c r="GT77" s="0"/>
-      <c r="GU77" s="0"/>
-      <c r="GV77" s="0"/>
-      <c r="GW77" s="0"/>
-      <c r="GX77" s="0"/>
-      <c r="GY77" s="0"/>
-      <c r="GZ77" s="0"/>
-      <c r="HA77" s="0"/>
-      <c r="HB77" s="0"/>
-      <c r="HC77" s="0"/>
-      <c r="HD77" s="0"/>
-      <c r="HE77" s="0"/>
-      <c r="HF77" s="0"/>
-      <c r="HG77" s="0"/>
-      <c r="HH77" s="0"/>
-      <c r="HI77" s="0"/>
-      <c r="HJ77" s="0"/>
-      <c r="HK77" s="0"/>
-      <c r="HL77" s="0"/>
-      <c r="HM77" s="0"/>
-      <c r="HN77" s="0"/>
-      <c r="HO77" s="0"/>
-      <c r="HP77" s="0"/>
-      <c r="HQ77" s="0"/>
-      <c r="HR77" s="0"/>
-      <c r="HS77" s="0"/>
-      <c r="HT77" s="0"/>
-      <c r="HU77" s="0"/>
-      <c r="HV77" s="0"/>
-      <c r="HW77" s="0"/>
-      <c r="HX77" s="0"/>
-      <c r="HY77" s="0"/>
-      <c r="HZ77" s="0"/>
-      <c r="IA77" s="0"/>
-      <c r="IB77" s="0"/>
-      <c r="IC77" s="0"/>
-      <c r="ID77" s="0"/>
-      <c r="IE77" s="0"/>
-      <c r="IF77" s="0"/>
-      <c r="IG77" s="0"/>
-      <c r="IH77" s="0"/>
-      <c r="II77" s="0"/>
-      <c r="IJ77" s="0"/>
-      <c r="IK77" s="0"/>
-      <c r="IL77" s="0"/>
-      <c r="IM77" s="0"/>
-      <c r="IN77" s="0"/>
-      <c r="IO77" s="0"/>
-      <c r="IP77" s="0"/>
-      <c r="IQ77" s="0"/>
-      <c r="IR77" s="0"/>
-      <c r="IS77" s="0"/>
-      <c r="IT77" s="0"/>
-      <c r="IU77" s="0"/>
-      <c r="IV77" s="0"/>
-      <c r="IW77" s="0"/>
-      <c r="IX77" s="0"/>
-      <c r="IY77" s="0"/>
-      <c r="IZ77" s="0"/>
-      <c r="JA77" s="0"/>
-      <c r="JB77" s="0"/>
-      <c r="JC77" s="0"/>
-      <c r="JD77" s="0"/>
-      <c r="JE77" s="0"/>
-      <c r="JF77" s="0"/>
-      <c r="JG77" s="0"/>
-      <c r="JH77" s="0"/>
-      <c r="JI77" s="0"/>
-      <c r="JJ77" s="0"/>
-      <c r="JK77" s="0"/>
-      <c r="JL77" s="0"/>
-      <c r="JM77" s="0"/>
-      <c r="JN77" s="0"/>
-      <c r="JO77" s="0"/>
-      <c r="JP77" s="0"/>
-      <c r="JQ77" s="0"/>
-      <c r="JR77" s="0"/>
-      <c r="JS77" s="0"/>
-      <c r="JT77" s="0"/>
-      <c r="JU77" s="0"/>
-      <c r="JV77" s="0"/>
-      <c r="JW77" s="0"/>
-      <c r="JX77" s="0"/>
-      <c r="JY77" s="0"/>
-      <c r="JZ77" s="0"/>
-      <c r="KA77" s="0"/>
-      <c r="KB77" s="0"/>
-      <c r="KC77" s="0"/>
-      <c r="KD77" s="0"/>
-      <c r="KE77" s="0"/>
-      <c r="KF77" s="0"/>
-      <c r="KG77" s="0"/>
-      <c r="KH77" s="0"/>
-      <c r="KI77" s="0"/>
-      <c r="KJ77" s="0"/>
-      <c r="KK77" s="0"/>
-      <c r="KL77" s="0"/>
-      <c r="KM77" s="0"/>
-      <c r="KN77" s="0"/>
-      <c r="KO77" s="0"/>
-      <c r="KP77" s="0"/>
-      <c r="KQ77" s="0"/>
-      <c r="KR77" s="0"/>
-      <c r="KS77" s="0"/>
-      <c r="KT77" s="0"/>
-      <c r="KU77" s="0"/>
-      <c r="KV77" s="0"/>
-      <c r="KW77" s="0"/>
-      <c r="KX77" s="0"/>
-      <c r="KY77" s="0"/>
-      <c r="KZ77" s="0"/>
-      <c r="LA77" s="0"/>
-      <c r="LB77" s="0"/>
-      <c r="LC77" s="0"/>
-      <c r="LD77" s="0"/>
-      <c r="LE77" s="0"/>
-      <c r="LF77" s="0"/>
-      <c r="LG77" s="0"/>
-      <c r="LH77" s="0"/>
-      <c r="LI77" s="0"/>
-      <c r="LJ77" s="0"/>
-      <c r="LK77" s="0"/>
-      <c r="LL77" s="0"/>
-      <c r="LM77" s="0"/>
-      <c r="LN77" s="0"/>
-      <c r="LO77" s="0"/>
-      <c r="LP77" s="0"/>
-      <c r="LQ77" s="0"/>
-      <c r="LR77" s="0"/>
-      <c r="LS77" s="0"/>
-      <c r="LT77" s="0"/>
-      <c r="LU77" s="0"/>
-      <c r="LV77" s="0"/>
-      <c r="LW77" s="0"/>
-      <c r="LX77" s="0"/>
-      <c r="LY77" s="0"/>
-      <c r="LZ77" s="0"/>
-      <c r="MA77" s="0"/>
-      <c r="MB77" s="0"/>
-      <c r="MC77" s="0"/>
-      <c r="MD77" s="0"/>
-      <c r="ME77" s="0"/>
-      <c r="MF77" s="0"/>
-      <c r="MG77" s="0"/>
-      <c r="MH77" s="0"/>
-      <c r="MI77" s="0"/>
-      <c r="MJ77" s="0"/>
-      <c r="MK77" s="0"/>
-      <c r="ML77" s="0"/>
-      <c r="MM77" s="0"/>
-      <c r="MN77" s="0"/>
-      <c r="MO77" s="0"/>
-      <c r="MP77" s="0"/>
-      <c r="MQ77" s="0"/>
-      <c r="MR77" s="0"/>
-      <c r="MS77" s="0"/>
-      <c r="MT77" s="0"/>
-      <c r="MU77" s="0"/>
-      <c r="MV77" s="0"/>
-      <c r="MW77" s="0"/>
-      <c r="MX77" s="0"/>
-      <c r="MY77" s="0"/>
-      <c r="MZ77" s="0"/>
-      <c r="NA77" s="0"/>
-      <c r="NB77" s="0"/>
-      <c r="NC77" s="0"/>
-      <c r="ND77" s="0"/>
-      <c r="NE77" s="0"/>
-      <c r="NF77" s="0"/>
-      <c r="NG77" s="0"/>
-      <c r="NH77" s="0"/>
-      <c r="NI77" s="0"/>
-      <c r="NJ77" s="0"/>
-      <c r="NK77" s="0"/>
-      <c r="NL77" s="0"/>
-      <c r="NM77" s="0"/>
-      <c r="NN77" s="0"/>
-      <c r="NO77" s="0"/>
-      <c r="NP77" s="0"/>
-      <c r="NQ77" s="0"/>
-      <c r="NR77" s="0"/>
-      <c r="NS77" s="0"/>
-      <c r="NT77" s="0"/>
-      <c r="NU77" s="0"/>
-      <c r="NV77" s="0"/>
-      <c r="NW77" s="0"/>
-      <c r="NX77" s="0"/>
-      <c r="NY77" s="0"/>
-      <c r="NZ77" s="0"/>
-      <c r="OA77" s="0"/>
-      <c r="OB77" s="0"/>
-      <c r="OC77" s="0"/>
-      <c r="OD77" s="0"/>
-      <c r="OE77" s="0"/>
-      <c r="OF77" s="0"/>
-      <c r="OG77" s="0"/>
-      <c r="OH77" s="0"/>
-      <c r="OI77" s="0"/>
-      <c r="OJ77" s="0"/>
-      <c r="OK77" s="0"/>
-      <c r="OL77" s="0"/>
-      <c r="OM77" s="0"/>
-      <c r="ON77" s="0"/>
-      <c r="OO77" s="0"/>
-      <c r="OP77" s="0"/>
-      <c r="OQ77" s="0"/>
-      <c r="OR77" s="0"/>
-      <c r="OS77" s="0"/>
-      <c r="OT77" s="0"/>
-      <c r="OU77" s="0"/>
-      <c r="OV77" s="0"/>
-      <c r="OW77" s="0"/>
-      <c r="OX77" s="0"/>
-      <c r="OY77" s="0"/>
-      <c r="OZ77" s="0"/>
-      <c r="PA77" s="0"/>
-      <c r="PB77" s="0"/>
-      <c r="PC77" s="0"/>
-      <c r="PD77" s="0"/>
-      <c r="PE77" s="0"/>
-      <c r="PF77" s="0"/>
-      <c r="PG77" s="0"/>
-      <c r="PH77" s="0"/>
-      <c r="PI77" s="0"/>
-      <c r="PJ77" s="0"/>
-      <c r="PK77" s="0"/>
-      <c r="PL77" s="0"/>
-      <c r="PM77" s="0"/>
-      <c r="PN77" s="0"/>
-      <c r="PO77" s="0"/>
-      <c r="PP77" s="0"/>
-      <c r="PQ77" s="0"/>
-      <c r="PR77" s="0"/>
-      <c r="PS77" s="0"/>
-      <c r="PT77" s="0"/>
-      <c r="PU77" s="0"/>
-      <c r="PV77" s="0"/>
-      <c r="PW77" s="0"/>
-      <c r="PX77" s="0"/>
-      <c r="PY77" s="0"/>
-      <c r="PZ77" s="0"/>
-      <c r="QA77" s="0"/>
-      <c r="QB77" s="0"/>
-      <c r="QC77" s="0"/>
-      <c r="QD77" s="0"/>
-      <c r="QE77" s="0"/>
-      <c r="QF77" s="0"/>
-      <c r="QG77" s="0"/>
-      <c r="QH77" s="0"/>
-      <c r="QI77" s="0"/>
-      <c r="QJ77" s="0"/>
-      <c r="QK77" s="0"/>
-      <c r="QL77" s="0"/>
-      <c r="QM77" s="0"/>
-      <c r="QN77" s="0"/>
-      <c r="QO77" s="0"/>
-      <c r="QP77" s="0"/>
-      <c r="QQ77" s="0"/>
-      <c r="QR77" s="0"/>
-      <c r="QS77" s="0"/>
-      <c r="QT77" s="0"/>
-      <c r="QU77" s="0"/>
-      <c r="QV77" s="0"/>
-      <c r="QW77" s="0"/>
-      <c r="QX77" s="0"/>
-      <c r="QY77" s="0"/>
-      <c r="QZ77" s="0"/>
-      <c r="RA77" s="0"/>
-      <c r="RB77" s="0"/>
-      <c r="RC77" s="0"/>
-      <c r="RD77" s="0"/>
-      <c r="RE77" s="0"/>
-      <c r="RF77" s="0"/>
-      <c r="RG77" s="0"/>
-      <c r="RH77" s="0"/>
-      <c r="RI77" s="0"/>
-      <c r="RJ77" s="0"/>
-      <c r="RK77" s="0"/>
-      <c r="RL77" s="0"/>
-      <c r="RM77" s="0"/>
-      <c r="RN77" s="0"/>
-      <c r="RO77" s="0"/>
-      <c r="RP77" s="0"/>
-      <c r="RQ77" s="0"/>
-      <c r="RR77" s="0"/>
-      <c r="RS77" s="0"/>
-      <c r="RT77" s="0"/>
-      <c r="RU77" s="0"/>
-      <c r="RV77" s="0"/>
-      <c r="RW77" s="0"/>
-      <c r="RX77" s="0"/>
-      <c r="RY77" s="0"/>
-      <c r="RZ77" s="0"/>
-      <c r="SA77" s="0"/>
-      <c r="SB77" s="0"/>
-      <c r="SC77" s="0"/>
-      <c r="SD77" s="0"/>
-      <c r="SE77" s="0"/>
-      <c r="SF77" s="0"/>
-      <c r="SG77" s="0"/>
-      <c r="SH77" s="0"/>
-      <c r="SI77" s="0"/>
-      <c r="SJ77" s="0"/>
-      <c r="SK77" s="0"/>
-      <c r="SL77" s="0"/>
-      <c r="SM77" s="0"/>
-      <c r="SN77" s="0"/>
-      <c r="SO77" s="0"/>
-      <c r="SP77" s="0"/>
-      <c r="SQ77" s="0"/>
-      <c r="SR77" s="0"/>
-      <c r="SS77" s="0"/>
-      <c r="ST77" s="0"/>
-      <c r="SU77" s="0"/>
-      <c r="SV77" s="0"/>
-      <c r="SW77" s="0"/>
-      <c r="SX77" s="0"/>
-      <c r="SY77" s="0"/>
-      <c r="SZ77" s="0"/>
-      <c r="TA77" s="0"/>
-      <c r="TB77" s="0"/>
-      <c r="TC77" s="0"/>
-      <c r="TD77" s="0"/>
-      <c r="TE77" s="0"/>
-      <c r="TF77" s="0"/>
-      <c r="TG77" s="0"/>
-      <c r="TH77" s="0"/>
-      <c r="TI77" s="0"/>
-      <c r="TJ77" s="0"/>
-      <c r="TK77" s="0"/>
-      <c r="TL77" s="0"/>
-      <c r="TM77" s="0"/>
-      <c r="TN77" s="0"/>
-      <c r="TO77" s="0"/>
-      <c r="TP77" s="0"/>
-      <c r="TQ77" s="0"/>
-      <c r="TR77" s="0"/>
-      <c r="TS77" s="0"/>
-      <c r="TT77" s="0"/>
-      <c r="TU77" s="0"/>
-      <c r="TV77" s="0"/>
-      <c r="TW77" s="0"/>
-      <c r="TX77" s="0"/>
-      <c r="TY77" s="0"/>
-      <c r="TZ77" s="0"/>
-      <c r="UA77" s="0"/>
-      <c r="UB77" s="0"/>
-      <c r="UC77" s="0"/>
-      <c r="UD77" s="0"/>
-      <c r="UE77" s="0"/>
-      <c r="UF77" s="0"/>
-      <c r="UG77" s="0"/>
-      <c r="UH77" s="0"/>
-      <c r="UI77" s="0"/>
-      <c r="UJ77" s="0"/>
-      <c r="UK77" s="0"/>
-      <c r="UL77" s="0"/>
-      <c r="UM77" s="0"/>
-      <c r="UN77" s="0"/>
-      <c r="UO77" s="0"/>
-      <c r="UP77" s="0"/>
-      <c r="UQ77" s="0"/>
-      <c r="UR77" s="0"/>
-      <c r="US77" s="0"/>
-      <c r="UT77" s="0"/>
-      <c r="UU77" s="0"/>
-      <c r="UV77" s="0"/>
-      <c r="UW77" s="0"/>
-      <c r="UX77" s="0"/>
-      <c r="UY77" s="0"/>
-      <c r="UZ77" s="0"/>
-      <c r="VA77" s="0"/>
-      <c r="VB77" s="0"/>
-      <c r="VC77" s="0"/>
-      <c r="VD77" s="0"/>
-      <c r="VE77" s="0"/>
-      <c r="VF77" s="0"/>
-      <c r="VG77" s="0"/>
-      <c r="VH77" s="0"/>
-      <c r="VI77" s="0"/>
-      <c r="VJ77" s="0"/>
-      <c r="VK77" s="0"/>
-      <c r="VL77" s="0"/>
-      <c r="VM77" s="0"/>
-      <c r="VN77" s="0"/>
-      <c r="VO77" s="0"/>
-      <c r="VP77" s="0"/>
-      <c r="VQ77" s="0"/>
-      <c r="VR77" s="0"/>
-      <c r="VS77" s="0"/>
-      <c r="VT77" s="0"/>
-      <c r="VU77" s="0"/>
-      <c r="VV77" s="0"/>
-      <c r="VW77" s="0"/>
-      <c r="VX77" s="0"/>
-      <c r="VY77" s="0"/>
-      <c r="VZ77" s="0"/>
-      <c r="WA77" s="0"/>
-      <c r="WB77" s="0"/>
-      <c r="WC77" s="0"/>
-      <c r="WD77" s="0"/>
-      <c r="WE77" s="0"/>
-      <c r="WF77" s="0"/>
-      <c r="WG77" s="0"/>
-      <c r="WH77" s="0"/>
-      <c r="WI77" s="0"/>
-      <c r="WJ77" s="0"/>
-      <c r="WK77" s="0"/>
-      <c r="WL77" s="0"/>
-      <c r="WM77" s="0"/>
-      <c r="WN77" s="0"/>
-      <c r="WO77" s="0"/>
-      <c r="WP77" s="0"/>
-      <c r="WQ77" s="0"/>
-      <c r="WR77" s="0"/>
-      <c r="WS77" s="0"/>
-      <c r="WT77" s="0"/>
-      <c r="WU77" s="0"/>
-      <c r="WV77" s="0"/>
-      <c r="WW77" s="0"/>
-      <c r="WX77" s="0"/>
-      <c r="WY77" s="0"/>
-      <c r="WZ77" s="0"/>
-      <c r="XA77" s="0"/>
-      <c r="XB77" s="0"/>
-      <c r="XC77" s="0"/>
-      <c r="XD77" s="0"/>
-      <c r="XE77" s="0"/>
-      <c r="XF77" s="0"/>
-      <c r="XG77" s="0"/>
-      <c r="XH77" s="0"/>
-      <c r="XI77" s="0"/>
-      <c r="XJ77" s="0"/>
-      <c r="XK77" s="0"/>
-      <c r="XL77" s="0"/>
-      <c r="XM77" s="0"/>
-      <c r="XN77" s="0"/>
-      <c r="XO77" s="0"/>
-      <c r="XP77" s="0"/>
-      <c r="XQ77" s="0"/>
-      <c r="XR77" s="0"/>
-      <c r="XS77" s="0"/>
-      <c r="XT77" s="0"/>
-      <c r="XU77" s="0"/>
-      <c r="XV77" s="0"/>
-      <c r="XW77" s="0"/>
-      <c r="XX77" s="0"/>
-      <c r="XY77" s="0"/>
-      <c r="XZ77" s="0"/>
-      <c r="YA77" s="0"/>
-      <c r="YB77" s="0"/>
-      <c r="YC77" s="0"/>
-      <c r="YD77" s="0"/>
-      <c r="YE77" s="0"/>
-      <c r="YF77" s="0"/>
-      <c r="YG77" s="0"/>
-      <c r="YH77" s="0"/>
-      <c r="YI77" s="0"/>
-      <c r="YJ77" s="0"/>
-      <c r="YK77" s="0"/>
-      <c r="YL77" s="0"/>
-      <c r="YM77" s="0"/>
-      <c r="YN77" s="0"/>
-      <c r="YO77" s="0"/>
-      <c r="YP77" s="0"/>
-      <c r="YQ77" s="0"/>
-      <c r="YR77" s="0"/>
-      <c r="YS77" s="0"/>
-      <c r="YT77" s="0"/>
-      <c r="YU77" s="0"/>
-      <c r="YV77" s="0"/>
-      <c r="YW77" s="0"/>
-      <c r="YX77" s="0"/>
-      <c r="YY77" s="0"/>
-      <c r="YZ77" s="0"/>
-      <c r="ZA77" s="0"/>
-      <c r="ZB77" s="0"/>
-      <c r="ZC77" s="0"/>
-      <c r="ZD77" s="0"/>
-      <c r="ZE77" s="0"/>
-      <c r="ZF77" s="0"/>
-      <c r="ZG77" s="0"/>
-      <c r="ZH77" s="0"/>
-      <c r="ZI77" s="0"/>
-      <c r="ZJ77" s="0"/>
-      <c r="ZK77" s="0"/>
-      <c r="ZL77" s="0"/>
-      <c r="ZM77" s="0"/>
-      <c r="ZN77" s="0"/>
-      <c r="ZO77" s="0"/>
-      <c r="ZP77" s="0"/>
-      <c r="ZQ77" s="0"/>
-      <c r="ZR77" s="0"/>
-      <c r="ZS77" s="0"/>
-      <c r="ZT77" s="0"/>
-      <c r="ZU77" s="0"/>
-      <c r="ZV77" s="0"/>
-      <c r="ZW77" s="0"/>
-      <c r="ZX77" s="0"/>
-      <c r="ZY77" s="0"/>
-      <c r="ZZ77" s="0"/>
-      <c r="AAA77" s="0"/>
-      <c r="AAB77" s="0"/>
-      <c r="AAC77" s="0"/>
-      <c r="AAD77" s="0"/>
-      <c r="AAE77" s="0"/>
-      <c r="AAF77" s="0"/>
-      <c r="AAG77" s="0"/>
-      <c r="AAH77" s="0"/>
-      <c r="AAI77" s="0"/>
-      <c r="AAJ77" s="0"/>
-      <c r="AAK77" s="0"/>
-      <c r="AAL77" s="0"/>
-      <c r="AAM77" s="0"/>
-      <c r="AAN77" s="0"/>
-      <c r="AAO77" s="0"/>
-      <c r="AAP77" s="0"/>
-      <c r="AAQ77" s="0"/>
-      <c r="AAR77" s="0"/>
-      <c r="AAS77" s="0"/>
-      <c r="AAT77" s="0"/>
-      <c r="AAU77" s="0"/>
-      <c r="AAV77" s="0"/>
-      <c r="AAW77" s="0"/>
-      <c r="AAX77" s="0"/>
-      <c r="AAY77" s="0"/>
-      <c r="AAZ77" s="0"/>
-      <c r="ABA77" s="0"/>
-      <c r="ABB77" s="0"/>
-      <c r="ABC77" s="0"/>
-      <c r="ABD77" s="0"/>
-      <c r="ABE77" s="0"/>
-      <c r="ABF77" s="0"/>
-      <c r="ABG77" s="0"/>
-      <c r="ABH77" s="0"/>
-      <c r="ABI77" s="0"/>
-      <c r="ABJ77" s="0"/>
-      <c r="ABK77" s="0"/>
-      <c r="ABL77" s="0"/>
-      <c r="ABM77" s="0"/>
-      <c r="ABN77" s="0"/>
-      <c r="ABO77" s="0"/>
-      <c r="ABP77" s="0"/>
-      <c r="ABQ77" s="0"/>
-      <c r="ABR77" s="0"/>
-      <c r="ABS77" s="0"/>
-      <c r="ABT77" s="0"/>
-      <c r="ABU77" s="0"/>
-      <c r="ABV77" s="0"/>
-      <c r="ABW77" s="0"/>
-      <c r="ABX77" s="0"/>
-      <c r="ABY77" s="0"/>
-      <c r="ABZ77" s="0"/>
-      <c r="ACA77" s="0"/>
-      <c r="ACB77" s="0"/>
-      <c r="ACC77" s="0"/>
-      <c r="ACD77" s="0"/>
-      <c r="ACE77" s="0"/>
-      <c r="ACF77" s="0"/>
-      <c r="ACG77" s="0"/>
-      <c r="ACH77" s="0"/>
-      <c r="ACI77" s="0"/>
-      <c r="ACJ77" s="0"/>
-      <c r="ACK77" s="0"/>
-      <c r="ACL77" s="0"/>
-      <c r="ACM77" s="0"/>
-      <c r="ACN77" s="0"/>
-      <c r="ACO77" s="0"/>
-      <c r="ACP77" s="0"/>
-      <c r="ACQ77" s="0"/>
-      <c r="ACR77" s="0"/>
-      <c r="ACS77" s="0"/>
-      <c r="ACT77" s="0"/>
-      <c r="ACU77" s="0"/>
-      <c r="ACV77" s="0"/>
-      <c r="ACW77" s="0"/>
-      <c r="ACX77" s="0"/>
-      <c r="ACY77" s="0"/>
-      <c r="ACZ77" s="0"/>
-      <c r="ADA77" s="0"/>
-      <c r="ADB77" s="0"/>
-      <c r="ADC77" s="0"/>
-      <c r="ADD77" s="0"/>
-      <c r="ADE77" s="0"/>
-      <c r="ADF77" s="0"/>
-      <c r="ADG77" s="0"/>
-      <c r="ADH77" s="0"/>
-      <c r="ADI77" s="0"/>
-      <c r="ADJ77" s="0"/>
-      <c r="ADK77" s="0"/>
-      <c r="ADL77" s="0"/>
-      <c r="ADM77" s="0"/>
-      <c r="ADN77" s="0"/>
-      <c r="ADO77" s="0"/>
-      <c r="ADP77" s="0"/>
-      <c r="ADQ77" s="0"/>
-      <c r="ADR77" s="0"/>
-      <c r="ADS77" s="0"/>
-      <c r="ADT77" s="0"/>
-      <c r="ADU77" s="0"/>
-      <c r="ADV77" s="0"/>
-      <c r="ADW77" s="0"/>
-      <c r="ADX77" s="0"/>
-      <c r="ADY77" s="0"/>
-      <c r="ADZ77" s="0"/>
-      <c r="AEA77" s="0"/>
-      <c r="AEB77" s="0"/>
-      <c r="AEC77" s="0"/>
-      <c r="AED77" s="0"/>
-      <c r="AEE77" s="0"/>
-      <c r="AEF77" s="0"/>
-      <c r="AEG77" s="0"/>
-      <c r="AEH77" s="0"/>
-      <c r="AEI77" s="0"/>
-      <c r="AEJ77" s="0"/>
-      <c r="AEK77" s="0"/>
-      <c r="AEL77" s="0"/>
-      <c r="AEM77" s="0"/>
-      <c r="AEN77" s="0"/>
-      <c r="AEO77" s="0"/>
-      <c r="AEP77" s="0"/>
-      <c r="AEQ77" s="0"/>
-      <c r="AER77" s="0"/>
-      <c r="AES77" s="0"/>
-      <c r="AET77" s="0"/>
-      <c r="AEU77" s="0"/>
-      <c r="AEV77" s="0"/>
-      <c r="AEW77" s="0"/>
-      <c r="AEX77" s="0"/>
-      <c r="AEY77" s="0"/>
-      <c r="AEZ77" s="0"/>
-      <c r="AFA77" s="0"/>
-      <c r="AFB77" s="0"/>
-      <c r="AFC77" s="0"/>
-      <c r="AFD77" s="0"/>
-      <c r="AFE77" s="0"/>
-      <c r="AFF77" s="0"/>
-      <c r="AFG77" s="0"/>
-      <c r="AFH77" s="0"/>
-      <c r="AFI77" s="0"/>
-      <c r="AFJ77" s="0"/>
-      <c r="AFK77" s="0"/>
-      <c r="AFL77" s="0"/>
-      <c r="AFM77" s="0"/>
-      <c r="AFN77" s="0"/>
-      <c r="AFO77" s="0"/>
-      <c r="AFP77" s="0"/>
-      <c r="AFQ77" s="0"/>
-      <c r="AFR77" s="0"/>
-      <c r="AFS77" s="0"/>
-      <c r="AFT77" s="0"/>
-      <c r="AFU77" s="0"/>
-      <c r="AFV77" s="0"/>
-      <c r="AFW77" s="0"/>
-      <c r="AFX77" s="0"/>
-      <c r="AFY77" s="0"/>
-      <c r="AFZ77" s="0"/>
-      <c r="AGA77" s="0"/>
-      <c r="AGB77" s="0"/>
-      <c r="AGC77" s="0"/>
-      <c r="AGD77" s="0"/>
-      <c r="AGE77" s="0"/>
-      <c r="AGF77" s="0"/>
-      <c r="AGG77" s="0"/>
-      <c r="AGH77" s="0"/>
-      <c r="AGI77" s="0"/>
-      <c r="AGJ77" s="0"/>
-      <c r="AGK77" s="0"/>
-      <c r="AGL77" s="0"/>
-      <c r="AGM77" s="0"/>
-      <c r="AGN77" s="0"/>
-      <c r="AGO77" s="0"/>
-      <c r="AGP77" s="0"/>
-      <c r="AGQ77" s="0"/>
-      <c r="AGR77" s="0"/>
-      <c r="AGS77" s="0"/>
-      <c r="AGT77" s="0"/>
-      <c r="AGU77" s="0"/>
-      <c r="AGV77" s="0"/>
-      <c r="AGW77" s="0"/>
-      <c r="AGX77" s="0"/>
-      <c r="AGY77" s="0"/>
-      <c r="AGZ77" s="0"/>
-      <c r="AHA77" s="0"/>
-      <c r="AHB77" s="0"/>
-      <c r="AHC77" s="0"/>
-      <c r="AHD77" s="0"/>
-      <c r="AHE77" s="0"/>
-      <c r="AHF77" s="0"/>
-      <c r="AHG77" s="0"/>
-      <c r="AHH77" s="0"/>
-      <c r="AHI77" s="0"/>
-      <c r="AHJ77" s="0"/>
-      <c r="AHK77" s="0"/>
-      <c r="AHL77" s="0"/>
-      <c r="AHM77" s="0"/>
-      <c r="AHN77" s="0"/>
-      <c r="AHO77" s="0"/>
-      <c r="AHP77" s="0"/>
-      <c r="AHQ77" s="0"/>
-      <c r="AHR77" s="0"/>
-      <c r="AHS77" s="0"/>
-      <c r="AHT77" s="0"/>
-      <c r="AHU77" s="0"/>
-      <c r="AHV77" s="0"/>
-      <c r="AHW77" s="0"/>
-      <c r="AHX77" s="0"/>
-      <c r="AHY77" s="0"/>
-      <c r="AHZ77" s="0"/>
-      <c r="AIA77" s="0"/>
-      <c r="AIB77" s="0"/>
-      <c r="AIC77" s="0"/>
-      <c r="AID77" s="0"/>
-      <c r="AIE77" s="0"/>
-      <c r="AIF77" s="0"/>
-      <c r="AIG77" s="0"/>
-      <c r="AIH77" s="0"/>
-      <c r="AII77" s="0"/>
-      <c r="AIJ77" s="0"/>
-      <c r="AIK77" s="0"/>
-      <c r="AIL77" s="0"/>
-      <c r="AIM77" s="0"/>
-      <c r="AIN77" s="0"/>
-      <c r="AIO77" s="0"/>
-      <c r="AIP77" s="0"/>
-      <c r="AIQ77" s="0"/>
-      <c r="AIR77" s="0"/>
-      <c r="AIS77" s="0"/>
-      <c r="AIT77" s="0"/>
-      <c r="AIU77" s="0"/>
-      <c r="AIV77" s="0"/>
-      <c r="AIW77" s="0"/>
-      <c r="AIX77" s="0"/>
-      <c r="AIY77" s="0"/>
-      <c r="AIZ77" s="0"/>
-      <c r="AJA77" s="0"/>
-      <c r="AJB77" s="0"/>
-      <c r="AJC77" s="0"/>
-      <c r="AJD77" s="0"/>
-      <c r="AJE77" s="0"/>
-      <c r="AJF77" s="0"/>
-      <c r="AJG77" s="0"/>
-      <c r="AJH77" s="0"/>
-      <c r="AJI77" s="0"/>
-      <c r="AJJ77" s="0"/>
-      <c r="AJK77" s="0"/>
-      <c r="AJL77" s="0"/>
-      <c r="AJM77" s="0"/>
-      <c r="AJN77" s="0"/>
-      <c r="AJO77" s="0"/>
-      <c r="AJP77" s="0"/>
-      <c r="AJQ77" s="0"/>
-      <c r="AJR77" s="0"/>
-      <c r="AJS77" s="0"/>
-      <c r="AJT77" s="0"/>
-      <c r="AJU77" s="0"/>
-      <c r="AJV77" s="0"/>
-      <c r="AJW77" s="0"/>
-      <c r="AJX77" s="0"/>
-      <c r="AJY77" s="0"/>
-      <c r="AJZ77" s="0"/>
-      <c r="AKA77" s="0"/>
-      <c r="AKB77" s="0"/>
-      <c r="AKC77" s="0"/>
-      <c r="AKD77" s="0"/>
-      <c r="AKE77" s="0"/>
-      <c r="AKF77" s="0"/>
-      <c r="AKG77" s="0"/>
-      <c r="AKH77" s="0"/>
-      <c r="AKI77" s="0"/>
-      <c r="AKJ77" s="0"/>
-      <c r="AKK77" s="0"/>
-      <c r="AKL77" s="0"/>
-      <c r="AKM77" s="0"/>
-      <c r="AKN77" s="0"/>
-      <c r="AKO77" s="0"/>
-      <c r="AKP77" s="0"/>
-      <c r="AKQ77" s="0"/>
-      <c r="AKR77" s="0"/>
-      <c r="AKS77" s="0"/>
-      <c r="AKT77" s="0"/>
-      <c r="AKU77" s="0"/>
-      <c r="AKV77" s="0"/>
-      <c r="AKW77" s="0"/>
-      <c r="AKX77" s="0"/>
-      <c r="AKY77" s="0"/>
-      <c r="AKZ77" s="0"/>
-      <c r="ALA77" s="0"/>
-      <c r="ALB77" s="0"/>
-      <c r="ALC77" s="0"/>
-      <c r="ALD77" s="0"/>
-      <c r="ALE77" s="0"/>
-      <c r="ALF77" s="0"/>
-      <c r="ALG77" s="0"/>
-      <c r="ALH77" s="0"/>
-      <c r="ALI77" s="0"/>
-      <c r="ALJ77" s="0"/>
-      <c r="ALK77" s="0"/>
-      <c r="ALL77" s="0"/>
-      <c r="ALM77" s="0"/>
-      <c r="ALN77" s="0"/>
-      <c r="ALO77" s="0"/>
-      <c r="ALP77" s="0"/>
-      <c r="ALQ77" s="0"/>
-      <c r="ALR77" s="0"/>
-      <c r="ALS77" s="0"/>
-      <c r="ALT77" s="0"/>
-      <c r="ALU77" s="0"/>
-      <c r="ALV77" s="0"/>
-      <c r="ALW77" s="0"/>
-      <c r="ALX77" s="0"/>
-      <c r="ALY77" s="0"/>
-      <c r="ALZ77" s="0"/>
-      <c r="AMA77" s="0"/>
-      <c r="AMB77" s="0"/>
-      <c r="AMC77" s="0"/>
-      <c r="AMD77" s="0"/>
-      <c r="AME77" s="0"/>
-      <c r="AMF77" s="0"/>
-      <c r="AMG77" s="0"/>
-      <c r="AMH77" s="0"/>
-      <c r="AMI77" s="0"/>
-      <c r="AMJ77" s="0"/>
+      <c r="C77" s="10"/>
+      <c r="L77" s="10"/>
+      <c r="M77" s="10"/>
+      <c r="N77" s="10"/>
+      <c r="O77" s="10"/>
+      <c r="P77" s="10"/>
+      <c r="Q77" s="10"/>
+      <c r="R77" s="10"/>
+      <c r="S77" s="10"/>
+      <c r="T77" s="10"/>
+      <c r="U77" s="10"/>
+      <c r="V77" s="10"/>
+      <c r="W77" s="10"/>
+      <c r="X77" s="10"/>
+      <c r="Y77" s="10"/>
+      <c r="Z77" s="10"/>
+      <c r="AA77" s="10"/>
+      <c r="AB77" s="10"/>
+      <c r="AC77" s="10"/>
+      <c r="AD77" s="10"/>
+      <c r="AE77" s="10"/>
+      <c r="AF77" s="10"/>
+      <c r="AG77" s="10"/>
+      <c r="AH77" s="10"/>
+      <c r="AI77" s="10"/>
+      <c r="AJ77" s="10"/>
+      <c r="AK77" s="10"/>
+      <c r="AL77" s="10"/>
+      <c r="AM77" s="10"/>
+      <c r="AN77" s="10"/>
+      <c r="AO77" s="10"/>
+      <c r="AP77" s="10"/>
+      <c r="AQ77" s="10"/>
+      <c r="AR77" s="10"/>
+      <c r="AS77" s="10"/>
+      <c r="AT77" s="10"/>
+      <c r="AU77" s="10"/>
+      <c r="AV77" s="10"/>
+      <c r="AW77" s="10"/>
+      <c r="AX77" s="10"/>
+      <c r="AY77" s="10"/>
+      <c r="AZ77" s="10"/>
+      <c r="BA77" s="10"/>
+      <c r="BB77" s="10"/>
+      <c r="BC77" s="10"/>
+      <c r="BD77" s="10"/>
+      <c r="BE77" s="10"/>
+      <c r="BF77" s="10"/>
+      <c r="BG77" s="10"/>
+      <c r="BH77" s="10"/>
+      <c r="BI77" s="10"/>
+      <c r="BJ77" s="10"/>
+      <c r="BK77" s="10"/>
+      <c r="BL77" s="10"/>
+      <c r="BM77" s="10"/>
+      <c r="BN77" s="10"/>
+      <c r="BO77" s="10"/>
+      <c r="BP77" s="10"/>
+      <c r="BQ77" s="10"/>
+      <c r="BR77" s="10"/>
+      <c r="BS77" s="10"/>
+      <c r="BT77" s="10"/>
+      <c r="BU77" s="10"/>
+      <c r="BV77" s="10"/>
+      <c r="BW77" s="10"/>
+      <c r="BX77" s="10"/>
+      <c r="BY77" s="10"/>
+      <c r="BZ77" s="10"/>
+      <c r="CA77" s="10"/>
+      <c r="CB77" s="10"/>
+      <c r="CC77" s="10"/>
+      <c r="CD77" s="10"/>
+      <c r="CE77" s="10"/>
+      <c r="CF77" s="10"/>
+      <c r="CG77" s="10"/>
+      <c r="CH77" s="10"/>
+      <c r="CI77" s="10"/>
+      <c r="CJ77" s="10"/>
+      <c r="CK77" s="10"/>
+      <c r="CL77" s="10"/>
+      <c r="CM77" s="10"/>
+      <c r="CN77" s="10"/>
+      <c r="CO77" s="10"/>
+      <c r="CP77" s="10"/>
+      <c r="CQ77" s="10"/>
+      <c r="CR77" s="10"/>
+      <c r="CS77" s="10"/>
+      <c r="CT77" s="10"/>
+      <c r="CU77" s="10"/>
+      <c r="CV77" s="10"/>
+      <c r="CW77" s="10"/>
+      <c r="CX77" s="10"/>
+      <c r="CY77" s="10"/>
+      <c r="CZ77" s="10"/>
+      <c r="DA77" s="10"/>
+      <c r="DB77" s="10"/>
+      <c r="DC77" s="10"/>
+      <c r="DD77" s="10"/>
+      <c r="DE77" s="10"/>
+      <c r="DF77" s="10"/>
+      <c r="DG77" s="10"/>
+      <c r="DH77" s="10"/>
+      <c r="DI77" s="10"/>
+      <c r="DJ77" s="10"/>
+      <c r="DK77" s="10"/>
+      <c r="DL77" s="10"/>
+      <c r="DM77" s="10"/>
+      <c r="DN77" s="10"/>
+      <c r="DO77" s="10"/>
+      <c r="DP77" s="10"/>
+      <c r="DQ77" s="10"/>
+      <c r="DR77" s="10"/>
+      <c r="DS77" s="10"/>
+      <c r="DT77" s="10"/>
+      <c r="DU77" s="10"/>
+      <c r="DV77" s="10"/>
+      <c r="DW77" s="10"/>
+      <c r="DX77" s="10"/>
+      <c r="DY77" s="10"/>
+      <c r="DZ77" s="10"/>
+      <c r="EA77" s="10"/>
+      <c r="EB77" s="10"/>
+      <c r="EC77" s="10"/>
+      <c r="ED77" s="10"/>
+      <c r="EE77" s="10"/>
+      <c r="EF77" s="10"/>
+      <c r="EG77" s="10"/>
+      <c r="EH77" s="10"/>
+      <c r="EI77" s="10"/>
+      <c r="EJ77" s="10"/>
+      <c r="EK77" s="10"/>
+      <c r="EL77" s="10"/>
+      <c r="EM77" s="10"/>
+      <c r="EN77" s="10"/>
+      <c r="EO77" s="10"/>
+      <c r="EP77" s="10"/>
+      <c r="EQ77" s="10"/>
+      <c r="ER77" s="10"/>
+      <c r="ES77" s="10"/>
+      <c r="ET77" s="10"/>
+      <c r="EU77" s="10"/>
+      <c r="EV77" s="10"/>
+      <c r="EW77" s="10"/>
+      <c r="EX77" s="10"/>
+      <c r="EY77" s="10"/>
+      <c r="EZ77" s="10"/>
+      <c r="FA77" s="10"/>
+      <c r="FB77" s="10"/>
+      <c r="FC77" s="10"/>
+      <c r="FD77" s="10"/>
+      <c r="FE77" s="10"/>
+      <c r="FF77" s="10"/>
+      <c r="FG77" s="10"/>
+      <c r="FH77" s="10"/>
+      <c r="FI77" s="10"/>
+      <c r="FJ77" s="10"/>
+      <c r="FK77" s="10"/>
+      <c r="FL77" s="10"/>
+      <c r="FM77" s="10"/>
+      <c r="FN77" s="10"/>
+      <c r="FO77" s="10"/>
+      <c r="FP77" s="10"/>
+      <c r="FQ77" s="10"/>
+      <c r="FR77" s="10"/>
+      <c r="FS77" s="10"/>
+      <c r="FT77" s="10"/>
+      <c r="FU77" s="10"/>
+      <c r="FV77" s="10"/>
+      <c r="FW77" s="10"/>
+      <c r="FX77" s="10"/>
+      <c r="FY77" s="10"/>
+      <c r="FZ77" s="10"/>
+      <c r="GA77" s="10"/>
+      <c r="GB77" s="10"/>
+      <c r="GC77" s="10"/>
+      <c r="GD77" s="10"/>
+      <c r="GE77" s="10"/>
+      <c r="GF77" s="10"/>
+      <c r="GG77" s="10"/>
+      <c r="GH77" s="10"/>
+      <c r="GI77" s="10"/>
+      <c r="GJ77" s="10"/>
+      <c r="GK77" s="10"/>
+      <c r="GL77" s="10"/>
+      <c r="GM77" s="10"/>
+      <c r="GN77" s="10"/>
+      <c r="GO77" s="10"/>
+      <c r="GP77" s="10"/>
+      <c r="GQ77" s="10"/>
+      <c r="GR77" s="10"/>
+      <c r="GS77" s="10"/>
+      <c r="GT77" s="10"/>
+      <c r="GU77" s="10"/>
+      <c r="GV77" s="10"/>
+      <c r="GW77" s="10"/>
+      <c r="GX77" s="10"/>
+      <c r="GY77" s="10"/>
+      <c r="GZ77" s="10"/>
+      <c r="HA77" s="10"/>
+      <c r="HB77" s="10"/>
+      <c r="HC77" s="10"/>
+      <c r="HD77" s="10"/>
+      <c r="HE77" s="10"/>
+      <c r="HF77" s="10"/>
+      <c r="HG77" s="10"/>
+      <c r="HH77" s="10"/>
+      <c r="HI77" s="10"/>
+      <c r="HJ77" s="10"/>
+      <c r="HK77" s="10"/>
+      <c r="HL77" s="10"/>
+      <c r="HM77" s="10"/>
+      <c r="HN77" s="10"/>
+      <c r="HO77" s="10"/>
+      <c r="HP77" s="10"/>
+      <c r="HQ77" s="10"/>
+      <c r="HR77" s="10"/>
+      <c r="HS77" s="10"/>
+      <c r="HT77" s="10"/>
+      <c r="HU77" s="10"/>
+      <c r="HV77" s="10"/>
+      <c r="HW77" s="10"/>
+      <c r="HX77" s="10"/>
+      <c r="HY77" s="10"/>
+      <c r="HZ77" s="10"/>
+      <c r="IA77" s="10"/>
+      <c r="IB77" s="10"/>
+      <c r="IC77" s="10"/>
+      <c r="ID77" s="10"/>
+      <c r="IE77" s="10"/>
+      <c r="IF77" s="10"/>
+      <c r="IG77" s="10"/>
+      <c r="IH77" s="10"/>
+      <c r="II77" s="10"/>
+      <c r="IJ77" s="10"/>
+      <c r="IK77" s="10"/>
+      <c r="IL77" s="10"/>
+      <c r="IM77" s="10"/>
+      <c r="IN77" s="10"/>
+      <c r="IO77" s="10"/>
+      <c r="IP77" s="10"/>
+      <c r="IQ77" s="10"/>
+      <c r="IR77" s="10"/>
+      <c r="IS77" s="10"/>
+      <c r="IT77" s="10"/>
+      <c r="IU77" s="10"/>
+      <c r="IV77" s="10"/>
+      <c r="IW77" s="10"/>
+      <c r="IX77" s="10"/>
+      <c r="IY77" s="10"/>
+      <c r="IZ77" s="10"/>
+      <c r="JA77" s="10"/>
+      <c r="JB77" s="10"/>
+      <c r="JC77" s="10"/>
+      <c r="JD77" s="10"/>
+      <c r="JE77" s="10"/>
+      <c r="JF77" s="10"/>
+      <c r="JG77" s="10"/>
+      <c r="JH77" s="10"/>
+      <c r="JI77" s="10"/>
+      <c r="JJ77" s="10"/>
+      <c r="JK77" s="10"/>
+      <c r="JL77" s="10"/>
+      <c r="JM77" s="10"/>
+      <c r="JN77" s="10"/>
+      <c r="JO77" s="10"/>
+      <c r="JP77" s="10"/>
+      <c r="JQ77" s="10"/>
+      <c r="JR77" s="10"/>
+      <c r="JS77" s="10"/>
+      <c r="JT77" s="10"/>
+      <c r="JU77" s="10"/>
+      <c r="JV77" s="10"/>
+      <c r="JW77" s="10"/>
+      <c r="JX77" s="10"/>
+      <c r="JY77" s="10"/>
+      <c r="JZ77" s="10"/>
+      <c r="KA77" s="10"/>
+      <c r="KB77" s="10"/>
+      <c r="KC77" s="10"/>
+      <c r="KD77" s="10"/>
+      <c r="KE77" s="10"/>
+      <c r="KF77" s="10"/>
+      <c r="KG77" s="10"/>
+      <c r="KH77" s="10"/>
+      <c r="KI77" s="10"/>
+      <c r="KJ77" s="10"/>
+      <c r="KK77" s="10"/>
+      <c r="KL77" s="10"/>
+      <c r="KM77" s="10"/>
+      <c r="KN77" s="10"/>
+      <c r="KO77" s="10"/>
+      <c r="KP77" s="10"/>
+      <c r="KQ77" s="10"/>
+      <c r="KR77" s="10"/>
+      <c r="KS77" s="10"/>
+      <c r="KT77" s="10"/>
+      <c r="KU77" s="10"/>
+      <c r="KV77" s="10"/>
+      <c r="KW77" s="10"/>
+      <c r="KX77" s="10"/>
+      <c r="KY77" s="10"/>
+      <c r="KZ77" s="10"/>
+      <c r="LA77" s="10"/>
+      <c r="LB77" s="10"/>
+      <c r="LC77" s="10"/>
+      <c r="LD77" s="10"/>
+      <c r="LE77" s="10"/>
+      <c r="LF77" s="10"/>
+      <c r="LG77" s="10"/>
+      <c r="LH77" s="10"/>
+      <c r="LI77" s="10"/>
+      <c r="LJ77" s="10"/>
+      <c r="LK77" s="10"/>
+      <c r="LL77" s="10"/>
+      <c r="LM77" s="10"/>
+      <c r="LN77" s="10"/>
+      <c r="LO77" s="10"/>
+      <c r="LP77" s="10"/>
+      <c r="LQ77" s="10"/>
+      <c r="LR77" s="10"/>
+      <c r="LS77" s="10"/>
+      <c r="LT77" s="10"/>
+      <c r="LU77" s="10"/>
+      <c r="LV77" s="10"/>
+      <c r="LW77" s="10"/>
+      <c r="LX77" s="10"/>
+      <c r="LY77" s="10"/>
+      <c r="LZ77" s="10"/>
+      <c r="MA77" s="10"/>
+      <c r="MB77" s="10"/>
+      <c r="MC77" s="10"/>
+      <c r="MD77" s="10"/>
+      <c r="ME77" s="10"/>
+      <c r="MF77" s="10"/>
+      <c r="MG77" s="10"/>
+      <c r="MH77" s="10"/>
+      <c r="MI77" s="10"/>
+      <c r="MJ77" s="10"/>
+      <c r="MK77" s="10"/>
+      <c r="ML77" s="10"/>
+      <c r="MM77" s="10"/>
+      <c r="MN77" s="10"/>
+      <c r="MO77" s="10"/>
+      <c r="MP77" s="10"/>
+      <c r="MQ77" s="10"/>
+      <c r="MR77" s="10"/>
+      <c r="MS77" s="10"/>
+      <c r="MT77" s="10"/>
+      <c r="MU77" s="10"/>
+      <c r="MV77" s="10"/>
+      <c r="MW77" s="10"/>
+      <c r="MX77" s="10"/>
+      <c r="MY77" s="10"/>
+      <c r="MZ77" s="10"/>
+      <c r="NA77" s="10"/>
+      <c r="NB77" s="10"/>
+      <c r="NC77" s="10"/>
+      <c r="ND77" s="10"/>
+      <c r="NE77" s="10"/>
+      <c r="NF77" s="10"/>
+      <c r="NG77" s="10"/>
+      <c r="NH77" s="10"/>
+      <c r="NI77" s="10"/>
+      <c r="NJ77" s="10"/>
+      <c r="NK77" s="10"/>
+      <c r="NL77" s="10"/>
+      <c r="NM77" s="10"/>
+      <c r="NN77" s="10"/>
+      <c r="NO77" s="10"/>
+      <c r="NP77" s="10"/>
+      <c r="NQ77" s="10"/>
+      <c r="NR77" s="10"/>
+      <c r="NS77" s="10"/>
+      <c r="NT77" s="10"/>
+      <c r="NU77" s="10"/>
+      <c r="NV77" s="10"/>
+      <c r="NW77" s="10"/>
+      <c r="NX77" s="10"/>
+      <c r="NY77" s="10"/>
+      <c r="NZ77" s="10"/>
+      <c r="OA77" s="10"/>
+      <c r="OB77" s="10"/>
+      <c r="OC77" s="10"/>
+      <c r="OD77" s="10"/>
+      <c r="OE77" s="10"/>
+      <c r="OF77" s="10"/>
+      <c r="OG77" s="10"/>
+      <c r="OH77" s="10"/>
+      <c r="OI77" s="10"/>
+      <c r="OJ77" s="10"/>
+      <c r="OK77" s="10"/>
+      <c r="OL77" s="10"/>
+      <c r="OM77" s="10"/>
+      <c r="ON77" s="10"/>
+      <c r="OO77" s="10"/>
+      <c r="OP77" s="10"/>
+      <c r="OQ77" s="10"/>
+      <c r="OR77" s="10"/>
+      <c r="OS77" s="10"/>
+      <c r="OT77" s="10"/>
+      <c r="OU77" s="10"/>
+      <c r="OV77" s="10"/>
+      <c r="OW77" s="10"/>
+      <c r="OX77" s="10"/>
+      <c r="OY77" s="10"/>
+      <c r="OZ77" s="10"/>
+      <c r="PA77" s="10"/>
+      <c r="PB77" s="10"/>
+      <c r="PC77" s="10"/>
+      <c r="PD77" s="10"/>
+      <c r="PE77" s="10"/>
+      <c r="PF77" s="10"/>
+      <c r="PG77" s="10"/>
+      <c r="PH77" s="10"/>
+      <c r="PI77" s="10"/>
+      <c r="PJ77" s="10"/>
+      <c r="PK77" s="10"/>
+      <c r="PL77" s="10"/>
+      <c r="PM77" s="10"/>
+      <c r="PN77" s="10"/>
+      <c r="PO77" s="10"/>
+      <c r="PP77" s="10"/>
+      <c r="PQ77" s="10"/>
+      <c r="PR77" s="10"/>
+      <c r="PS77" s="10"/>
+      <c r="PT77" s="10"/>
+      <c r="PU77" s="10"/>
+      <c r="PV77" s="10"/>
+      <c r="PW77" s="10"/>
+      <c r="PX77" s="10"/>
+      <c r="PY77" s="10"/>
+      <c r="PZ77" s="10"/>
+      <c r="QA77" s="10"/>
+      <c r="QB77" s="10"/>
+      <c r="QC77" s="10"/>
+      <c r="QD77" s="10"/>
+      <c r="QE77" s="10"/>
+      <c r="QF77" s="10"/>
+      <c r="QG77" s="10"/>
+      <c r="QH77" s="10"/>
+      <c r="QI77" s="10"/>
+      <c r="QJ77" s="10"/>
+      <c r="QK77" s="10"/>
+      <c r="QL77" s="10"/>
+      <c r="QM77" s="10"/>
+      <c r="QN77" s="10"/>
+      <c r="QO77" s="10"/>
+      <c r="QP77" s="10"/>
+      <c r="QQ77" s="10"/>
+      <c r="QR77" s="10"/>
+      <c r="QS77" s="10"/>
+      <c r="QT77" s="10"/>
+      <c r="QU77" s="10"/>
+      <c r="QV77" s="10"/>
+      <c r="QW77" s="10"/>
+      <c r="QX77" s="10"/>
+      <c r="QY77" s="10"/>
+      <c r="QZ77" s="10"/>
+      <c r="RA77" s="10"/>
+      <c r="RB77" s="10"/>
+      <c r="RC77" s="10"/>
+      <c r="RD77" s="10"/>
+      <c r="RE77" s="10"/>
+      <c r="RF77" s="10"/>
+      <c r="RG77" s="10"/>
+      <c r="RH77" s="10"/>
+      <c r="RI77" s="10"/>
+      <c r="RJ77" s="10"/>
+      <c r="RK77" s="10"/>
+      <c r="RL77" s="10"/>
+      <c r="RM77" s="10"/>
+      <c r="RN77" s="10"/>
+      <c r="RO77" s="10"/>
+      <c r="RP77" s="10"/>
+      <c r="RQ77" s="10"/>
+      <c r="RR77" s="10"/>
+      <c r="RS77" s="10"/>
+      <c r="RT77" s="10"/>
+      <c r="RU77" s="10"/>
+      <c r="RV77" s="10"/>
+      <c r="RW77" s="10"/>
+      <c r="RX77" s="10"/>
+      <c r="RY77" s="10"/>
+      <c r="RZ77" s="10"/>
+      <c r="SA77" s="10"/>
+      <c r="SB77" s="10"/>
+      <c r="SC77" s="10"/>
+      <c r="SD77" s="10"/>
+      <c r="SE77" s="10"/>
+      <c r="SF77" s="10"/>
+      <c r="SG77" s="10"/>
+      <c r="SH77" s="10"/>
+      <c r="SI77" s="10"/>
+      <c r="SJ77" s="10"/>
+      <c r="SK77" s="10"/>
+      <c r="SL77" s="10"/>
+      <c r="SM77" s="10"/>
+      <c r="SN77" s="10"/>
+      <c r="SO77" s="10"/>
+      <c r="SP77" s="10"/>
+      <c r="SQ77" s="10"/>
+      <c r="SR77" s="10"/>
+      <c r="SS77" s="10"/>
+      <c r="ST77" s="10"/>
+      <c r="SU77" s="10"/>
+      <c r="SV77" s="10"/>
+      <c r="SW77" s="10"/>
+      <c r="SX77" s="10"/>
+      <c r="SY77" s="10"/>
+      <c r="SZ77" s="10"/>
+      <c r="TA77" s="10"/>
+      <c r="TB77" s="10"/>
+      <c r="TC77" s="10"/>
+      <c r="TD77" s="10"/>
+      <c r="TE77" s="10"/>
+      <c r="TF77" s="10"/>
+      <c r="TG77" s="10"/>
+      <c r="TH77" s="10"/>
+      <c r="TI77" s="10"/>
+      <c r="TJ77" s="10"/>
+      <c r="TK77" s="10"/>
+      <c r="TL77" s="10"/>
+      <c r="TM77" s="10"/>
+      <c r="TN77" s="10"/>
+      <c r="TO77" s="10"/>
+      <c r="TP77" s="10"/>
+      <c r="TQ77" s="10"/>
+      <c r="TR77" s="10"/>
+      <c r="TS77" s="10"/>
+      <c r="TT77" s="10"/>
+      <c r="TU77" s="10"/>
+      <c r="TV77" s="10"/>
+      <c r="TW77" s="10"/>
+      <c r="TX77" s="10"/>
+      <c r="TY77" s="10"/>
+      <c r="TZ77" s="10"/>
+      <c r="UA77" s="10"/>
+      <c r="UB77" s="10"/>
+      <c r="UC77" s="10"/>
+      <c r="UD77" s="10"/>
+      <c r="UE77" s="10"/>
+      <c r="UF77" s="10"/>
+      <c r="UG77" s="10"/>
+      <c r="UH77" s="10"/>
+      <c r="UI77" s="10"/>
+      <c r="UJ77" s="10"/>
+      <c r="UK77" s="10"/>
+      <c r="UL77" s="10"/>
+      <c r="UM77" s="10"/>
+      <c r="UN77" s="10"/>
+      <c r="UO77" s="10"/>
+      <c r="UP77" s="10"/>
+      <c r="UQ77" s="10"/>
+      <c r="UR77" s="10"/>
+      <c r="US77" s="10"/>
+      <c r="UT77" s="10"/>
+      <c r="UU77" s="10"/>
+      <c r="UV77" s="10"/>
+      <c r="UW77" s="10"/>
+      <c r="UX77" s="10"/>
+      <c r="UY77" s="10"/>
+      <c r="UZ77" s="10"/>
+      <c r="VA77" s="10"/>
+      <c r="VB77" s="10"/>
+      <c r="VC77" s="10"/>
+      <c r="VD77" s="10"/>
+      <c r="VE77" s="10"/>
+      <c r="VF77" s="10"/>
+      <c r="VG77" s="10"/>
+      <c r="VH77" s="10"/>
+      <c r="VI77" s="10"/>
+      <c r="VJ77" s="10"/>
+      <c r="VK77" s="10"/>
+      <c r="VL77" s="10"/>
+      <c r="VM77" s="10"/>
+      <c r="VN77" s="10"/>
+      <c r="VO77" s="10"/>
+      <c r="VP77" s="10"/>
+      <c r="VQ77" s="10"/>
+      <c r="VR77" s="10"/>
+      <c r="VS77" s="10"/>
+      <c r="VT77" s="10"/>
+      <c r="VU77" s="10"/>
+      <c r="VV77" s="10"/>
+      <c r="VW77" s="10"/>
+      <c r="VX77" s="10"/>
+      <c r="VY77" s="10"/>
+      <c r="VZ77" s="10"/>
+      <c r="WA77" s="10"/>
+      <c r="WB77" s="10"/>
+      <c r="WC77" s="10"/>
+      <c r="WD77" s="10"/>
+      <c r="WE77" s="10"/>
+      <c r="WF77" s="10"/>
+      <c r="WG77" s="10"/>
+      <c r="WH77" s="10"/>
+      <c r="WI77" s="10"/>
+      <c r="WJ77" s="10"/>
+      <c r="WK77" s="10"/>
+      <c r="WL77" s="10"/>
+      <c r="WM77" s="10"/>
+      <c r="WN77" s="10"/>
+      <c r="WO77" s="10"/>
+      <c r="WP77" s="10"/>
+      <c r="WQ77" s="10"/>
+      <c r="WR77" s="10"/>
+      <c r="WS77" s="10"/>
+      <c r="WT77" s="10"/>
+      <c r="WU77" s="10"/>
+      <c r="WV77" s="10"/>
+      <c r="WW77" s="10"/>
+      <c r="WX77" s="10"/>
+      <c r="WY77" s="10"/>
+      <c r="WZ77" s="10"/>
+      <c r="XA77" s="10"/>
+      <c r="XB77" s="10"/>
+      <c r="XC77" s="10"/>
+      <c r="XD77" s="10"/>
+      <c r="XE77" s="10"/>
+      <c r="XF77" s="10"/>
+      <c r="XG77" s="10"/>
+      <c r="XH77" s="10"/>
+      <c r="XI77" s="10"/>
+      <c r="XJ77" s="10"/>
+      <c r="XK77" s="10"/>
+      <c r="XL77" s="10"/>
+      <c r="XM77" s="10"/>
+      <c r="XN77" s="10"/>
+      <c r="XO77" s="10"/>
+      <c r="XP77" s="10"/>
+      <c r="XQ77" s="10"/>
+      <c r="XR77" s="10"/>
+      <c r="XS77" s="10"/>
+      <c r="XT77" s="10"/>
+      <c r="XU77" s="10"/>
+      <c r="XV77" s="10"/>
+      <c r="XW77" s="10"/>
+      <c r="XX77" s="10"/>
+      <c r="XY77" s="10"/>
+      <c r="XZ77" s="10"/>
+      <c r="YA77" s="10"/>
+      <c r="YB77" s="10"/>
+      <c r="YC77" s="10"/>
+      <c r="YD77" s="10"/>
+      <c r="YE77" s="10"/>
+      <c r="YF77" s="10"/>
+      <c r="YG77" s="10"/>
+      <c r="YH77" s="10"/>
+      <c r="YI77" s="10"/>
+      <c r="YJ77" s="10"/>
+      <c r="YK77" s="10"/>
+      <c r="YL77" s="10"/>
+      <c r="YM77" s="10"/>
+      <c r="YN77" s="10"/>
+      <c r="YO77" s="10"/>
+      <c r="YP77" s="10"/>
+      <c r="YQ77" s="10"/>
+      <c r="YR77" s="10"/>
+      <c r="YS77" s="10"/>
+      <c r="YT77" s="10"/>
+      <c r="YU77" s="10"/>
+      <c r="YV77" s="10"/>
+      <c r="YW77" s="10"/>
+      <c r="YX77" s="10"/>
+      <c r="YY77" s="10"/>
+      <c r="YZ77" s="10"/>
+      <c r="ZA77" s="10"/>
+      <c r="ZB77" s="10"/>
+      <c r="ZC77" s="10"/>
+      <c r="ZD77" s="10"/>
+      <c r="ZE77" s="10"/>
+      <c r="ZF77" s="10"/>
+      <c r="ZG77" s="10"/>
+      <c r="ZH77" s="10"/>
+      <c r="ZI77" s="10"/>
+      <c r="ZJ77" s="10"/>
+      <c r="ZK77" s="10"/>
+      <c r="ZL77" s="10"/>
+      <c r="ZM77" s="10"/>
+      <c r="ZN77" s="10"/>
+      <c r="ZO77" s="10"/>
+      <c r="ZP77" s="10"/>
+      <c r="ZQ77" s="10"/>
+      <c r="ZR77" s="10"/>
+      <c r="ZS77" s="10"/>
+      <c r="ZT77" s="10"/>
+      <c r="ZU77" s="10"/>
+      <c r="ZV77" s="10"/>
+      <c r="ZW77" s="10"/>
+      <c r="ZX77" s="10"/>
+      <c r="ZY77" s="10"/>
+      <c r="ZZ77" s="10"/>
+      <c r="AAA77" s="10"/>
+      <c r="AAB77" s="10"/>
+      <c r="AAC77" s="10"/>
+      <c r="AAD77" s="10"/>
+      <c r="AAE77" s="10"/>
+      <c r="AAF77" s="10"/>
+      <c r="AAG77" s="10"/>
+      <c r="AAH77" s="10"/>
+      <c r="AAI77" s="10"/>
+      <c r="AAJ77" s="10"/>
+      <c r="AAK77" s="10"/>
+      <c r="AAL77" s="10"/>
+      <c r="AAM77" s="10"/>
+      <c r="AAN77" s="10"/>
+      <c r="AAO77" s="10"/>
+      <c r="AAP77" s="10"/>
+      <c r="AAQ77" s="10"/>
+      <c r="AAR77" s="10"/>
+      <c r="AAS77" s="10"/>
+      <c r="AAT77" s="10"/>
+      <c r="AAU77" s="10"/>
+      <c r="AAV77" s="10"/>
+      <c r="AAW77" s="10"/>
+      <c r="AAX77" s="10"/>
+      <c r="AAY77" s="10"/>
+      <c r="AAZ77" s="10"/>
+      <c r="ABA77" s="10"/>
+      <c r="ABB77" s="10"/>
+      <c r="ABC77" s="10"/>
+      <c r="ABD77" s="10"/>
+      <c r="ABE77" s="10"/>
+      <c r="ABF77" s="10"/>
+      <c r="ABG77" s="10"/>
+      <c r="ABH77" s="10"/>
+      <c r="ABI77" s="10"/>
+      <c r="ABJ77" s="10"/>
+      <c r="ABK77" s="10"/>
+      <c r="ABL77" s="10"/>
+      <c r="ABM77" s="10"/>
+      <c r="ABN77" s="10"/>
+      <c r="ABO77" s="10"/>
+      <c r="ABP77" s="10"/>
+      <c r="ABQ77" s="10"/>
+      <c r="ABR77" s="10"/>
+      <c r="ABS77" s="10"/>
+      <c r="ABT77" s="10"/>
+      <c r="ABU77" s="10"/>
+      <c r="ABV77" s="10"/>
+      <c r="ABW77" s="10"/>
+      <c r="ABX77" s="10"/>
+      <c r="ABY77" s="10"/>
+      <c r="ABZ77" s="10"/>
+      <c r="ACA77" s="10"/>
+      <c r="ACB77" s="10"/>
+      <c r="ACC77" s="10"/>
+      <c r="ACD77" s="10"/>
+      <c r="ACE77" s="10"/>
+      <c r="ACF77" s="10"/>
+      <c r="ACG77" s="10"/>
+      <c r="ACH77" s="10"/>
+      <c r="ACI77" s="10"/>
+      <c r="ACJ77" s="10"/>
+      <c r="ACK77" s="10"/>
+      <c r="ACL77" s="10"/>
+      <c r="ACM77" s="10"/>
+      <c r="ACN77" s="10"/>
+      <c r="ACO77" s="10"/>
+      <c r="ACP77" s="10"/>
+      <c r="ACQ77" s="10"/>
+      <c r="ACR77" s="10"/>
+      <c r="ACS77" s="10"/>
+      <c r="ACT77" s="10"/>
+      <c r="ACU77" s="10"/>
+      <c r="ACV77" s="10"/>
+      <c r="ACW77" s="10"/>
+      <c r="ACX77" s="10"/>
+      <c r="ACY77" s="10"/>
+      <c r="ACZ77" s="10"/>
+      <c r="ADA77" s="10"/>
+      <c r="ADB77" s="10"/>
+      <c r="ADC77" s="10"/>
+      <c r="ADD77" s="10"/>
+      <c r="ADE77" s="10"/>
+      <c r="ADF77" s="10"/>
+      <c r="ADG77" s="10"/>
+      <c r="ADH77" s="10"/>
+      <c r="ADI77" s="10"/>
+      <c r="ADJ77" s="10"/>
+      <c r="ADK77" s="10"/>
+      <c r="ADL77" s="10"/>
+      <c r="ADM77" s="10"/>
+      <c r="ADN77" s="10"/>
+      <c r="ADO77" s="10"/>
+      <c r="ADP77" s="10"/>
+      <c r="ADQ77" s="10"/>
+      <c r="ADR77" s="10"/>
+      <c r="ADS77" s="10"/>
+      <c r="ADT77" s="10"/>
+      <c r="ADU77" s="10"/>
+      <c r="ADV77" s="10"/>
+      <c r="ADW77" s="10"/>
+      <c r="ADX77" s="10"/>
+      <c r="ADY77" s="10"/>
+      <c r="ADZ77" s="10"/>
+      <c r="AEA77" s="10"/>
+      <c r="AEB77" s="10"/>
+      <c r="AEC77" s="10"/>
+      <c r="AED77" s="10"/>
+      <c r="AEE77" s="10"/>
+      <c r="AEF77" s="10"/>
+      <c r="AEG77" s="10"/>
+      <c r="AEH77" s="10"/>
+      <c r="AEI77" s="10"/>
+      <c r="AEJ77" s="10"/>
+      <c r="AEK77" s="10"/>
+      <c r="AEL77" s="10"/>
+      <c r="AEM77" s="10"/>
+      <c r="AEN77" s="10"/>
+      <c r="AEO77" s="10"/>
+      <c r="AEP77" s="10"/>
+      <c r="AEQ77" s="10"/>
+      <c r="AER77" s="10"/>
+      <c r="AES77" s="10"/>
+      <c r="AET77" s="10"/>
+      <c r="AEU77" s="10"/>
+      <c r="AEV77" s="10"/>
+      <c r="AEW77" s="10"/>
+      <c r="AEX77" s="10"/>
+      <c r="AEY77" s="10"/>
+      <c r="AEZ77" s="10"/>
+      <c r="AFA77" s="10"/>
+      <c r="AFB77" s="10"/>
+      <c r="AFC77" s="10"/>
+      <c r="AFD77" s="10"/>
+      <c r="AFE77" s="10"/>
+      <c r="AFF77" s="10"/>
+      <c r="AFG77" s="10"/>
+      <c r="AFH77" s="10"/>
+      <c r="AFI77" s="10"/>
+      <c r="AFJ77" s="10"/>
+      <c r="AFK77" s="10"/>
+      <c r="AFL77" s="10"/>
+      <c r="AFM77" s="10"/>
+      <c r="AFN77" s="10"/>
+      <c r="AFO77" s="10"/>
+      <c r="AFP77" s="10"/>
+      <c r="AFQ77" s="10"/>
+      <c r="AFR77" s="10"/>
+      <c r="AFS77" s="10"/>
+      <c r="AFT77" s="10"/>
+      <c r="AFU77" s="10"/>
+      <c r="AFV77" s="10"/>
+      <c r="AFW77" s="10"/>
+      <c r="AFX77" s="10"/>
+      <c r="AFY77" s="10"/>
+      <c r="AFZ77" s="10"/>
+      <c r="AGA77" s="10"/>
+      <c r="AGB77" s="10"/>
+      <c r="AGC77" s="10"/>
+      <c r="AGD77" s="10"/>
+      <c r="AGE77" s="10"/>
+      <c r="AGF77" s="10"/>
+      <c r="AGG77" s="10"/>
+      <c r="AGH77" s="10"/>
+      <c r="AGI77" s="10"/>
+      <c r="AGJ77" s="10"/>
+      <c r="AGK77" s="10"/>
+      <c r="AGL77" s="10"/>
+      <c r="AGM77" s="10"/>
+      <c r="AGN77" s="10"/>
+      <c r="AGO77" s="10"/>
+      <c r="AGP77" s="10"/>
+      <c r="AGQ77" s="10"/>
+      <c r="AGR77" s="10"/>
+      <c r="AGS77" s="10"/>
+      <c r="AGT77" s="10"/>
+      <c r="AGU77" s="10"/>
+      <c r="AGV77" s="10"/>
+      <c r="AGW77" s="10"/>
+      <c r="AGX77" s="10"/>
+      <c r="AGY77" s="10"/>
+      <c r="AGZ77" s="10"/>
+      <c r="AHA77" s="10"/>
+      <c r="AHB77" s="10"/>
+      <c r="AHC77" s="10"/>
+      <c r="AHD77" s="10"/>
+      <c r="AHE77" s="10"/>
+      <c r="AHF77" s="10"/>
+      <c r="AHG77" s="10"/>
+      <c r="AHH77" s="10"/>
+      <c r="AHI77" s="10"/>
+      <c r="AHJ77" s="10"/>
+      <c r="AHK77" s="10"/>
+      <c r="AHL77" s="10"/>
+      <c r="AHM77" s="10"/>
+      <c r="AHN77" s="10"/>
+      <c r="AHO77" s="10"/>
+      <c r="AHP77" s="10"/>
+      <c r="AHQ77" s="10"/>
+      <c r="AHR77" s="10"/>
+      <c r="AHS77" s="10"/>
+      <c r="AHT77" s="10"/>
+      <c r="AHU77" s="10"/>
+      <c r="AHV77" s="10"/>
+      <c r="AHW77" s="10"/>
+      <c r="AHX77" s="10"/>
+      <c r="AHY77" s="10"/>
+      <c r="AHZ77" s="10"/>
+      <c r="AIA77" s="10"/>
+      <c r="AIB77" s="10"/>
+      <c r="AIC77" s="10"/>
+      <c r="AID77" s="10"/>
+      <c r="AIE77" s="10"/>
+      <c r="AIF77" s="10"/>
+      <c r="AIG77" s="10"/>
+      <c r="AIH77" s="10"/>
+      <c r="AII77" s="10"/>
+      <c r="AIJ77" s="10"/>
+      <c r="AIK77" s="10"/>
+      <c r="AIL77" s="10"/>
+      <c r="AIM77" s="10"/>
+      <c r="AIN77" s="10"/>
+      <c r="AIO77" s="10"/>
+      <c r="AIP77" s="10"/>
+      <c r="AIQ77" s="10"/>
+      <c r="AIR77" s="10"/>
+      <c r="AIS77" s="10"/>
+      <c r="AIT77" s="10"/>
+      <c r="AIU77" s="10"/>
+      <c r="AIV77" s="10"/>
+      <c r="AIW77" s="10"/>
+      <c r="AIX77" s="10"/>
+      <c r="AIY77" s="10"/>
+      <c r="AIZ77" s="10"/>
+      <c r="AJA77" s="10"/>
+      <c r="AJB77" s="10"/>
+      <c r="AJC77" s="10"/>
+      <c r="AJD77" s="10"/>
+      <c r="AJE77" s="10"/>
+      <c r="AJF77" s="10"/>
+      <c r="AJG77" s="10"/>
+      <c r="AJH77" s="10"/>
+      <c r="AJI77" s="10"/>
+      <c r="AJJ77" s="10"/>
+      <c r="AJK77" s="10"/>
+      <c r="AJL77" s="10"/>
+      <c r="AJM77" s="10"/>
+      <c r="AJN77" s="10"/>
+      <c r="AJO77" s="10"/>
+      <c r="AJP77" s="10"/>
+      <c r="AJQ77" s="10"/>
+      <c r="AJR77" s="10"/>
+      <c r="AJS77" s="10"/>
+      <c r="AJT77" s="10"/>
+      <c r="AJU77" s="10"/>
+      <c r="AJV77" s="10"/>
+      <c r="AJW77" s="10"/>
+      <c r="AJX77" s="10"/>
+      <c r="AJY77" s="10"/>
+      <c r="AJZ77" s="10"/>
+      <c r="AKA77" s="10"/>
+      <c r="AKB77" s="10"/>
+      <c r="AKC77" s="10"/>
+      <c r="AKD77" s="10"/>
+      <c r="AKE77" s="10"/>
+      <c r="AKF77" s="10"/>
+      <c r="AKG77" s="10"/>
+      <c r="AKH77" s="10"/>
+      <c r="AKI77" s="10"/>
+      <c r="AKJ77" s="10"/>
+      <c r="AKK77" s="10"/>
+      <c r="AKL77" s="10"/>
+      <c r="AKM77" s="10"/>
+      <c r="AKN77" s="10"/>
+      <c r="AKO77" s="10"/>
+      <c r="AKP77" s="10"/>
+      <c r="AKQ77" s="10"/>
+      <c r="AKR77" s="10"/>
+      <c r="AKS77" s="10"/>
+      <c r="AKT77" s="10"/>
+      <c r="AKU77" s="10"/>
+      <c r="AKV77" s="10"/>
+      <c r="AKW77" s="10"/>
+      <c r="AKX77" s="10"/>
+      <c r="AKY77" s="10"/>
+      <c r="AKZ77" s="10"/>
+      <c r="ALA77" s="10"/>
+      <c r="ALB77" s="10"/>
+      <c r="ALC77" s="10"/>
+      <c r="ALD77" s="10"/>
+      <c r="ALE77" s="10"/>
+      <c r="ALF77" s="10"/>
+      <c r="ALG77" s="10"/>
+      <c r="ALH77" s="10"/>
+      <c r="ALI77" s="10"/>
+      <c r="ALJ77" s="10"/>
+      <c r="ALK77" s="10"/>
+      <c r="ALL77" s="10"/>
+      <c r="ALM77" s="10"/>
+      <c r="ALN77" s="10"/>
+      <c r="ALO77" s="10"/>
+      <c r="ALP77" s="10"/>
+      <c r="ALQ77" s="10"/>
+      <c r="ALR77" s="10"/>
+      <c r="ALS77" s="10"/>
+      <c r="ALT77" s="10"/>
+      <c r="ALU77" s="10"/>
+      <c r="ALV77" s="10"/>
+      <c r="ALW77" s="10"/>
+      <c r="ALX77" s="10"/>
+      <c r="ALY77" s="10"/>
+      <c r="ALZ77" s="10"/>
+      <c r="AMA77" s="10"/>
+      <c r="AMB77" s="10"/>
+      <c r="AMC77" s="10"/>
+      <c r="AMD77" s="10"/>
+      <c r="AME77" s="10"/>
+      <c r="AMF77" s="10"/>
+      <c r="AMG77" s="10"/>
+      <c r="AMH77" s="10"/>
+      <c r="AMI77" s="10"/>
+      <c r="AMJ77" s="10"/>
     </row>
     <row r="78" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
@@ -19901,8 +19927,12 @@
       <c r="AMJ78" s="2"/>
     </row>
     <row r="79" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
+      <c r="A79" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="B79" s="20" t="s">
+        <v>155</v>
+      </c>
       <c r="C79" s="1"/>
       <c r="D79" s="10"/>
       <c r="E79" s="10"/>
@@ -20926,6 +20956,22 @@
       <c r="AMI79" s="2"/>
       <c r="AMJ79" s="2"/>
     </row>
+    <row r="80" customFormat="false" ht="23.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="B80" s="20" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B81" s="20" t="s">
+        <v>159</v>
+      </c>
+    </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -20949,7 +20995,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A27" activeCellId="1" sqref="A79:A80 A27"/>
+      <selection pane="bottomLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20959,114 +21005,114 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="2" width="9.13"/>
   </cols>
   <sheetData>
-    <row r="1" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20" t="s">
+    <row r="1" s="24" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-    </row>
-    <row r="3" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
-        <v>154</v>
+    <row r="2" s="28" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+    </row>
+    <row r="3" s="28" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="25" t="s">
+        <v>160</v>
       </c>
-      <c r="B3" s="23" t="s">
-        <v>155</v>
+      <c r="B3" s="25" t="s">
+        <v>161</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-    </row>
-    <row r="4" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="23" t="s">
-        <v>156</v>
+      <c r="C3" s="26"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+    </row>
+    <row r="4" s="28" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="25" t="s">
+        <v>162</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-    </row>
-    <row r="5" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="26" t="s">
-        <v>157</v>
+      <c r="C4" s="26"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+    </row>
+    <row r="5" s="28" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="28" t="s">
+        <v>163</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-    </row>
-    <row r="6" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="26" t="s">
-        <v>158</v>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+    </row>
+    <row r="6" s="29" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="28" t="s">
+        <v>164</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>159</v>
+      <c r="B6" s="28" t="s">
+        <v>165</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-    </row>
-    <row r="7" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="26" t="s">
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+    </row>
+    <row r="7" s="29" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>32</v>
@@ -21074,7 +21120,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>32</v>
@@ -21082,59 +21128,59 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="11" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>165</v>
-      </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-    </row>
-    <row r="12" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="26" t="s">
-        <v>166</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>167</v>
-      </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-    </row>
-    <row r="13" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="26" t="s">
-        <v>168</v>
-      </c>
-      <c r="B13" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
+    </row>
+    <row r="11" s="28" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+    </row>
+    <row r="12" s="28" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+    </row>
+    <row r="13" s="28" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
@@ -21149,7 +21195,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>70</v>
@@ -21157,7 +21203,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>30</v>
@@ -21165,118 +21211,118 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="26" t="s">
+    <row r="18" s="28" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-    </row>
-    <row r="20" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="26" t="s">
-        <v>173</v>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+    </row>
+    <row r="20" s="28" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="28" t="s">
+        <v>179</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
-    <row r="24" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="26" t="s">
-        <v>182</v>
+    <row r="24" s="28" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="28" t="s">
+        <v>188</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="C24" s="25" t="s">
-        <v>183</v>
+      <c r="C24" s="27" t="s">
+        <v>189</v>
       </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
     </row>
     <row r="30" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="12" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
@@ -31313,7 +31359,7 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A79:A80 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -31323,10 +31369,10 @@
   <sheetData>
     <row r="1" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>22</v>
@@ -31335,7 +31381,7 @@
         <v>19</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>

</xml_diff>

<commit_message>
Updated linting rules to replace x with multiplication sign in more equations without tags (2)
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -651,25 +651,7 @@
     <t xml:space="preserve">$1$3$4 $5</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFC9211E"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(&lt;img[^&gt;]+/&gt;)\s*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFC9211E"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(?!\u200C)</t>
-    </r>
+    <t xml:space="preserve">(&lt;img[^&gt;]+/&gt;)\s*(?!\u200C)</t>
   </si>
   <si>
     <t xml:space="preserve">$1‌‌</t>
@@ -1262,6 +1244,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">×</t>
     </r>
@@ -1280,6 +1263,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">×</t>
     </r>
@@ -1298,6 +1282,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">×</t>
     </r>
@@ -1312,7 +1297,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">W x (B – L)² x D x g</t>
+    <t xml:space="preserve">W x \(B – L\)² x D x g</t>
   </si>
   <si>
     <r>
@@ -1330,6 +1315,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">×</t>
     </r>
@@ -1348,6 +1334,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">×</t>
     </r>
@@ -1366,6 +1353,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">×</t>
     </r>
@@ -1398,6 +1386,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">×</t>
     </r>
@@ -1416,6 +1405,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">×</t>
     </r>
@@ -1434,6 +1424,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">×</t>
     </r>
@@ -1448,7 +1439,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">W² x (B – L)² x D x g</t>
+    <t xml:space="preserve">W² x \(B – L\)² x D x g</t>
   </si>
   <si>
     <r>
@@ -1466,6 +1457,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">×</t>
     </r>
@@ -1484,6 +1476,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">×</t>
     </r>
@@ -1502,6 +1495,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">×</t>
     </r>
@@ -1748,7 +1742,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1836,23 +1830,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFC9211E"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1978,11 +1960,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2026,7 +2008,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2110,9 +2092,9 @@
   <dimension ref="A1:AMJ90"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B78" activeCellId="0" sqref="B78"/>
+      <selection pane="bottomLeft" activeCell="A78" activeCellId="0" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6611,8 +6593,8 @@
       <c r="K42" s="2"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0"/>
-      <c r="B43" s="0"/>
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="K43" s="2"/>
     </row>

</xml_diff>